<commit_message>
Lots of bugfixes & improvements
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1357,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="14">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="14">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1387,7 +1387,7 @@
       </c>
       <c r="D4" s="14">
         <f t="shared" ref="D4:D8" si="0">ROUND(POWER(B4+1,$H$2) * POWER($H$3,B4),2)</f>
-        <v>9.6</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="D5" s="14">
         <f t="shared" si="0"/>
-        <v>38.880000000000003</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="D6" s="14">
         <f t="shared" si="0"/>
-        <v>110.59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="D7" s="14">
         <f t="shared" si="0"/>
-        <v>259.2</v>
+        <v>11.18</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="D8" s="14">
         <f t="shared" si="0"/>
-        <v>537.48</v>
+        <v>14.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making mercenaries cheaper to hire; Display cash on all shops; Lots of tweaks
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
     <sheet name="Levels and Experience" sheetId="2" r:id="rId2"/>
     <sheet name="Map Size" sheetId="3" r:id="rId3"/>
     <sheet name="Item Levels" sheetId="4" r:id="rId4"/>
+    <sheet name="Mercenary Cost" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>BASE</t>
   </si>
@@ -108,6 +109,9 @@
   </si>
   <si>
     <t>Legendary</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -935,7 +939,7 @@
   <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection sqref="A1:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1442,4 +1446,226 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <f>$B3*POWER($F$4,$F$5*$B3)*$F$3</f>
+        <v>17.141191951192397</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <f>$B4*POWER($F$4,$F$5*$B4)*$F$3</f>
+        <v>39.176061534349742</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <f>$B5*POWER($F$4,$F$5*$B5)*$F$3</f>
+        <v>67.152439065201392</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <f>$B6*POWER($F$4,$F$5*$B6)*$F$3</f>
+        <v>102.31758648954383</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <f>$B7*POWER($F$4,$F$5*$B7)*$F$3</f>
+        <v>146.15378250000009</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4">
+        <f>$B8*POWER($F$4,$F$5*$B8)*$F$3</f>
+        <v>200.42000321802604</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4">
+        <f>$B9*POWER($F$4,$F$5*$B9)*$F$3</f>
+        <v>267.20071357923865</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4">
+        <f>$B10*POWER($F$4,$F$5*$B10)*$F$3</f>
+        <v>348.96295016817601</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4">
+        <f>$B11*POWER($F$4,$F$5*$B11)*$F$3</f>
+        <v>448.62306845153205</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4">
+        <f>$B12*POWER($F$4,$F$5*$B12)*$F$3</f>
+        <v>569.62475037486206</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <f>$B13*POWER($F$4,$F$5*$B13)*$F$3</f>
+        <v>716.03012699720796</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <f>$B14*POWER($F$4,$F$5*$B14)*$F$3</f>
+        <v>892.62617088696811</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4">
+        <f>$B15*POWER($F$4,$F$5*$B15)*$F$3</f>
+        <v>1105.0488609211561</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4">
+        <f>$B16*POWER($F$4,$F$5*$B16)*$F$3</f>
+        <v>1359.9280254715111</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <f>$B17*POWER($F$4,$F$5*$B17)*$F$3</f>
+        <v>1665.0562374580884</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4">
+        <f>$B18*POWER($F$4,$F$5*$B18)*$F$3</f>
+        <v>2029.5856765012818</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>17</v>
+      </c>
+      <c r="C19" s="4">
+        <f>$B19*POWER($F$4,$F$5*$B19)*$F$3</f>
+        <v>2464.2575010795235</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" s="4">
+        <f>$B20*POWER($F$4,$F$5*$B20)*$F$3</f>
+        <v>2981.6690006943409</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4">
+        <f>$B21*POWER($F$4,$F$5*$B21)*$F$3</f>
+        <v>3596.5846401504168</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>20</v>
+      </c>
+      <c r="C22" s="4">
+        <f>$B22*POWER($F$4,$F$5*$B22)*$F$3</f>
+        <v>4326.2980831949862</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rebalancing equipment and materials; Adding IsEquipped check on Foundry
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -1337,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,7 +1361,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="14">
-        <v>1.5</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="D4" s="14">
         <f t="shared" ref="D4:D8" si="0">ROUND(POWER(B4+1,$H$2) * POWER($H$3,B4),2)</f>
-        <v>2.83</v>
+        <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="D5" s="14">
         <f t="shared" si="0"/>
-        <v>5.2</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="D6" s="14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="D7" s="14">
         <f t="shared" si="0"/>
-        <v>11.18</v>
+        <v>8.7799999999999994</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="D8" s="14">
         <f t="shared" si="0"/>
-        <v>14.7</v>
+        <v>11.23</v>
       </c>
     </row>
   </sheetData>
@@ -1452,7 +1452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1471,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <f>$B3*POWER($F$4,$F$5*$B3)*$F$3</f>
+        <f t="shared" ref="C3:C22" si="0">$B3*POWER($F$4,$F$5*$B3)*$F$3</f>
         <v>17.141191951192397</v>
       </c>
       <c r="E3" t="s">
@@ -1486,7 +1486,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4">
-        <f>$B4*POWER($F$4,$F$5*$B4)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>39.176061534349742</v>
       </c>
       <c r="E4" t="s">
@@ -1501,7 +1501,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4">
-        <f>$B5*POWER($F$4,$F$5*$B5)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>67.152439065201392</v>
       </c>
       <c r="E5" t="s">
@@ -1516,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <f>$B6*POWER($F$4,$F$5*$B6)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>102.31758648954383</v>
       </c>
     </row>
@@ -1525,7 +1525,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4">
-        <f>$B7*POWER($F$4,$F$5*$B7)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>146.15378250000009</v>
       </c>
     </row>
@@ -1534,7 +1534,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4">
-        <f>$B8*POWER($F$4,$F$5*$B8)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>200.42000321802604</v>
       </c>
     </row>
@@ -1543,7 +1543,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="4">
-        <f>$B9*POWER($F$4,$F$5*$B9)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>267.20071357923865</v>
       </c>
     </row>
@@ -1552,7 +1552,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4">
-        <f>$B10*POWER($F$4,$F$5*$B10)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>348.96295016817601</v>
       </c>
     </row>
@@ -1561,7 +1561,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="4">
-        <f>$B11*POWER($F$4,$F$5*$B11)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>448.62306845153205</v>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="4">
-        <f>$B12*POWER($F$4,$F$5*$B12)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>569.62475037486206</v>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="4">
-        <f>$B13*POWER($F$4,$F$5*$B13)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>716.03012699720796</v>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="4">
-        <f>$B14*POWER($F$4,$F$5*$B14)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>892.62617088696811</v>
       </c>
     </row>
@@ -1597,7 +1597,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="4">
-        <f>$B15*POWER($F$4,$F$5*$B15)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>1105.0488609211561</v>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="4">
-        <f>$B16*POWER($F$4,$F$5*$B16)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>1359.9280254715111</v>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="4">
-        <f>$B17*POWER($F$4,$F$5*$B17)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>1665.0562374580884</v>
       </c>
     </row>
@@ -1624,7 +1624,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="4">
-        <f>$B18*POWER($F$4,$F$5*$B18)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>2029.5856765012818</v>
       </c>
     </row>
@@ -1633,7 +1633,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="4">
-        <f>$B19*POWER($F$4,$F$5*$B19)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>2464.2575010795235</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="4">
-        <f>$B20*POWER($F$4,$F$5*$B20)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>2981.6690006943409</v>
       </c>
     </row>
@@ -1651,7 +1651,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="4">
-        <f>$B21*POWER($F$4,$F$5*$B21)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>3596.5846401504168</v>
       </c>
     </row>
@@ -1660,7 +1660,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="4">
-        <f>$B22*POWER($F$4,$F$5*$B22)*$F$3</f>
+        <f t="shared" si="0"/>
         <v>4326.2980831949862</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor fixes/scaling; Fixed race relations scaling by experience; Fewer encounters in space;
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Map Size" sheetId="3" r:id="rId3"/>
     <sheet name="Item Levels" sheetId="4" r:id="rId4"/>
     <sheet name="Mercenary Cost" sheetId="5" r:id="rId5"/>
+    <sheet name="Relations Levels" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>BASE</t>
   </si>
@@ -112,6 +113,12 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Level = Math.Floor((Math.Sqrt(d + 0.25) - 0.5)</t>
+  </si>
+  <si>
+    <t>Where d = exp / Scale</t>
   </si>
 </sst>
 </file>
@@ -939,7 +946,7 @@
   <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H27"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -1668,4 +1675,1537 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>(B6/1000) + 0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="D6">
+        <f>SQRT(C6)-0.5</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>FLOOR(D6,1)</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f>-B6</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>(-G6/1000) + 0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="I6">
+        <f>SQRT(H6)-0.5</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f>-FLOOR(I6,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>200</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C50" si="0">(B7/1000) + 0.25</f>
+        <v>0.45</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D50" si="1">SQRT(C7)-0.5</f>
+        <v>0.17082039324993692</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E50" si="2">FLOOR(D7,1)</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G50" si="3">-B7</f>
+        <v>-200</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H50" si="4">(-G7/1000) + 0.25</f>
+        <v>0.45</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I50" si="5">SQRT(H7)-0.5</f>
+        <v>0.17082039324993692</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:J50" si="6">-FLOOR(I7,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>400</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.30622577482985502</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>-400</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>0.65</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>0.30622577482985502</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>600</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.42195444572928875</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>-600</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>0.85</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>0.42195444572928875</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>800</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>1.05</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0.52469507659595993</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>-800</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>1.05</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>0.52469507659595993</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0.6180339887498949</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>-1000</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>1.25</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>0.6180339887498949</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1500</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>0.82287565553229536</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>-1500</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>1.75</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>0.82287565553229536</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2000</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>-2000</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>2.25</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2500</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>1.1583123951776999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>-2500</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>2.75</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>1.1583123951776999</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>3000</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>1.3027756377319946</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>-3000</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>3.25</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>1.3027756377319946</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>3500</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>1.4364916731037085</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>-3500</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>3.75</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>1.4364916731037085</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>4000</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>4.25</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>1.5615528128088303</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>-4000</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>4.25</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>1.5615528128088303</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>4500</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>1.679449471770337</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>-4500</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>4.75</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>1.679449471770337</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>5000</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>5.25</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>1.7912878474779199</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>-5000</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="4"/>
+        <v>5.25</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="5"/>
+        <v>1.7912878474779199</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>6000</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>-6000</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>6.25</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>7000</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>7.25</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>2.1925824035672519</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>-7000</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>7.25</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="5"/>
+        <v>2.1925824035672519</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>8000</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>8.25</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>2.3722813232690143</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>-8000</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>8.25</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="5"/>
+        <v>2.3722813232690143</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>9000</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>9.25</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>2.5413812651491097</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>-9000</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>9.25</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="5"/>
+        <v>2.5413812651491097</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>10000</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>10.25</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>2.7015621187164243</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>-10000</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>10.25</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="5"/>
+        <v>2.7015621187164243</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>11000</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>2.8541019662496847</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>-11000</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>11.25</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="5"/>
+        <v>2.8541019662496847</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>12000</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>12.25</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>-12000</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>12.25</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>13000</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>13.25</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>3.140054944640259</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>-13000</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="4"/>
+        <v>13.25</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="5"/>
+        <v>3.140054944640259</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>14000</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>14.25</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>3.2749172176353749</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>-14000</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>14.25</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="5"/>
+        <v>3.2749172176353749</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>15000</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>15.25</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>3.405124837953327</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>-15000</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>15.25</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="5"/>
+        <v>3.405124837953327</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>16000</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>16.25</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>3.5311288741492746</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>-16000</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="4"/>
+        <v>16.25</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="5"/>
+        <v>3.5311288741492746</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>17000</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>17.25</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>3.6533119314590374</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>-17000</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>17.25</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="5"/>
+        <v>3.6533119314590374</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>18000</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>18.25</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>3.7720018726587652</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>-18000</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>18.25</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="5"/>
+        <v>3.7720018726587652</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>19000</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>19.25</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>3.8874821936960613</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>-19000</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="4"/>
+        <v>19.25</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="5"/>
+        <v>3.8874821936960613</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>20000</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>20.25</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>-20000</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="4"/>
+        <v>20.25</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>21000</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>21.25</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>4.1097722286464435</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>-21000</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="4"/>
+        <v>21.25</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="5"/>
+        <v>4.1097722286464435</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>22000</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>22.25</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>4.2169905660283016</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>-22000</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="4"/>
+        <v>22.25</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="5"/>
+        <v>4.2169905660283016</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>23000</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>23.25</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>4.3218253804964775</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>-23000</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="4"/>
+        <v>23.25</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="5"/>
+        <v>4.3218253804964775</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>24000</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>24.25</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>4.424428900898052</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>-24000</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="4"/>
+        <v>24.25</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="5"/>
+        <v>4.424428900898052</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>25000</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>25.25</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>4.524937810560445</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="3"/>
+        <v>-25000</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>25.25</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="5"/>
+        <v>4.524937810560445</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>26000</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>26.25</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>4.623475382979799</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>-26000</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>26.25</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="5"/>
+        <v>4.623475382979799</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>27000</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>27.25</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>4.7201532544552753</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="3"/>
+        <v>-27000</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="4"/>
+        <v>27.25</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="5"/>
+        <v>4.7201532544552753</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>28000</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>28.25</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>4.815072906367325</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="3"/>
+        <v>-28000</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="4"/>
+        <v>28.25</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="5"/>
+        <v>4.815072906367325</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>29000</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>29.25</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>4.9083269131959844</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="3"/>
+        <v>-29000</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="4"/>
+        <v>29.25</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="5"/>
+        <v>4.9083269131959844</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>30000</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>30.25</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="3"/>
+        <v>-30000</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="4"/>
+        <v>30.25</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>31000</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>31.25</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>5.0901699437494745</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="3"/>
+        <v>-31000</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="4"/>
+        <v>31.25</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="5"/>
+        <v>5.0901699437494745</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>32000</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>32.25</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>5.1789083458002736</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="3"/>
+        <v>-32000</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="4"/>
+        <v>32.25</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="5"/>
+        <v>5.1789083458002736</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>33000</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>33.25</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>5.2662812973353983</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="3"/>
+        <v>-33000</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="4"/>
+        <v>33.25</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="5"/>
+        <v>5.2662812973353983</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>34000</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>34.25</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>5.3523499553598128</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="3"/>
+        <v>-34000</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="4"/>
+        <v>34.25</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="5"/>
+        <v>5.3523499553598128</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>35000</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>35.25</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>5.4371710435189584</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="3"/>
+        <v>-35000</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="4"/>
+        <v>35.25</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="5"/>
+        <v>5.4371710435189584</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>40000</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>40.25</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>5.8442887702247601</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="3"/>
+        <v>-40000</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="4"/>
+        <v>40.25</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="5"/>
+        <v>5.8442887702247601</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lots of fixes for first contact
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -1682,13 +1682,13 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1748,7 +1748,6 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <f>-FLOOR(I6,1)</f>
         <v>0</v>
       </c>
     </row>
@@ -1781,8 +1780,8 @@
         <v>0.17082039324993692</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J50" si="6">-FLOOR(I7,1)</f>
-        <v>0</v>
+        <f t="shared" ref="J7:J50" si="6">-FLOOR(I7,1)-1</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1815,7 +1814,7 @@
       </c>
       <c r="J8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1848,7 +1847,7 @@
       </c>
       <c r="J9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1881,7 +1880,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1914,7 +1913,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1947,7 +1946,7 @@
       </c>
       <c r="J12">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1980,7 +1979,7 @@
       </c>
       <c r="J13">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2013,7 +2012,7 @@
       </c>
       <c r="J14">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2046,7 +2045,7 @@
       </c>
       <c r="J15">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2079,7 +2078,7 @@
       </c>
       <c r="J16">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -2112,7 +2111,7 @@
       </c>
       <c r="J17">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -2145,7 +2144,7 @@
       </c>
       <c r="J18">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -2178,7 +2177,7 @@
       </c>
       <c r="J19">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -2211,7 +2210,7 @@
       </c>
       <c r="J20">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -2244,7 +2243,7 @@
       </c>
       <c r="J21">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -2277,7 +2276,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -2310,7 +2309,7 @@
       </c>
       <c r="J23">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -2343,7 +2342,7 @@
       </c>
       <c r="J24">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -2376,7 +2375,7 @@
       </c>
       <c r="J25">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -2409,7 +2408,7 @@
       </c>
       <c r="J26">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -2442,7 +2441,7 @@
       </c>
       <c r="J27">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -2475,7 +2474,7 @@
       </c>
       <c r="J28">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -2508,7 +2507,7 @@
       </c>
       <c r="J29">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -2541,7 +2540,7 @@
       </c>
       <c r="J30">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
@@ -2574,7 +2573,7 @@
       </c>
       <c r="J31">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -2607,7 +2606,7 @@
       </c>
       <c r="J32">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
@@ -2640,7 +2639,7 @@
       </c>
       <c r="J33">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
@@ -2673,7 +2672,7 @@
       </c>
       <c r="J34">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
@@ -2706,7 +2705,7 @@
       </c>
       <c r="J35">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
@@ -2739,7 +2738,7 @@
       </c>
       <c r="J36">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
@@ -2772,7 +2771,7 @@
       </c>
       <c r="J37">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -2805,7 +2804,7 @@
       </c>
       <c r="J38">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
@@ -2838,7 +2837,7 @@
       </c>
       <c r="J39">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
@@ -2857,22 +2856,6 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G40">
-        <f t="shared" si="3"/>
-        <v>-26000</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="4"/>
-        <v>26.25</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="5"/>
-        <v>4.623475382979799</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="6"/>
-        <v>-4</v>
-      </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41">
@@ -2890,22 +2873,6 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G41">
-        <f t="shared" si="3"/>
-        <v>-27000</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="4"/>
-        <v>27.25</v>
-      </c>
-      <c r="I41">
-        <f t="shared" si="5"/>
-        <v>4.7201532544552753</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="6"/>
-        <v>-4</v>
-      </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42">
@@ -2923,22 +2890,6 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G42">
-        <f t="shared" si="3"/>
-        <v>-28000</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="4"/>
-        <v>28.25</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="5"/>
-        <v>4.815072906367325</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="6"/>
-        <v>-4</v>
-      </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43">
@@ -2956,22 +2907,6 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G43">
-        <f t="shared" si="3"/>
-        <v>-29000</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="4"/>
-        <v>29.25</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="5"/>
-        <v>4.9083269131959844</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="6"/>
-        <v>-4</v>
-      </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44">
@@ -2989,22 +2924,6 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G44">
-        <f t="shared" si="3"/>
-        <v>-30000</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="4"/>
-        <v>30.25</v>
-      </c>
-      <c r="I44">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="6"/>
-        <v>-5</v>
-      </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45">
@@ -3022,22 +2941,6 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G45">
-        <f t="shared" si="3"/>
-        <v>-31000</v>
-      </c>
-      <c r="H45">
-        <f t="shared" si="4"/>
-        <v>31.25</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="5"/>
-        <v>5.0901699437494745</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="6"/>
-        <v>-5</v>
-      </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46">
@@ -3055,22 +2958,6 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G46">
-        <f t="shared" si="3"/>
-        <v>-32000</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="4"/>
-        <v>32.25</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="5"/>
-        <v>5.1789083458002736</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="6"/>
-        <v>-5</v>
-      </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47">
@@ -3088,22 +2975,6 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G47">
-        <f t="shared" si="3"/>
-        <v>-33000</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="4"/>
-        <v>33.25</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="5"/>
-        <v>5.2662812973353983</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="6"/>
-        <v>-5</v>
-      </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48">
@@ -3121,24 +2992,8 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G48">
-        <f t="shared" si="3"/>
-        <v>-34000</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="4"/>
-        <v>34.25</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="5"/>
-        <v>5.3523499553598128</v>
-      </c>
-      <c r="J48">
-        <f t="shared" si="6"/>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>35000</v>
       </c>
@@ -3154,24 +3009,8 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G49">
-        <f t="shared" si="3"/>
-        <v>-35000</v>
-      </c>
-      <c r="H49">
-        <f t="shared" si="4"/>
-        <v>35.25</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="5"/>
-        <v>5.4371710435189584</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="6"/>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>40000</v>
       </c>
@@ -3186,22 +3025,6 @@
       <c r="E50">
         <f t="shared" si="2"/>
         <v>5</v>
-      </c>
-      <c r="G50">
-        <f t="shared" si="3"/>
-        <v>-40000</v>
-      </c>
-      <c r="H50">
-        <f t="shared" si="4"/>
-        <v>40.25</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="5"/>
-        <v>5.8442887702247601</v>
-      </c>
-      <c r="J50">
-        <f t="shared" si="6"/>
-        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaking objective defense missions, a few bugfixes, checking difficulty scaling by distance
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Item Levels" sheetId="4" r:id="rId4"/>
     <sheet name="Mercenary Cost" sheetId="5" r:id="rId5"/>
     <sheet name="Relations Levels" sheetId="6" r:id="rId6"/>
+    <sheet name="Difficulty Scaling" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>BASE</t>
   </si>
@@ -120,6 +121,30 @@
   <si>
     <t>Where d = exp / Scale</t>
   </si>
+  <si>
+    <t>Dist / ly</t>
+  </si>
+  <si>
+    <t>Pow</t>
+  </si>
+  <si>
+    <t>Base Diff</t>
+  </si>
+  <si>
+    <t>Inner</t>
+  </si>
+  <si>
+    <t>Outer</t>
+  </si>
+  <si>
+    <t>Inner Rad</t>
+  </si>
+  <si>
+    <t>Inner bit</t>
+  </si>
+  <si>
+    <t>Outer bit</t>
+  </si>
 </sst>
 </file>
 
@@ -159,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -240,11 +265,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,6 +305,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -280,6 +324,1162 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Difficulty Scaling'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Base Diff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Difficulty Scaling'!$A$3:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Difficulty Scaling'!$D$3:$D$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="544718872"/>
+        <c:axId val="544726712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="544718872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544726712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="544726712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544718872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1681,7 +2881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1768,19 +2968,19 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G50" si="3">-B7</f>
+        <f t="shared" ref="G7:G39" si="3">-B7</f>
         <v>-200</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:H50" si="4">(-G7/1000) + 0.25</f>
+        <f t="shared" ref="H7:H39" si="4">(-G7/1000) + 0.25</f>
         <v>0.45</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I50" si="5">SQRT(H7)-0.5</f>
+        <f t="shared" ref="I7:I39" si="5">SQRT(H7)-0.5</f>
         <v>0.17082039324993692</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J50" si="6">-FLOOR(I7,1)-1</f>
+        <f t="shared" ref="J7:J39" si="6">-FLOOR(I7,1)-1</f>
         <v>-1</v>
       </c>
     </row>
@@ -3031,4 +4231,850 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>POWER(MIN($I$6,A3)/$I$3,$I$4)</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>POWER(MAX(0,A3-$I$6)/$J$3,$J$4)</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>1+ROUND(B3+C3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="17">
+        <v>1</v>
+      </c>
+      <c r="J3" s="17">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.5</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B48" si="0">POWER(MIN($I$6,A4)/$I$3,$I$4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C48" si="1">POWER(MAX(0,A4-$I$6)/$J$3,$J$4)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D48" si="2">1+ROUND(B4+C4,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="17">
+        <v>1</v>
+      </c>
+      <c r="J4" s="17">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="17">
+        <v>5</v>
+      </c>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2.5</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3.5</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4.5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.46198883129171492</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.77696950424091227</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>1.0531068011637541</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>1.3067017417552778</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>1.544752759668611</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>1.7711074679558145</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>1.9881768219176268</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>2.197601620895596</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>2.4005643849798499</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>2.5979541161172355</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>2.7904612136214872</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>2.9786358416662546</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>3.1629257048074275</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>3.3437015248821096</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>3.5212748169149664</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>3.6959106503337189</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>22</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>3.8678370351754467</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>23</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>4.037251971830587</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>24</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>4.2043288433264205</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>4.3692206064732311</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>4.5320630960351513</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>4.6929776628776771</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>4.8520733044687701</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>29</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>5.0094484032067692</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>30</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>5.1651921580697824</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>31</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>5.3193857737727885</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>5.4721034562358728</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>33</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>5.6234132519034921</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>34</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>5.7733777600998772</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>35</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>5.9220547413339508</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>36</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>6.069497639707075</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>6.2157560339272981</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>38</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>6.3608760286087715</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>39</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>6.5049005953291763</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>40</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>6.6478698711812365</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Making levels a bit easier
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>BASE</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Exp</t>
-  </si>
-  <si>
-    <t>Power</t>
   </si>
   <si>
     <t>Scale</t>
@@ -144,6 +141,18 @@
   </si>
   <si>
     <t>Outer bit</t>
+  </si>
+  <si>
+    <t>Util</t>
+  </si>
+  <si>
+    <t>SoldierLevelExperience</t>
+  </si>
+  <si>
+    <t>SoldierLevelExponent</t>
+  </si>
+  <si>
+    <t>SoldierLevelScale</t>
   </si>
 </sst>
 </file>
@@ -284,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -309,6 +318,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,7 +358,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -719,11 +735,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="544718872"/>
-        <c:axId val="544726712"/>
+        <c:axId val="639271248"/>
+        <c:axId val="639271640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="544718872"/>
+        <c:axId val="639271248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,12 +796,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="544726712"/>
+        <c:crossAx val="639271640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="544726712"/>
+        <c:axId val="639271640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="544718872"/>
+        <c:crossAx val="639271248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1769,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>2</v>
@@ -1781,10 +1797,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K4">
         <v>0.82</v>
@@ -2143,46 +2159,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G22"/>
+  <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="6"/>
+    <col min="6" max="6" width="19.140625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="19">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -2190,173 +2214,250 @@
         <f>INT($G$4*((POWER($G$2,$B4-2)*$G$3)-($G$3-1)))</f>
         <v>1000</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4">
+      <c r="D4" s="4">
+        <f t="shared" ref="D4:D22" si="0">ROUND($C4,2-(1+INT(LOG10($C4))))</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="19">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C22" si="0">INT($G$4*((POWER($G$2,$B5-2)*$G$3)-($G$3-1)))</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B5-2)*$G$3)-($G$3-1)))</f>
+        <v>3800</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <f t="shared" si="0"/>
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B6-2)*$G$3)-($G$3-1)))</f>
+        <v>8560</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>8600</v>
+      </c>
+      <c r="J6" s="21"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>5</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" si="0"/>
-        <v>11500</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B7-2)*$G$3)-($G$3-1)))</f>
+        <v>16652</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>6</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" si="0"/>
-        <v>23500</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B8-2)*$G$3)-($G$3-1)))</f>
+        <v>30408</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>7</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" si="0"/>
-        <v>47500</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B9-2)*$G$3)-($G$3-1)))</f>
+        <v>53794</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>8</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" si="0"/>
-        <v>95500</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B10-2)*$G$3)-($G$3-1)))</f>
+        <v>93550</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>94000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>9</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="0"/>
-        <v>191500</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B11-2)*$G$3)-($G$3-1)))</f>
+        <v>161135</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>10</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" si="0"/>
-        <v>383500</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B12-2)*$G$3)-($G$3-1)))</f>
+        <v>276030</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>11</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" si="0"/>
-        <v>767500</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B13-2)*$G$3)-($G$3-1)))</f>
+        <v>471351</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>470000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>12</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" si="0"/>
-        <v>1535500</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B14-2)*$G$3)-($G$3-1)))</f>
+        <v>803397</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>13</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" si="0"/>
-        <v>3071500</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B15-2)*$G$3)-($G$3-1)))</f>
+        <v>1367875</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>14</v>
       </c>
       <c r="C16" s="4">
-        <f t="shared" si="0"/>
-        <v>6143500</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B16-2)*$G$3)-($G$3-1)))</f>
+        <v>2327488</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>2300000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>15</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" si="0"/>
-        <v>12287500</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B17-2)*$G$3)-($G$3-1)))</f>
+        <v>3958831</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="0"/>
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>16</v>
       </c>
       <c r="C18" s="4">
-        <f t="shared" si="0"/>
-        <v>24575500</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B18-2)*$G$3)-($G$3-1)))</f>
+        <v>6732113</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>6700000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>17</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" si="0"/>
-        <v>49151500</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B19-2)*$G$3)-($G$3-1)))</f>
+        <v>11446692</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="0"/>
+        <v>11000000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>18</v>
       </c>
       <c r="C20" s="4">
-        <f t="shared" si="0"/>
-        <v>98303500</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B20-2)*$G$3)-($G$3-1)))</f>
+        <v>19461476</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="0"/>
+        <v>19000000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>19</v>
       </c>
       <c r="C21" s="4">
-        <f t="shared" si="0"/>
-        <v>196607500</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+        <f>INT($G$4*((POWER($G$2,$B21-2)*$G$3)-($G$3-1)))</f>
+        <v>33086610</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="0"/>
+        <v>33000000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>20</v>
       </c>
       <c r="C22" s="4">
-        <f t="shared" si="0"/>
-        <v>393215500</v>
+        <f>INT($G$4*((POWER($G$2,$B22-2)*$G$3)-($G$3-1)))</f>
+        <v>56249337</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>56000000</v>
       </c>
     </row>
   </sheetData>
@@ -2380,7 +2481,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="12">
         <v>1.5</v>
@@ -2388,7 +2489,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="12">
         <v>12</v>
@@ -2396,7 +2497,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="12">
         <v>12</v>
@@ -2404,7 +2505,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="12">
         <v>3</v>
@@ -2412,7 +2513,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="12">
         <v>3</v>
@@ -2420,16 +2521,16 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="E9" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -2559,10 +2660,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>6</v>
@@ -2576,14 +2677,14 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="14">
         <f>ROUND(POWER(B3+1,$H$2) * POWER($H$3,B3),2)</f>
         <v>1</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="14">
         <v>1</v>
@@ -2594,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="14">
         <f t="shared" ref="D4:D8" si="0">ROUND(POWER(B4+1,$H$2) * POWER($H$3,B4),2)</f>
@@ -2606,7 +2707,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="14">
         <f t="shared" si="0"/>
@@ -2618,7 +2719,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="14">
         <f t="shared" si="0"/>
@@ -2630,7 +2731,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="14">
         <f t="shared" si="0"/>
@@ -2642,7 +2743,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="14">
         <f t="shared" si="0"/>
@@ -2670,7 +2771,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -2682,7 +2783,7 @@
         <v>17.141191951192397</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3">
         <v>15</v>
@@ -2697,7 +2798,7 @@
         <v>39.176061534349742</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>1.1000000000000001</v>
@@ -2882,7 +2983,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2893,12 +2994,15 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -4237,7 +4341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -4245,22 +4349,22 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="D2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4280,7 +4384,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3" s="17">
         <v>1</v>
@@ -4306,7 +4410,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="17">
         <v>1</v>
@@ -4351,7 +4455,7 @@
         <v>3</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="17">
         <v>5</v>

</xml_diff>

<commit_message>
Change rate of colony expansion
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Mercenary Cost" sheetId="5" r:id="rId5"/>
     <sheet name="Relations Levels" sheetId="6" r:id="rId6"/>
     <sheet name="Difficulty Scaling" sheetId="7" r:id="rId7"/>
+    <sheet name="Colony Growth" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>BASE</t>
   </si>
@@ -154,12 +155,63 @@
   <si>
     <t>SoldierLevelScale</t>
   </si>
+  <si>
+    <t>double dt = Math.Pow(BaseSize, 1.7) * (Const.DaysPerYear * (2.5 + rand.NextDouble()));</t>
+  </si>
+  <si>
+    <t>double tdiff = Location.TDiff(Owner); // Abs value, doubled for +ve</t>
+  </si>
+  <si>
+    <t>// Tougher to grow if far from ideal temp</t>
+  </si>
+  <si>
+    <t>if (tdiff &gt; 20d) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    dt *= Math.Pow(1.1, (tdiff - 20d) / 10d);</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>Base Size</t>
+  </si>
+  <si>
+    <t>Tdiff</t>
+  </si>
+  <si>
+    <t>GrowthScale</t>
+  </si>
+  <si>
+    <t>GrowthExponent</t>
+  </si>
+  <si>
+    <t>Days Per Year</t>
+  </si>
+  <si>
+    <t>Growth Temp Scale</t>
+  </si>
+  <si>
+    <t>Growth Temp Base</t>
+  </si>
+  <si>
+    <t>Growth Temp Offset</t>
+  </si>
+  <si>
+    <t>MIN time</t>
+  </si>
+  <si>
+    <t>MAX time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,13 +236,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -293,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -326,6 +398,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,6 +437,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -735,11 +815,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="639271248"/>
-        <c:axId val="639271640"/>
+        <c:axId val="625918912"/>
+        <c:axId val="625919304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="639271248"/>
+        <c:axId val="625918912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,12 +876,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="639271640"/>
+        <c:crossAx val="625919304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="639271640"/>
+        <c:axId val="625919304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,7 +938,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="639271248"/>
+        <c:crossAx val="625918912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2161,7 +2241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -2211,11 +2291,11 @@
         <v>2</v>
       </c>
       <c r="C4" s="4">
-        <f>INT($G$4*((POWER($G$2,$B4-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" ref="C4:C22" si="0">INT($G$4*((POWER($G$2,$B4-2)*$G$3)-($G$3-1)))</f>
         <v>1000</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D22" si="0">ROUND($C4,2-(1+INT(LOG10($C4))))</f>
+        <f t="shared" ref="D4:D22" si="1">ROUND($C4,2-(1+INT(LOG10($C4))))</f>
         <v>1000</v>
       </c>
       <c r="F4" s="18" t="s">
@@ -2230,11 +2310,11 @@
         <v>3</v>
       </c>
       <c r="C5" s="4">
-        <f>INT($G$4*((POWER($G$2,$B5-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>3800</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3800</v>
       </c>
     </row>
@@ -2243,11 +2323,11 @@
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <f>INT($G$4*((POWER($G$2,$B6-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>8560</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8600</v>
       </c>
       <c r="J6" s="21"/>
@@ -2257,11 +2337,11 @@
         <v>5</v>
       </c>
       <c r="C7" s="4">
-        <f>INT($G$4*((POWER($G$2,$B7-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>16652</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17000</v>
       </c>
     </row>
@@ -2270,11 +2350,11 @@
         <v>6</v>
       </c>
       <c r="C8" s="4">
-        <f>INT($G$4*((POWER($G$2,$B8-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>30408</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30000</v>
       </c>
     </row>
@@ -2283,11 +2363,11 @@
         <v>7</v>
       </c>
       <c r="C9" s="4">
-        <f>INT($G$4*((POWER($G$2,$B9-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>53794</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54000</v>
       </c>
     </row>
@@ -2296,11 +2376,11 @@
         <v>8</v>
       </c>
       <c r="C10" s="4">
-        <f>INT($G$4*((POWER($G$2,$B10-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>93550</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>94000</v>
       </c>
     </row>
@@ -2309,11 +2389,11 @@
         <v>9</v>
       </c>
       <c r="C11" s="4">
-        <f>INT($G$4*((POWER($G$2,$B11-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>161135</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>160000</v>
       </c>
     </row>
@@ -2322,11 +2402,11 @@
         <v>10</v>
       </c>
       <c r="C12" s="4">
-        <f>INT($G$4*((POWER($G$2,$B12-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>276030</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280000</v>
       </c>
     </row>
@@ -2335,11 +2415,11 @@
         <v>11</v>
       </c>
       <c r="C13" s="4">
-        <f>INT($G$4*((POWER($G$2,$B13-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>471351</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>470000</v>
       </c>
     </row>
@@ -2348,11 +2428,11 @@
         <v>12</v>
       </c>
       <c r="C14" s="4">
-        <f>INT($G$4*((POWER($G$2,$B14-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>803397</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>800000</v>
       </c>
     </row>
@@ -2361,11 +2441,11 @@
         <v>13</v>
       </c>
       <c r="C15" s="4">
-        <f>INT($G$4*((POWER($G$2,$B15-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>1367875</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1400000</v>
       </c>
     </row>
@@ -2374,11 +2454,11 @@
         <v>14</v>
       </c>
       <c r="C16" s="4">
-        <f>INT($G$4*((POWER($G$2,$B16-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>2327488</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2300000</v>
       </c>
     </row>
@@ -2387,11 +2467,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="4">
-        <f>INT($G$4*((POWER($G$2,$B17-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>3958831</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4000000</v>
       </c>
     </row>
@@ -2400,11 +2480,11 @@
         <v>16</v>
       </c>
       <c r="C18" s="4">
-        <f>INT($G$4*((POWER($G$2,$B18-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>6732113</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6700000</v>
       </c>
     </row>
@@ -2413,11 +2493,11 @@
         <v>17</v>
       </c>
       <c r="C19" s="4">
-        <f>INT($G$4*((POWER($G$2,$B19-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>11446692</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11000000</v>
       </c>
     </row>
@@ -2426,11 +2506,11 @@
         <v>18</v>
       </c>
       <c r="C20" s="4">
-        <f>INT($G$4*((POWER($G$2,$B20-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>19461476</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19000000</v>
       </c>
     </row>
@@ -2439,11 +2519,11 @@
         <v>19</v>
       </c>
       <c r="C21" s="4">
-        <f>INT($G$4*((POWER($G$2,$B21-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>33086610</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33000000</v>
       </c>
     </row>
@@ -2452,11 +2532,11 @@
         <v>20</v>
       </c>
       <c r="C22" s="4">
-        <f>INT($G$4*((POWER($G$2,$B22-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" si="0"/>
         <v>56249337</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56000000</v>
       </c>
     </row>
@@ -5181,4 +5261,913 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>4</v>
+      </c>
+      <c r="G4" s="8">
+        <v>5</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4">
+        <v>2.5</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="23">
+        <v>0</v>
+      </c>
+      <c r="C5" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="24">
+        <f t="shared" ref="D5:G5" si="0">POWER(D$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
+        <v>8.7055056329612412</v>
+      </c>
+      <c r="E5" s="24">
+        <f t="shared" si="0"/>
+        <v>18.061685139605196</v>
+      </c>
+      <c r="F5" s="24">
+        <f t="shared" si="0"/>
+        <v>30.31433133020796</v>
+      </c>
+      <c r="G5" s="24">
+        <f t="shared" si="0"/>
+        <v>45.298728979855973</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5">
+        <v>365</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="23">
+        <v>10</v>
+      </c>
+      <c r="C6" s="24">
+        <f t="shared" ref="C6:G19" si="1">POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B6-$K$8)/$K$7))) / $K$5</f>
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="24">
+        <f t="shared" si="1"/>
+        <v>8.7055056329612412</v>
+      </c>
+      <c r="E6" s="24">
+        <f t="shared" si="1"/>
+        <v>18.061685139605196</v>
+      </c>
+      <c r="F6" s="24">
+        <f t="shared" si="1"/>
+        <v>30.31433133020796</v>
+      </c>
+      <c r="G6" s="24">
+        <f t="shared" si="1"/>
+        <v>45.298728979855973</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="23">
+        <v>20</v>
+      </c>
+      <c r="C7" s="24">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="24">
+        <f t="shared" si="1"/>
+        <v>8.7055056329612412</v>
+      </c>
+      <c r="E7" s="24">
+        <f t="shared" si="1"/>
+        <v>18.061685139605196</v>
+      </c>
+      <c r="F7" s="24">
+        <f t="shared" si="1"/>
+        <v>30.31433133020796</v>
+      </c>
+      <c r="G7" s="24">
+        <f t="shared" si="1"/>
+        <v>45.298728979855973</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="N7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="23">
+        <v>30</v>
+      </c>
+      <c r="C8" s="24">
+        <f t="shared" si="1"/>
+        <v>3.1922499999999991</v>
+      </c>
+      <c r="D8" s="24">
+        <f t="shared" si="1"/>
+        <v>11.116060142728207</v>
+      </c>
+      <c r="E8" s="24">
+        <f t="shared" si="1"/>
+        <v>23.062965754761869</v>
+      </c>
+      <c r="F8" s="24">
+        <f t="shared" si="1"/>
+        <v>38.708369675542535</v>
+      </c>
+      <c r="G8" s="24">
+        <f t="shared" si="1"/>
+        <v>57.841947034378073</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="N8" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="23">
+        <v>40</v>
+      </c>
+      <c r="C9" s="24">
+        <f t="shared" si="1"/>
+        <v>4.0761840249999981</v>
+      </c>
+      <c r="D9" s="24">
+        <f t="shared" si="1"/>
+        <v>14.194097196249643</v>
+      </c>
+      <c r="E9" s="24">
+        <f t="shared" si="1"/>
+        <v>29.449100972255422</v>
+      </c>
+      <c r="F9" s="24">
+        <f t="shared" si="1"/>
+        <v>49.426717238700256</v>
+      </c>
+      <c r="G9" s="24">
+        <f t="shared" si="1"/>
+        <v>73.858382168197352</v>
+      </c>
+      <c r="N9" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="23">
+        <v>50</v>
+      </c>
+      <c r="C10" s="24">
+        <f t="shared" si="1"/>
+        <v>5.2048793815224963</v>
+      </c>
+      <c r="D10" s="24">
+        <f t="shared" si="1"/>
+        <v>18.124442709891163</v>
+      </c>
+      <c r="E10" s="24">
+        <f t="shared" si="1"/>
+        <v>37.603557031472938</v>
+      </c>
+      <c r="F10" s="24">
+        <f t="shared" si="1"/>
+        <v>63.112975242096333</v>
+      </c>
+      <c r="G10" s="24">
+        <f t="shared" si="1"/>
+        <v>94.309768190571162</v>
+      </c>
+      <c r="N10" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="23">
+        <v>60</v>
+      </c>
+      <c r="C11" s="24">
+        <f t="shared" si="1"/>
+        <v>6.6461104822660744</v>
+      </c>
+      <c r="D11" s="24">
+        <f t="shared" si="1"/>
+        <v>23.143100896260023</v>
+      </c>
+      <c r="E11" s="24">
+        <f t="shared" si="1"/>
+        <v>48.01598197348779</v>
+      </c>
+      <c r="F11" s="24">
+        <f t="shared" si="1"/>
+        <v>80.5889580866328</v>
+      </c>
+      <c r="G11" s="24">
+        <f t="shared" si="1"/>
+        <v>120.4241430025403</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="23">
+        <v>70</v>
+      </c>
+      <c r="C12" s="24">
+        <f t="shared" si="1"/>
+        <v>8.4864184748055482</v>
+      </c>
+      <c r="D12" s="24">
+        <f t="shared" si="1"/>
+        <v>29.551425534434419</v>
+      </c>
+      <c r="E12" s="24">
+        <f t="shared" si="1"/>
+        <v>61.311607381946537</v>
+      </c>
+      <c r="F12" s="24">
+        <f t="shared" si="1"/>
+        <v>102.9040405808214</v>
+      </c>
+      <c r="G12" s="24">
+        <f t="shared" si="1"/>
+        <v>153.76958819994368</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="23">
+        <v>80</v>
+      </c>
+      <c r="C13" s="24">
+        <f t="shared" si="1"/>
+        <v>10.8363077504792</v>
+      </c>
+      <c r="D13" s="24">
+        <f t="shared" si="1"/>
+        <v>37.7342152649193</v>
+      </c>
+      <c r="E13" s="24">
+        <f t="shared" si="1"/>
+        <v>78.288791466007524</v>
+      </c>
+      <c r="F13" s="24">
+        <f t="shared" si="1"/>
+        <v>131.39816941765079</v>
+      </c>
+      <c r="G13" s="24">
+        <f t="shared" si="1"/>
+        <v>196.34838717250804</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="23">
+        <v>90</v>
+      </c>
+      <c r="C14" s="24">
+        <f t="shared" si="1"/>
+        <v>13.836881366586889</v>
+      </c>
+      <c r="D14" s="24">
+        <f t="shared" si="1"/>
+        <v>48.182819471775439</v>
+      </c>
+      <c r="E14" s="24">
+        <f t="shared" si="1"/>
+        <v>99.966957822944977</v>
+      </c>
+      <c r="F14" s="24">
+        <f t="shared" si="1"/>
+        <v>167.78232252939827</v>
+      </c>
+      <c r="G14" s="24">
+        <f t="shared" si="1"/>
+        <v>250.71725558057545</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="23">
+        <v>100</v>
+      </c>
+      <c r="C15" s="24">
+        <f t="shared" si="1"/>
+        <v>17.668313816994797</v>
+      </c>
+      <c r="D15" s="24">
+        <f t="shared" si="1"/>
+        <v>61.524642183510053</v>
+      </c>
+      <c r="E15" s="24">
+        <f t="shared" si="1"/>
+        <v>127.64780844411843</v>
+      </c>
+      <c r="F15" s="24">
+        <f t="shared" si="1"/>
+        <v>214.24124763778863</v>
+      </c>
+      <c r="G15" s="24">
+        <f t="shared" si="1"/>
+        <v>320.14086365083676</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="23">
+        <v>110</v>
+      </c>
+      <c r="C16" s="24">
+        <f t="shared" si="1"/>
+        <v>22.560669912920648</v>
+      </c>
+      <c r="D16" s="24">
+        <f t="shared" si="1"/>
+        <v>78.560815604123974</v>
+      </c>
+      <c r="E16" s="24">
+        <f t="shared" si="1"/>
+        <v>162.99348660229478</v>
+      </c>
+      <c r="F16" s="24">
+        <f t="shared" si="1"/>
+        <v>273.56464910869221</v>
+      </c>
+      <c r="G16" s="24">
+        <f t="shared" si="1"/>
+        <v>408.78786879575335</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="23">
+        <v>120</v>
+      </c>
+      <c r="C17" s="24">
+        <f t="shared" si="1"/>
+        <v>28.807719411808367</v>
+      </c>
+      <c r="D17" s="24">
+        <f t="shared" si="1"/>
+        <v>100.31430544490587</v>
+      </c>
+      <c r="E17" s="24">
+        <f t="shared" si="1"/>
+        <v>208.12638304247014</v>
+      </c>
+      <c r="F17" s="24">
+        <f t="shared" si="1"/>
+        <v>349.31470044688899</v>
+      </c>
+      <c r="G17" s="24">
+        <f t="shared" si="1"/>
+        <v>521.98122966529729</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="23">
+        <v>130</v>
+      </c>
+      <c r="C18" s="24">
+        <f t="shared" si="1"/>
+        <v>36.7845769169381</v>
+      </c>
+      <c r="D18" s="24">
+        <f t="shared" si="1"/>
+        <v>128.09133662260027</v>
+      </c>
+      <c r="E18" s="24">
+        <f t="shared" si="1"/>
+        <v>265.75657850693005</v>
+      </c>
+      <c r="F18" s="24">
+        <f t="shared" si="1"/>
+        <v>446.03994100063244</v>
+      </c>
+      <c r="G18" s="24">
+        <f t="shared" si="1"/>
+        <v>666.51783215961791</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="23">
+        <v>140</v>
+      </c>
+      <c r="C19" s="24">
+        <f t="shared" si="1"/>
+        <v>46.97022626523826</v>
+      </c>
+      <c r="D19" s="24">
+        <f t="shared" si="1"/>
+        <v>163.55982773339827</v>
+      </c>
+      <c r="E19" s="24">
+        <f t="shared" si="1"/>
+        <v>339.34457509549895</v>
+      </c>
+      <c r="F19" s="24">
+        <f t="shared" si="1"/>
+        <v>569.54840066370753</v>
+      </c>
+      <c r="G19" s="24">
+        <f t="shared" si="1"/>
+        <v>851.07661988461609</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8">
+        <v>2</v>
+      </c>
+      <c r="E26" s="8">
+        <v>3</v>
+      </c>
+      <c r="F26" s="8">
+        <v>4</v>
+      </c>
+      <c r="G26" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="23">
+        <v>0</v>
+      </c>
+      <c r="C27" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+        <v>3.5</v>
+      </c>
+      <c r="D27" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+        <v>12.187707886145738</v>
+      </c>
+      <c r="E27" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+        <v>25.286359195447272</v>
+      </c>
+      <c r="F27" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+        <v>42.44006386229114</v>
+      </c>
+      <c r="G27" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+        <v>63.418220571798358</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="23">
+        <v>10</v>
+      </c>
+      <c r="C28" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+        <v>3.5</v>
+      </c>
+      <c r="D28" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+        <v>12.187707886145738</v>
+      </c>
+      <c r="E28" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+        <v>25.286359195447272</v>
+      </c>
+      <c r="F28" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+        <v>42.44006386229114</v>
+      </c>
+      <c r="G28" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+        <v>63.418220571798358</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="23">
+        <v>20</v>
+      </c>
+      <c r="C29" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+        <v>3.5</v>
+      </c>
+      <c r="D29" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+        <v>12.187707886145738</v>
+      </c>
+      <c r="E29" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+        <v>25.286359195447272</v>
+      </c>
+      <c r="F29" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+        <v>42.44006386229114</v>
+      </c>
+      <c r="G29" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+        <v>63.418220571798358</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="23">
+        <v>30</v>
+      </c>
+      <c r="C30" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+        <v>4.4691499999999991</v>
+      </c>
+      <c r="D30" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+        <v>15.56248419981949</v>
+      </c>
+      <c r="E30" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+        <v>32.288152056666611</v>
+      </c>
+      <c r="F30" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+        <v>54.191717545759545</v>
+      </c>
+      <c r="G30" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+        <v>80.978725848129301</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="23">
+        <v>40</v>
+      </c>
+      <c r="C31" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+        <v>5.7066576349999965</v>
+      </c>
+      <c r="D31" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+        <v>19.871736074749503</v>
+      </c>
+      <c r="E31" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+        <v>41.228741361157589</v>
+      </c>
+      <c r="F31" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+        <v>69.197404134180346</v>
+      </c>
+      <c r="G31" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+        <v>103.40173503547628</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="23">
+        <v>50</v>
+      </c>
+      <c r="C32" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+        <v>7.2868311341314937</v>
+      </c>
+      <c r="D32" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+        <v>25.374219793847633</v>
+      </c>
+      <c r="E32" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+        <v>52.644979844062107</v>
+      </c>
+      <c r="F32" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+        <v>88.358165338934867</v>
+      </c>
+      <c r="G32" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+        <v>132.03367546679962</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="23">
+        <v>60</v>
+      </c>
+      <c r="C33" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+        <v>9.3045546751725041</v>
+      </c>
+      <c r="D33" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+        <v>32.400341254764037</v>
+      </c>
+      <c r="E33" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+        <v>67.222374762882893</v>
+      </c>
+      <c r="F33" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+        <v>112.82454132128592</v>
+      </c>
+      <c r="G33" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+        <v>168.59380020355641</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="23">
+        <v>70</v>
+      </c>
+      <c r="C34" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+        <v>11.880985864727768</v>
+      </c>
+      <c r="D34" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+        <v>41.371995748208192</v>
+      </c>
+      <c r="E34" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+        <v>85.83625033472515</v>
+      </c>
+      <c r="F34" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+        <v>144.06565681314996</v>
+      </c>
+      <c r="G34" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+        <v>215.27742347992114</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="23">
+        <v>80</v>
+      </c>
+      <c r="C35" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+        <v>15.170830850670884</v>
+      </c>
+      <c r="D35" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+        <v>52.82790137088702</v>
+      </c>
+      <c r="E35" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+        <v>109.6043080524105</v>
+      </c>
+      <c r="F35" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+        <v>183.95743718471113</v>
+      </c>
+      <c r="G35" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+        <v>274.88774204151122</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="23">
+        <v>90</v>
+      </c>
+      <c r="C36" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+        <v>19.371633913221643</v>
+      </c>
+      <c r="D36" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+        <v>67.455947260485615</v>
+      </c>
+      <c r="E36" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+        <v>139.95374095212296</v>
+      </c>
+      <c r="F36" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+        <v>234.89525154115753</v>
+      </c>
+      <c r="G36" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+        <v>351.00415781280554</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="23">
+        <v>100</v>
+      </c>
+      <c r="C37" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+        <v>24.735639343792712</v>
+      </c>
+      <c r="D37" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+        <v>86.13449905691408</v>
+      </c>
+      <c r="E37" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+        <v>178.70693182176578</v>
+      </c>
+      <c r="F37" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+        <v>299.93774669290406</v>
+      </c>
+      <c r="G37" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+        <v>448.19720911117139</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="23">
+        <v>110</v>
+      </c>
+      <c r="C38" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+        <v>31.584937878088908</v>
+      </c>
+      <c r="D38" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+        <v>109.98514184577355</v>
+      </c>
+      <c r="E38" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+        <v>228.19088124321266</v>
+      </c>
+      <c r="F38" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+        <v>382.99050875216915</v>
+      </c>
+      <c r="G38" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+        <v>572.30301631405462</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="23">
+        <v>120</v>
+      </c>
+      <c r="C39" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+        <v>40.330807176531721</v>
+      </c>
+      <c r="D39" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+        <v>140.44002762286823</v>
+      </c>
+      <c r="E39" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+        <v>291.3769362594582</v>
+      </c>
+      <c r="F39" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+        <v>489.04058062564462</v>
+      </c>
+      <c r="G39" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+        <v>730.77372153141607</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="23">
+        <v>130</v>
+      </c>
+      <c r="C40" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+        <v>51.498407683713339</v>
+      </c>
+      <c r="D40" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+        <v>179.32787127164036</v>
+      </c>
+      <c r="E40" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+        <v>372.05920990970202</v>
+      </c>
+      <c r="F40" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+        <v>624.45591740088537</v>
+      </c>
+      <c r="G40" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+        <v>933.12496502346505</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="23">
+        <v>140</v>
+      </c>
+      <c r="C41" s="24">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+        <v>65.758316771333554</v>
+      </c>
+      <c r="D41" s="24">
+        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+        <v>228.98375882675759</v>
+      </c>
+      <c r="E41" s="24">
+        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+        <v>475.0824051336985</v>
+      </c>
+      <c r="F41" s="24">
+        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+        <v>797.36776092919047</v>
+      </c>
+      <c r="G41" s="24">
+        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+        <v>1191.5072678384624</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove RequiredRace for items and move it all to research; ItemType stamina cost; Fix creature freq scaling;
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
-  <si>
-    <t>BASE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>Width</t>
   </si>
@@ -203,15 +200,27 @@
   <si>
     <t>MAX time</t>
   </si>
+  <si>
+    <t>Floor Fract</t>
+  </si>
+  <si>
+    <t>Floor Count</t>
+  </si>
+  <si>
+    <t>FREQ SCALE</t>
+  </si>
+  <si>
+    <t>int nCreatures = (int)(Math.Pow(nFloorTiles, Const.CreatureCountExponent) * ((double)soldierCount + 1d) * cg.QuantityScale * Const.CreatureFrequencyScale);</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +253,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
@@ -365,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -377,7 +393,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -402,9 +417,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +456,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -815,11 +833,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="625918912"/>
-        <c:axId val="625919304"/>
+        <c:axId val="647433336"/>
+        <c:axId val="647434512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="625918912"/>
+        <c:axId val="647433336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,12 +894,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="625919304"/>
+        <c:crossAx val="647434512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="625919304"/>
+        <c:axId val="647434512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="625918912"/>
+        <c:crossAx val="647433336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1841,52 +1859,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K19"/>
+  <dimension ref="B4:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J3" t="s">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="K3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="E4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="27">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>20</v>
       </c>
@@ -1894,22 +1911,35 @@
         <v>20</v>
       </c>
       <c r="D5" s="7">
-        <f>B5*C5</f>
+        <f>$B5*$C5</f>
         <v>400</v>
       </c>
       <c r="E5" s="6">
-        <f>POWER(D5,$K$4)</f>
-        <v>136.04706997702485</v>
-      </c>
-      <c r="F5" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F5" s="6">
+        <f>$D5*$E5</f>
+        <v>320</v>
+      </c>
+      <c r="G5" s="6">
+        <f>POWER($F5,$M$4)</f>
+        <v>142.7016456115976</v>
+      </c>
+      <c r="H5" s="7">
         <v>1</v>
       </c>
-      <c r="G5">
-        <f>INT($E5/($K$3-($F5*2)))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f>INT($G5*($H5+1)*$M$5)</f>
+        <v>2</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="27">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>20</v>
       </c>
@@ -1917,22 +1947,29 @@
         <v>20</v>
       </c>
       <c r="D6" s="7">
-        <f t="shared" ref="D6:D19" si="0">B6*C6</f>
+        <f t="shared" ref="D6:D34" si="0">$B6*$C6</f>
         <v>400</v>
       </c>
       <c r="E6" s="6">
-        <f t="shared" ref="E6:E19" si="1">POWER(D6,$K$4)</f>
-        <v>136.04706997702485</v>
-      </c>
-      <c r="F6" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" ref="F6:G21" si="1">$D6*$E6</f>
+        <v>320</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" ref="G6:H21" si="2">POWER($F6,$M$4)</f>
+        <v>142.7016456115976</v>
+      </c>
+      <c r="H6" s="7">
         <v>2</v>
       </c>
-      <c r="G6">
-        <f t="shared" ref="G6:G19" si="2">INT($E6/($K$3-($F6*2)))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" ref="I6:J21" si="3">INT($G6*($H6+1)*$M$5)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>20</v>
       </c>
@@ -1944,18 +1981,25 @@
         <v>400</v>
       </c>
       <c r="E7" s="6">
-        <f t="shared" si="1"/>
-        <v>136.04706997702485</v>
-      </c>
-      <c r="F7" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="2"/>
+        <v>142.7016456115976</v>
+      </c>
+      <c r="H7" s="7">
         <v>3</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>30</v>
       </c>
@@ -1967,18 +2011,25 @@
         <v>600</v>
       </c>
       <c r="E8" s="6">
-        <f t="shared" si="1"/>
-        <v>189.70729227194849</v>
-      </c>
-      <c r="F8" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="2"/>
+        <v>202.24018978153325</v>
+      </c>
+      <c r="H8" s="7">
         <v>1</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>30</v>
       </c>
@@ -1990,18 +2041,25 @@
         <v>600</v>
       </c>
       <c r="E9" s="6">
-        <f t="shared" si="1"/>
-        <v>189.70729227194849</v>
-      </c>
-      <c r="F9" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="2"/>
+        <v>202.24018978153325</v>
+      </c>
+      <c r="H9" s="7">
         <v>2</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>30</v>
       </c>
@@ -2013,18 +2071,25 @@
         <v>600</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" si="1"/>
-        <v>189.70729227194849</v>
-      </c>
-      <c r="F10" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="2"/>
+        <v>202.24018978153325</v>
+      </c>
+      <c r="H10" s="7">
         <v>3</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
+      <c r="I10">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>30</v>
       </c>
@@ -2036,18 +2101,25 @@
         <v>900</v>
       </c>
       <c r="E11" s="6">
-        <f t="shared" si="1"/>
-        <v>264.53239123218282</v>
-      </c>
-      <c r="F11" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="1"/>
+        <v>720</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="2"/>
+        <v>286.61964049240453</v>
+      </c>
+      <c r="H11" s="7">
         <v>1</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>30</v>
       </c>
@@ -2059,18 +2131,28 @@
         <v>900</v>
       </c>
       <c r="E12" s="6">
-        <f t="shared" si="1"/>
-        <v>264.53239123218282</v>
-      </c>
-      <c r="F12" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="1"/>
+        <v>720</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="2"/>
+        <v>286.61964049240453</v>
+      </c>
+      <c r="H12" s="7">
         <v>2</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>30</v>
       </c>
@@ -2082,18 +2164,25 @@
         <v>900</v>
       </c>
       <c r="E13" s="6">
-        <f t="shared" si="1"/>
-        <v>264.53239123218282</v>
-      </c>
-      <c r="F13" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="1"/>
+        <v>720</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="2"/>
+        <v>286.61964049240453</v>
+      </c>
+      <c r="H13" s="7">
         <v>3</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>35</v>
       </c>
@@ -2105,18 +2194,25 @@
         <v>1225</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" si="1"/>
-        <v>340.62113577610364</v>
-      </c>
-      <c r="F14" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="1"/>
+        <v>980</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="2"/>
+        <v>373.64091341151982</v>
+      </c>
+      <c r="H14" s="7">
         <v>2</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>35</v>
       </c>
@@ -2128,18 +2224,25 @@
         <v>1225</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="1"/>
-        <v>340.62113577610364</v>
-      </c>
-      <c r="F15" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="1"/>
+        <v>980</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="2"/>
+        <v>373.64091341151982</v>
+      </c>
+      <c r="H15" s="7">
         <v>4</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>40</v>
       </c>
@@ -2151,18 +2254,25 @@
         <v>1600</v>
       </c>
       <c r="E16" s="6">
-        <f t="shared" si="1"/>
-        <v>424.01223237076442</v>
-      </c>
-      <c r="F16" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="1"/>
+        <v>1280</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="2"/>
+        <v>470.11117390004944</v>
+      </c>
+      <c r="H16" s="7">
         <v>2</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>40</v>
       </c>
@@ -2174,18 +2284,25 @@
         <v>1600</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="1"/>
-        <v>424.01223237076442</v>
-      </c>
-      <c r="F17" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="1"/>
+        <v>1280</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="2"/>
+        <v>470.11117390004944</v>
+      </c>
+      <c r="H17" s="7">
         <v>4</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>50</v>
       </c>
@@ -2196,19 +2313,26 @@
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="E18" s="11">
-        <f t="shared" si="1"/>
-        <v>611.37940805570872</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="E18" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="2"/>
+        <v>690.05831961875413</v>
+      </c>
+      <c r="H18" s="7">
         <v>3</v>
       </c>
-      <c r="G18">
-        <f t="shared" si="2"/>
+      <c r="I18">
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>50</v>
       </c>
@@ -2220,15 +2344,472 @@
         <v>2500</v>
       </c>
       <c r="E19" s="6">
-        <f t="shared" si="1"/>
-        <v>611.37940805570872</v>
-      </c>
-      <c r="F19" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" si="2"/>
+        <v>690.05831961875413</v>
+      </c>
+      <c r="H19" s="7">
         <v>4</v>
       </c>
-      <c r="G19">
-        <f t="shared" si="2"/>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5">
+        <v>20</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F20" s="6">
+        <f>$D20*$E20</f>
+        <v>240</v>
+      </c>
+      <c r="G20" s="6">
+        <f>POWER($F20,$M$4)</f>
+        <v>111.42474987806408</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f>INT($G20*($H20+1)*$M$5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5">
+        <v>20</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="2"/>
+        <v>111.42474987806408</v>
+      </c>
+      <c r="H21" s="7">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5">
+        <v>20</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" ref="F22:G34" si="4">$D22*$E22</f>
+        <v>240</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" ref="G22:H34" si="5">POWER($F22,$M$4)</f>
+        <v>111.42474987806408</v>
+      </c>
+      <c r="H22" s="7">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22:I34" si="6">INT($G22*($H22+1)*$M$5)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23">
         <v>30</v>
+      </c>
+      <c r="C23" s="5">
+        <v>20</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" si="4"/>
+        <v>360</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="5"/>
+        <v>157.91382408464779</v>
+      </c>
+      <c r="H23" s="7">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24" s="5">
+        <v>20</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="4"/>
+        <v>360</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="5"/>
+        <v>157.91382408464779</v>
+      </c>
+      <c r="H24" s="7">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>30</v>
+      </c>
+      <c r="C25" s="5">
+        <v>20</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="4"/>
+        <v>360</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="5"/>
+        <v>157.91382408464779</v>
+      </c>
+      <c r="H25" s="7">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>30</v>
+      </c>
+      <c r="C26" s="5">
+        <v>30</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="4"/>
+        <v>540</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="5"/>
+        <v>223.79925343629878</v>
+      </c>
+      <c r="H26" s="7">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="C27" s="5">
+        <v>30</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="4"/>
+        <v>540</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="5"/>
+        <v>223.79925343629878</v>
+      </c>
+      <c r="H27" s="7">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28" s="5">
+        <v>30</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="4"/>
+        <v>540</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="5"/>
+        <v>223.79925343629878</v>
+      </c>
+      <c r="H28" s="7">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>35</v>
+      </c>
+      <c r="C29" s="5">
+        <v>35</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>1225</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" si="4"/>
+        <v>735</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="5"/>
+        <v>291.74747875301625</v>
+      </c>
+      <c r="H29" s="7">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>35</v>
+      </c>
+      <c r="C30" s="5">
+        <v>35</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>1225</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" si="4"/>
+        <v>735</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="5"/>
+        <v>291.74747875301625</v>
+      </c>
+      <c r="H30" s="7">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>40</v>
+      </c>
+      <c r="C31" s="5">
+        <v>40</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F31" s="6">
+        <f t="shared" si="4"/>
+        <v>960</v>
+      </c>
+      <c r="G31" s="6">
+        <f t="shared" si="5"/>
+        <v>367.07369240343866</v>
+      </c>
+      <c r="H31" s="7">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>40</v>
+      </c>
+      <c r="C32" s="5">
+        <v>40</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F32" s="6">
+        <f t="shared" si="4"/>
+        <v>960</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" si="5"/>
+        <v>367.07369240343866</v>
+      </c>
+      <c r="H32" s="7">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>50</v>
+      </c>
+      <c r="C33" s="5">
+        <v>50</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F33" s="6">
+        <f t="shared" si="4"/>
+        <v>1500</v>
+      </c>
+      <c r="G33" s="6">
+        <f t="shared" si="5"/>
+        <v>538.81351777871805</v>
+      </c>
+      <c r="H33" s="7">
+        <v>3</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>50</v>
+      </c>
+      <c r="C34" s="5">
+        <v>50</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F34" s="6">
+        <f t="shared" si="4"/>
+        <v>1500</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="5"/>
+        <v>538.81351777871805</v>
+      </c>
+      <c r="H34" s="7">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="6"/>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2250,22 +2831,22 @@
     <col min="3" max="3" width="12" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="6"/>
-    <col min="6" max="6" width="19.140625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="19"/>
+    <col min="6" max="6" width="19.140625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>5</v>
+      <c r="B2" s="19" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="19">
+        <v>5</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="18">
         <v>1.7</v>
       </c>
     </row>
@@ -2279,10 +2860,10 @@
       <c r="D3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="19">
+      <c r="F3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2298,10 +2879,10 @@
         <f t="shared" ref="D4:D22" si="1">ROUND($C4,2-(1+INT(LOG10($C4))))</f>
         <v>1000</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="19">
+      <c r="F4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="18">
         <v>1000</v>
       </c>
     </row>
@@ -2330,7 +2911,7 @@
         <f t="shared" si="1"/>
         <v>8600</v>
       </c>
-      <c r="J6" s="21"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -2560,57 +3141,57 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="12">
+      <c r="B2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="11">
         <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="12">
+      <c r="B4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="11">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="E9" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -2736,96 +3317,96 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="H2" s="13">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="14">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="14">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <f>ROUND(POWER(B3+1,$H$2) * POWER($H$3,B3),2)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="14">
+      <c r="G3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="14">
+        <v>20</v>
+      </c>
+      <c r="D4" s="13">
         <f t="shared" ref="D4:D8" si="0">ROUND(POWER(B4+1,$H$2) * POWER($H$3,B4),2)</f>
         <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="13">
+        <f t="shared" si="0"/>
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="14">
-        <f t="shared" si="0"/>
-        <v>4.41</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="14">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" s="13">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="13">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="14">
-        <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="14">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" s="13">
+        <f t="shared" si="0"/>
+        <v>8.7799999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="13">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="14">
-        <f t="shared" si="0"/>
-        <v>8.7799999999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="14">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <f t="shared" si="0"/>
         <v>11.23</v>
       </c>
@@ -2848,10 +3429,10 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -2863,7 +3444,7 @@
         <v>17.141191951192397</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>15</v>
@@ -2878,7 +3459,7 @@
         <v>39.176061534349742</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <v>1.1000000000000001</v>
@@ -2893,7 +3474,7 @@
         <v>67.152439065201392</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>1.4</v>
@@ -3074,33 +3655,33 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>5</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4428,23 +5009,23 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4463,13 +5044,13 @@
         <f>1+ROUND(B3+C3,0)</f>
         <v>1</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="17">
+      <c r="H3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="16">
         <v>1</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="16">
         <v>2.8</v>
       </c>
     </row>
@@ -4489,13 +5070,13 @@
         <f t="shared" ref="D4:D48" si="2">1+ROUND(B4+C4,0)</f>
         <v>2</v>
       </c>
-      <c r="H4" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="17">
+      <c r="H4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="16">
         <v>1</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="16">
         <v>0.75</v>
       </c>
     </row>
@@ -4515,8 +5096,8 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -4534,13 +5115,13 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="17">
+      <c r="H6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="16">
         <v>5</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -5267,31 +5848,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>55</v>
+      <c r="B2" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>50</v>
+      <c r="E3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="K3">
         <v>1.8</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
-        <v>48</v>
+      <c r="B4" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
@@ -5308,472 +5889,472 @@
       <c r="G4" s="8">
         <v>5</v>
       </c>
-      <c r="J4" s="22" t="s">
-        <v>49</v>
+      <c r="J4" s="21" t="s">
+        <v>48</v>
       </c>
       <c r="K4">
         <v>2.5</v>
       </c>
-      <c r="N4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
+      <c r="N4" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <v>0</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <f>POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
         <v>2.5</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <f t="shared" ref="D5:G5" si="0">POWER(D$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
         <v>8.7055056329612412</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <f t="shared" si="0"/>
         <v>18.061685139605196</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <f t="shared" si="0"/>
         <v>30.31433133020796</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <f t="shared" si="0"/>
         <v>45.298728979855973</v>
       </c>
-      <c r="J5" s="22" t="s">
-        <v>51</v>
+      <c r="J5" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="K5">
         <v>365</v>
       </c>
-      <c r="N5" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
+      <c r="N5" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>10</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <f t="shared" ref="C6:G19" si="1">POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B6-$K$8)/$K$7))) / $K$5</f>
         <v>2.5</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <f t="shared" si="1"/>
         <v>8.7055056329612412</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="23">
         <f t="shared" si="1"/>
         <v>18.061685139605196</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <f t="shared" si="1"/>
         <v>30.31433133020796</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="23">
         <f t="shared" si="1"/>
         <v>45.298728979855973</v>
       </c>
-      <c r="J6" s="22" t="s">
-        <v>53</v>
+      <c r="J6" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="K6">
         <v>1.1299999999999999</v>
       </c>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>20</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="23">
         <f t="shared" si="1"/>
         <v>8.7055056329612412</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="23">
         <f t="shared" si="1"/>
         <v>18.061685139605196</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <f t="shared" si="1"/>
         <v>30.31433133020796</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="23">
         <f t="shared" si="1"/>
         <v>45.298728979855973</v>
       </c>
-      <c r="J7" s="22" t="s">
-        <v>52</v>
+      <c r="J7" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="K7">
         <v>5</v>
       </c>
-      <c r="N7" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
+      <c r="N7" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>30</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <f t="shared" si="1"/>
         <v>3.1922499999999991</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <f t="shared" si="1"/>
         <v>11.116060142728207</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="23">
         <f t="shared" si="1"/>
         <v>23.062965754761869</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <f t="shared" si="1"/>
         <v>38.708369675542535</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="23">
         <f t="shared" si="1"/>
         <v>57.841947034378073</v>
       </c>
-      <c r="J8" s="22" t="s">
-        <v>54</v>
+      <c r="J8" s="21" t="s">
+        <v>53</v>
       </c>
       <c r="K8">
         <v>20</v>
       </c>
-      <c r="N8" s="26" t="s">
+      <c r="N8" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="22">
+        <v>40</v>
+      </c>
+      <c r="C9" s="23">
+        <f t="shared" si="1"/>
+        <v>4.0761840249999981</v>
+      </c>
+      <c r="D9" s="23">
+        <f t="shared" si="1"/>
+        <v>14.194097196249643</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" si="1"/>
+        <v>29.449100972255422</v>
+      </c>
+      <c r="F9" s="23">
+        <f t="shared" si="1"/>
+        <v>49.426717238700256</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" si="1"/>
+        <v>73.858382168197352</v>
+      </c>
+      <c r="N9" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="23">
-        <v>40</v>
-      </c>
-      <c r="C9" s="24">
-        <f t="shared" si="1"/>
-        <v>4.0761840249999981</v>
-      </c>
-      <c r="D9" s="24">
-        <f t="shared" si="1"/>
-        <v>14.194097196249643</v>
-      </c>
-      <c r="E9" s="24">
-        <f t="shared" si="1"/>
-        <v>29.449100972255422</v>
-      </c>
-      <c r="F9" s="24">
-        <f t="shared" si="1"/>
-        <v>49.426717238700256</v>
-      </c>
-      <c r="G9" s="24">
-        <f t="shared" si="1"/>
-        <v>73.858382168197352</v>
-      </c>
-      <c r="N9" s="26" t="s">
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="22">
+        <v>50</v>
+      </c>
+      <c r="C10" s="23">
+        <f t="shared" si="1"/>
+        <v>5.2048793815224963</v>
+      </c>
+      <c r="D10" s="23">
+        <f t="shared" si="1"/>
+        <v>18.124442709891163</v>
+      </c>
+      <c r="E10" s="23">
+        <f t="shared" si="1"/>
+        <v>37.603557031472938</v>
+      </c>
+      <c r="F10" s="23">
+        <f t="shared" si="1"/>
+        <v>63.112975242096333</v>
+      </c>
+      <c r="G10" s="23">
+        <f t="shared" si="1"/>
+        <v>94.309768190571162</v>
+      </c>
+      <c r="N10" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="23">
-        <v>50</v>
-      </c>
-      <c r="C10" s="24">
-        <f t="shared" si="1"/>
-        <v>5.2048793815224963</v>
-      </c>
-      <c r="D10" s="24">
-        <f t="shared" si="1"/>
-        <v>18.124442709891163</v>
-      </c>
-      <c r="E10" s="24">
-        <f t="shared" si="1"/>
-        <v>37.603557031472938</v>
-      </c>
-      <c r="F10" s="24">
-        <f t="shared" si="1"/>
-        <v>63.112975242096333</v>
-      </c>
-      <c r="G10" s="24">
-        <f t="shared" si="1"/>
-        <v>94.309768190571162</v>
-      </c>
-      <c r="N10" s="26" t="s">
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="22">
+        <v>60</v>
+      </c>
+      <c r="C11" s="23">
+        <f t="shared" si="1"/>
+        <v>6.6461104822660744</v>
+      </c>
+      <c r="D11" s="23">
+        <f t="shared" si="1"/>
+        <v>23.143100896260023</v>
+      </c>
+      <c r="E11" s="23">
+        <f t="shared" si="1"/>
+        <v>48.01598197348779</v>
+      </c>
+      <c r="F11" s="23">
+        <f t="shared" si="1"/>
+        <v>80.5889580866328</v>
+      </c>
+      <c r="G11" s="23">
+        <f t="shared" si="1"/>
+        <v>120.4241430025403</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="22">
+        <v>70</v>
+      </c>
+      <c r="C12" s="23">
+        <f t="shared" si="1"/>
+        <v>8.4864184748055482</v>
+      </c>
+      <c r="D12" s="23">
+        <f t="shared" si="1"/>
+        <v>29.551425534434419</v>
+      </c>
+      <c r="E12" s="23">
+        <f t="shared" si="1"/>
+        <v>61.311607381946537</v>
+      </c>
+      <c r="F12" s="23">
+        <f t="shared" si="1"/>
+        <v>102.9040405808214</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="1"/>
+        <v>153.76958819994368</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="22">
+        <v>80</v>
+      </c>
+      <c r="C13" s="23">
+        <f t="shared" si="1"/>
+        <v>10.8363077504792</v>
+      </c>
+      <c r="D13" s="23">
+        <f t="shared" si="1"/>
+        <v>37.7342152649193</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="1"/>
+        <v>78.288791466007524</v>
+      </c>
+      <c r="F13" s="23">
+        <f t="shared" si="1"/>
+        <v>131.39816941765079</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="1"/>
+        <v>196.34838717250804</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="22">
+        <v>90</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" si="1"/>
+        <v>13.836881366586889</v>
+      </c>
+      <c r="D14" s="23">
+        <f t="shared" si="1"/>
+        <v>48.182819471775439</v>
+      </c>
+      <c r="E14" s="23">
+        <f t="shared" si="1"/>
+        <v>99.966957822944977</v>
+      </c>
+      <c r="F14" s="23">
+        <f t="shared" si="1"/>
+        <v>167.78232252939827</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="1"/>
+        <v>250.71725558057545</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="22">
+        <v>100</v>
+      </c>
+      <c r="C15" s="23">
+        <f t="shared" si="1"/>
+        <v>17.668313816994797</v>
+      </c>
+      <c r="D15" s="23">
+        <f t="shared" si="1"/>
+        <v>61.524642183510053</v>
+      </c>
+      <c r="E15" s="23">
+        <f t="shared" si="1"/>
+        <v>127.64780844411843</v>
+      </c>
+      <c r="F15" s="23">
+        <f t="shared" si="1"/>
+        <v>214.24124763778863</v>
+      </c>
+      <c r="G15" s="23">
+        <f t="shared" si="1"/>
+        <v>320.14086365083676</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="22">
+        <v>110</v>
+      </c>
+      <c r="C16" s="23">
+        <f t="shared" si="1"/>
+        <v>22.560669912920648</v>
+      </c>
+      <c r="D16" s="23">
+        <f t="shared" si="1"/>
+        <v>78.560815604123974</v>
+      </c>
+      <c r="E16" s="23">
+        <f t="shared" si="1"/>
+        <v>162.99348660229478</v>
+      </c>
+      <c r="F16" s="23">
+        <f t="shared" si="1"/>
+        <v>273.56464910869221</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" si="1"/>
+        <v>408.78786879575335</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="22">
+        <v>120</v>
+      </c>
+      <c r="C17" s="23">
+        <f t="shared" si="1"/>
+        <v>28.807719411808367</v>
+      </c>
+      <c r="D17" s="23">
+        <f t="shared" si="1"/>
+        <v>100.31430544490587</v>
+      </c>
+      <c r="E17" s="23">
+        <f t="shared" si="1"/>
+        <v>208.12638304247014</v>
+      </c>
+      <c r="F17" s="23">
+        <f t="shared" si="1"/>
+        <v>349.31470044688899</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="1"/>
+        <v>521.98122966529729</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="22">
+        <v>130</v>
+      </c>
+      <c r="C18" s="23">
+        <f t="shared" si="1"/>
+        <v>36.7845769169381</v>
+      </c>
+      <c r="D18" s="23">
+        <f t="shared" si="1"/>
+        <v>128.09133662260027</v>
+      </c>
+      <c r="E18" s="23">
+        <f t="shared" si="1"/>
+        <v>265.75657850693005</v>
+      </c>
+      <c r="F18" s="23">
+        <f t="shared" si="1"/>
+        <v>446.03994100063244</v>
+      </c>
+      <c r="G18" s="23">
+        <f t="shared" si="1"/>
+        <v>666.51783215961791</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="22">
+        <v>140</v>
+      </c>
+      <c r="C19" s="23">
+        <f t="shared" si="1"/>
+        <v>46.97022626523826</v>
+      </c>
+      <c r="D19" s="23">
+        <f t="shared" si="1"/>
+        <v>163.55982773339827</v>
+      </c>
+      <c r="E19" s="23">
+        <f t="shared" si="1"/>
+        <v>339.34457509549895</v>
+      </c>
+      <c r="F19" s="23">
+        <f t="shared" si="1"/>
+        <v>569.54840066370753</v>
+      </c>
+      <c r="G19" s="23">
+        <f t="shared" si="1"/>
+        <v>851.07661988461609</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="23">
-        <v>60</v>
-      </c>
-      <c r="C11" s="24">
-        <f t="shared" si="1"/>
-        <v>6.6461104822660744</v>
-      </c>
-      <c r="D11" s="24">
-        <f t="shared" si="1"/>
-        <v>23.143100896260023</v>
-      </c>
-      <c r="E11" s="24">
-        <f t="shared" si="1"/>
-        <v>48.01598197348779</v>
-      </c>
-      <c r="F11" s="24">
-        <f t="shared" si="1"/>
-        <v>80.5889580866328</v>
-      </c>
-      <c r="G11" s="24">
-        <f t="shared" si="1"/>
-        <v>120.4241430025403</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="23">
-        <v>70</v>
-      </c>
-      <c r="C12" s="24">
-        <f t="shared" si="1"/>
-        <v>8.4864184748055482</v>
-      </c>
-      <c r="D12" s="24">
-        <f t="shared" si="1"/>
-        <v>29.551425534434419</v>
-      </c>
-      <c r="E12" s="24">
-        <f t="shared" si="1"/>
-        <v>61.311607381946537</v>
-      </c>
-      <c r="F12" s="24">
-        <f t="shared" si="1"/>
-        <v>102.9040405808214</v>
-      </c>
-      <c r="G12" s="24">
-        <f t="shared" si="1"/>
-        <v>153.76958819994368</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="23">
-        <v>80</v>
-      </c>
-      <c r="C13" s="24">
-        <f t="shared" si="1"/>
-        <v>10.8363077504792</v>
-      </c>
-      <c r="D13" s="24">
-        <f t="shared" si="1"/>
-        <v>37.7342152649193</v>
-      </c>
-      <c r="E13" s="24">
-        <f t="shared" si="1"/>
-        <v>78.288791466007524</v>
-      </c>
-      <c r="F13" s="24">
-        <f t="shared" si="1"/>
-        <v>131.39816941765079</v>
-      </c>
-      <c r="G13" s="24">
-        <f t="shared" si="1"/>
-        <v>196.34838717250804</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="23">
-        <v>90</v>
-      </c>
-      <c r="C14" s="24">
-        <f t="shared" si="1"/>
-        <v>13.836881366586889</v>
-      </c>
-      <c r="D14" s="24">
-        <f t="shared" si="1"/>
-        <v>48.182819471775439</v>
-      </c>
-      <c r="E14" s="24">
-        <f t="shared" si="1"/>
-        <v>99.966957822944977</v>
-      </c>
-      <c r="F14" s="24">
-        <f t="shared" si="1"/>
-        <v>167.78232252939827</v>
-      </c>
-      <c r="G14" s="24">
-        <f t="shared" si="1"/>
-        <v>250.71725558057545</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="23">
-        <v>100</v>
-      </c>
-      <c r="C15" s="24">
-        <f t="shared" si="1"/>
-        <v>17.668313816994797</v>
-      </c>
-      <c r="D15" s="24">
-        <f t="shared" si="1"/>
-        <v>61.524642183510053</v>
-      </c>
-      <c r="E15" s="24">
-        <f t="shared" si="1"/>
-        <v>127.64780844411843</v>
-      </c>
-      <c r="F15" s="24">
-        <f t="shared" si="1"/>
-        <v>214.24124763778863</v>
-      </c>
-      <c r="G15" s="24">
-        <f t="shared" si="1"/>
-        <v>320.14086365083676</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="23">
-        <v>110</v>
-      </c>
-      <c r="C16" s="24">
-        <f t="shared" si="1"/>
-        <v>22.560669912920648</v>
-      </c>
-      <c r="D16" s="24">
-        <f t="shared" si="1"/>
-        <v>78.560815604123974</v>
-      </c>
-      <c r="E16" s="24">
-        <f t="shared" si="1"/>
-        <v>162.99348660229478</v>
-      </c>
-      <c r="F16" s="24">
-        <f t="shared" si="1"/>
-        <v>273.56464910869221</v>
-      </c>
-      <c r="G16" s="24">
-        <f t="shared" si="1"/>
-        <v>408.78786879575335</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="23">
-        <v>120</v>
-      </c>
-      <c r="C17" s="24">
-        <f t="shared" si="1"/>
-        <v>28.807719411808367</v>
-      </c>
-      <c r="D17" s="24">
-        <f t="shared" si="1"/>
-        <v>100.31430544490587</v>
-      </c>
-      <c r="E17" s="24">
-        <f t="shared" si="1"/>
-        <v>208.12638304247014</v>
-      </c>
-      <c r="F17" s="24">
-        <f t="shared" si="1"/>
-        <v>349.31470044688899</v>
-      </c>
-      <c r="G17" s="24">
-        <f t="shared" si="1"/>
-        <v>521.98122966529729</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="23">
-        <v>130</v>
-      </c>
-      <c r="C18" s="24">
-        <f t="shared" si="1"/>
-        <v>36.7845769169381</v>
-      </c>
-      <c r="D18" s="24">
-        <f t="shared" si="1"/>
-        <v>128.09133662260027</v>
-      </c>
-      <c r="E18" s="24">
-        <f t="shared" si="1"/>
-        <v>265.75657850693005</v>
-      </c>
-      <c r="F18" s="24">
-        <f t="shared" si="1"/>
-        <v>446.03994100063244</v>
-      </c>
-      <c r="G18" s="24">
-        <f t="shared" si="1"/>
-        <v>666.51783215961791</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="23">
-        <v>140</v>
-      </c>
-      <c r="C19" s="24">
-        <f t="shared" si="1"/>
-        <v>46.97022626523826</v>
-      </c>
-      <c r="D19" s="24">
-        <f t="shared" si="1"/>
-        <v>163.55982773339827</v>
-      </c>
-      <c r="E19" s="24">
-        <f t="shared" si="1"/>
-        <v>339.34457509549895</v>
-      </c>
-      <c r="F19" s="24">
-        <f t="shared" si="1"/>
-        <v>569.54840066370753</v>
-      </c>
-      <c r="G19" s="24">
-        <f t="shared" si="1"/>
-        <v>851.07661988461609</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="12" t="s">
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
-        <v>48</v>
       </c>
       <c r="C26" s="8">
         <v>1</v>
@@ -5792,377 +6373,377 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="23">
+      <c r="B27" s="22">
         <v>0</v>
       </c>
-      <c r="C27" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+      <c r="C27" s="23">
+        <f t="shared" ref="C27:G41" si="2">POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
         <v>3.5</v>
       </c>
-      <c r="D27" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+      <c r="D27" s="23">
+        <f t="shared" si="2"/>
         <v>12.187707886145738</v>
       </c>
-      <c r="E27" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+      <c r="E27" s="23">
+        <f t="shared" si="2"/>
         <v>25.286359195447272</v>
       </c>
-      <c r="F27" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+      <c r="F27" s="23">
+        <f t="shared" si="2"/>
         <v>42.44006386229114</v>
       </c>
-      <c r="G27" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+      <c r="G27" s="23">
+        <f t="shared" si="2"/>
         <v>63.418220571798358</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="23">
+      <c r="B28" s="22">
         <v>10</v>
       </c>
-      <c r="C28" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+      <c r="C28" s="23">
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="D28" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+      <c r="D28" s="23">
+        <f t="shared" si="2"/>
         <v>12.187707886145738</v>
       </c>
-      <c r="E28" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+      <c r="E28" s="23">
+        <f t="shared" si="2"/>
         <v>25.286359195447272</v>
       </c>
-      <c r="F28" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+      <c r="F28" s="23">
+        <f t="shared" si="2"/>
         <v>42.44006386229114</v>
       </c>
-      <c r="G28" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B28-$K$8)/$K$7))) / $K$5</f>
+      <c r="G28" s="23">
+        <f t="shared" si="2"/>
         <v>63.418220571798358</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="23">
+      <c r="B29" s="22">
         <v>20</v>
       </c>
-      <c r="C29" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+      <c r="C29" s="23">
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="D29" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+      <c r="D29" s="23">
+        <f t="shared" si="2"/>
         <v>12.187707886145738</v>
       </c>
-      <c r="E29" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+      <c r="E29" s="23">
+        <f t="shared" si="2"/>
         <v>25.286359195447272</v>
       </c>
-      <c r="F29" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+      <c r="F29" s="23">
+        <f t="shared" si="2"/>
         <v>42.44006386229114</v>
       </c>
-      <c r="G29" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B29-$K$8)/$K$7))) / $K$5</f>
+      <c r="G29" s="23">
+        <f t="shared" si="2"/>
         <v>63.418220571798358</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="23">
+      <c r="B30" s="22">
         <v>30</v>
       </c>
-      <c r="C30" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+      <c r="C30" s="23">
+        <f t="shared" si="2"/>
         <v>4.4691499999999991</v>
       </c>
-      <c r="D30" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+      <c r="D30" s="23">
+        <f t="shared" si="2"/>
         <v>15.56248419981949</v>
       </c>
-      <c r="E30" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+      <c r="E30" s="23">
+        <f t="shared" si="2"/>
         <v>32.288152056666611</v>
       </c>
-      <c r="F30" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+      <c r="F30" s="23">
+        <f t="shared" si="2"/>
         <v>54.191717545759545</v>
       </c>
-      <c r="G30" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B30-$K$8)/$K$7))) / $K$5</f>
+      <c r="G30" s="23">
+        <f t="shared" si="2"/>
         <v>80.978725848129301</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="23">
+      <c r="B31" s="22">
         <v>40</v>
       </c>
-      <c r="C31" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+      <c r="C31" s="23">
+        <f t="shared" si="2"/>
         <v>5.7066576349999965</v>
       </c>
-      <c r="D31" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+      <c r="D31" s="23">
+        <f t="shared" si="2"/>
         <v>19.871736074749503</v>
       </c>
-      <c r="E31" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+      <c r="E31" s="23">
+        <f t="shared" si="2"/>
         <v>41.228741361157589</v>
       </c>
-      <c r="F31" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+      <c r="F31" s="23">
+        <f t="shared" si="2"/>
         <v>69.197404134180346</v>
       </c>
-      <c r="G31" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B31-$K$8)/$K$7))) / $K$5</f>
+      <c r="G31" s="23">
+        <f t="shared" si="2"/>
         <v>103.40173503547628</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="23">
+      <c r="B32" s="22">
         <v>50</v>
       </c>
-      <c r="C32" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+      <c r="C32" s="23">
+        <f t="shared" si="2"/>
         <v>7.2868311341314937</v>
       </c>
-      <c r="D32" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+      <c r="D32" s="23">
+        <f t="shared" si="2"/>
         <v>25.374219793847633</v>
       </c>
-      <c r="E32" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+      <c r="E32" s="23">
+        <f t="shared" si="2"/>
         <v>52.644979844062107</v>
       </c>
-      <c r="F32" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+      <c r="F32" s="23">
+        <f t="shared" si="2"/>
         <v>88.358165338934867</v>
       </c>
-      <c r="G32" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B32-$K$8)/$K$7))) / $K$5</f>
+      <c r="G32" s="23">
+        <f t="shared" si="2"/>
         <v>132.03367546679962</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="23">
+      <c r="B33" s="22">
         <v>60</v>
       </c>
-      <c r="C33" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+      <c r="C33" s="23">
+        <f t="shared" si="2"/>
         <v>9.3045546751725041</v>
       </c>
-      <c r="D33" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+      <c r="D33" s="23">
+        <f t="shared" si="2"/>
         <v>32.400341254764037</v>
       </c>
-      <c r="E33" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+      <c r="E33" s="23">
+        <f t="shared" si="2"/>
         <v>67.222374762882893</v>
       </c>
-      <c r="F33" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+      <c r="F33" s="23">
+        <f t="shared" si="2"/>
         <v>112.82454132128592</v>
       </c>
-      <c r="G33" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B33-$K$8)/$K$7))) / $K$5</f>
+      <c r="G33" s="23">
+        <f t="shared" si="2"/>
         <v>168.59380020355641</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="23">
+      <c r="B34" s="22">
         <v>70</v>
       </c>
-      <c r="C34" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+      <c r="C34" s="23">
+        <f t="shared" si="2"/>
         <v>11.880985864727768</v>
       </c>
-      <c r="D34" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+      <c r="D34" s="23">
+        <f t="shared" si="2"/>
         <v>41.371995748208192</v>
       </c>
-      <c r="E34" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+      <c r="E34" s="23">
+        <f t="shared" si="2"/>
         <v>85.83625033472515</v>
       </c>
-      <c r="F34" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+      <c r="F34" s="23">
+        <f t="shared" si="2"/>
         <v>144.06565681314996</v>
       </c>
-      <c r="G34" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B34-$K$8)/$K$7))) / $K$5</f>
+      <c r="G34" s="23">
+        <f t="shared" si="2"/>
         <v>215.27742347992114</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="23">
+      <c r="B35" s="22">
         <v>80</v>
       </c>
-      <c r="C35" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+      <c r="C35" s="23">
+        <f t="shared" si="2"/>
         <v>15.170830850670884</v>
       </c>
-      <c r="D35" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+      <c r="D35" s="23">
+        <f t="shared" si="2"/>
         <v>52.82790137088702</v>
       </c>
-      <c r="E35" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+      <c r="E35" s="23">
+        <f t="shared" si="2"/>
         <v>109.6043080524105</v>
       </c>
-      <c r="F35" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+      <c r="F35" s="23">
+        <f t="shared" si="2"/>
         <v>183.95743718471113</v>
       </c>
-      <c r="G35" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B35-$K$8)/$K$7))) / $K$5</f>
+      <c r="G35" s="23">
+        <f t="shared" si="2"/>
         <v>274.88774204151122</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="23">
+      <c r="B36" s="22">
         <v>90</v>
       </c>
-      <c r="C36" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+      <c r="C36" s="23">
+        <f t="shared" si="2"/>
         <v>19.371633913221643</v>
       </c>
-      <c r="D36" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+      <c r="D36" s="23">
+        <f t="shared" si="2"/>
         <v>67.455947260485615</v>
       </c>
-      <c r="E36" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+      <c r="E36" s="23">
+        <f t="shared" si="2"/>
         <v>139.95374095212296</v>
       </c>
-      <c r="F36" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+      <c r="F36" s="23">
+        <f t="shared" si="2"/>
         <v>234.89525154115753</v>
       </c>
-      <c r="G36" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B36-$K$8)/$K$7))) / $K$5</f>
+      <c r="G36" s="23">
+        <f t="shared" si="2"/>
         <v>351.00415781280554</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="23">
+      <c r="B37" s="22">
         <v>100</v>
       </c>
-      <c r="C37" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+      <c r="C37" s="23">
+        <f t="shared" si="2"/>
         <v>24.735639343792712</v>
       </c>
-      <c r="D37" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+      <c r="D37" s="23">
+        <f t="shared" si="2"/>
         <v>86.13449905691408</v>
       </c>
-      <c r="E37" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+      <c r="E37" s="23">
+        <f t="shared" si="2"/>
         <v>178.70693182176578</v>
       </c>
-      <c r="F37" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+      <c r="F37" s="23">
+        <f t="shared" si="2"/>
         <v>299.93774669290406</v>
       </c>
-      <c r="G37" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B37-$K$8)/$K$7))) / $K$5</f>
+      <c r="G37" s="23">
+        <f t="shared" si="2"/>
         <v>448.19720911117139</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="23">
+      <c r="B38" s="22">
         <v>110</v>
       </c>
-      <c r="C38" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+      <c r="C38" s="23">
+        <f t="shared" si="2"/>
         <v>31.584937878088908</v>
       </c>
-      <c r="D38" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+      <c r="D38" s="23">
+        <f t="shared" si="2"/>
         <v>109.98514184577355</v>
       </c>
-      <c r="E38" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+      <c r="E38" s="23">
+        <f t="shared" si="2"/>
         <v>228.19088124321266</v>
       </c>
-      <c r="F38" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+      <c r="F38" s="23">
+        <f t="shared" si="2"/>
         <v>382.99050875216915</v>
       </c>
-      <c r="G38" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B38-$K$8)/$K$7))) / $K$5</f>
+      <c r="G38" s="23">
+        <f t="shared" si="2"/>
         <v>572.30301631405462</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="23">
+      <c r="B39" s="22">
         <v>120</v>
       </c>
-      <c r="C39" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+      <c r="C39" s="23">
+        <f t="shared" si="2"/>
         <v>40.330807176531721</v>
       </c>
-      <c r="D39" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+      <c r="D39" s="23">
+        <f t="shared" si="2"/>
         <v>140.44002762286823</v>
       </c>
-      <c r="E39" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+      <c r="E39" s="23">
+        <f t="shared" si="2"/>
         <v>291.3769362594582</v>
       </c>
-      <c r="F39" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+      <c r="F39" s="23">
+        <f t="shared" si="2"/>
         <v>489.04058062564462</v>
       </c>
-      <c r="G39" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B39-$K$8)/$K$7))) / $K$5</f>
+      <c r="G39" s="23">
+        <f t="shared" si="2"/>
         <v>730.77372153141607</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="23">
+      <c r="B40" s="22">
         <v>130</v>
       </c>
-      <c r="C40" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+      <c r="C40" s="23">
+        <f t="shared" si="2"/>
         <v>51.498407683713339</v>
       </c>
-      <c r="D40" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+      <c r="D40" s="23">
+        <f t="shared" si="2"/>
         <v>179.32787127164036</v>
       </c>
-      <c r="E40" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+      <c r="E40" s="23">
+        <f t="shared" si="2"/>
         <v>372.05920990970202</v>
       </c>
-      <c r="F40" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+      <c r="F40" s="23">
+        <f t="shared" si="2"/>
         <v>624.45591740088537</v>
       </c>
-      <c r="G40" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B40-$K$8)/$K$7))) / $K$5</f>
+      <c r="G40" s="23">
+        <f t="shared" si="2"/>
         <v>933.12496502346505</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23">
+      <c r="B41" s="22">
         <v>140</v>
       </c>
-      <c r="C41" s="24">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+      <c r="C41" s="23">
+        <f t="shared" si="2"/>
         <v>65.758316771333554</v>
       </c>
-      <c r="D41" s="24">
-        <f>POWER(D$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+      <c r="D41" s="23">
+        <f t="shared" si="2"/>
         <v>228.98375882675759</v>
       </c>
-      <c r="E41" s="24">
-        <f>POWER(E$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+      <c r="E41" s="23">
+        <f t="shared" si="2"/>
         <v>475.0824051336985</v>
       </c>
-      <c r="F41" s="24">
-        <f>POWER(F$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+      <c r="F41" s="23">
+        <f t="shared" si="2"/>
         <v>797.36776092919047</v>
       </c>
-      <c r="G41" s="24">
-        <f>POWER(G$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B41-$K$8)/$K$7))) / $K$5</f>
+      <c r="G41" s="23">
+        <f t="shared" si="2"/>
         <v>1191.5072678384624</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More complex artifact missions; Lower level xp; Adding new armour types
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>Width</t>
   </si>
@@ -212,6 +212,12 @@
   <si>
     <t>int nCreatures = (int)(Math.Pow(nFloorTiles, Const.CreatureCountExponent) * ((double)soldierCount + 1d) * cg.QuantityScale * Const.CreatureFrequencyScale);</t>
   </si>
+  <si>
+    <t>Exp (Raw)</t>
+  </si>
+  <si>
+    <t>Exp (Tidy)</t>
+  </si>
 </sst>
 </file>
 
@@ -267,7 +273,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +283,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -422,6 +434,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -833,11 +851,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="647433336"/>
-        <c:axId val="647434512"/>
+        <c:axId val="641692432"/>
+        <c:axId val="641692824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="647433336"/>
+        <c:axId val="641692432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,12 +912,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="647434512"/>
+        <c:crossAx val="641692824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="647434512"/>
+        <c:axId val="641692824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +974,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="647433336"/>
+        <c:crossAx val="641692432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1861,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,18 +1972,18 @@
         <v>0.8</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" ref="F6:G21" si="1">$D6*$E6</f>
+        <f t="shared" ref="F6:F21" si="1">$D6*$E6</f>
         <v>320</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" ref="G6:H21" si="2">POWER($F6,$M$4)</f>
+        <f t="shared" ref="G6:G21" si="2">POWER($F6,$M$4)</f>
         <v>142.7016456115976</v>
       </c>
       <c r="H6" s="7">
         <v>2</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:J21" si="3">INT($G6*($H6+1)*$M$5)</f>
+        <f t="shared" ref="I6:I21" si="3">INT($G6*($H6+1)*$M$5)</f>
         <v>4</v>
       </c>
     </row>
@@ -2437,11 +2455,11 @@
         <v>0.6</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" ref="F22:G34" si="4">$D22*$E22</f>
+        <f t="shared" ref="F22:F34" si="4">$D22*$E22</f>
         <v>240</v>
       </c>
       <c r="G22" s="6">
-        <f t="shared" ref="G22:H34" si="5">POWER($F22,$M$4)</f>
+        <f t="shared" ref="G22:G34" si="5">POWER($F22,$M$4)</f>
         <v>111.42474987806408</v>
       </c>
       <c r="H22" s="7">
@@ -2822,16 +2840,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="6"/>
-    <col min="6" max="6" width="19.140625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="18"/>
   </cols>
   <sheetData>
@@ -2839,15 +2857,17 @@
       <c r="B2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="18">
-        <v>1.7</v>
+      <c r="G2" s="29">
+        <v>1.65</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -2860,10 +2880,10 @@
       <c r="D3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="29">
         <v>4</v>
       </c>
     </row>
@@ -2879,10 +2899,10 @@
         <f t="shared" ref="D4:D22" si="1">ROUND($C4,2-(1+INT(LOG10($C4))))</f>
         <v>1000</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="29">
         <v>1000</v>
       </c>
     </row>
@@ -2892,11 +2912,11 @@
       </c>
       <c r="C5" s="4">
         <f t="shared" si="0"/>
-        <v>3800</v>
+        <v>3600</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="1"/>
-        <v>3800</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -2905,11 +2925,11 @@
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>8560</v>
+        <v>7890</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="1"/>
-        <v>8600</v>
+        <v>7900</v>
       </c>
       <c r="J6" s="20"/>
     </row>
@@ -2919,11 +2939,11 @@
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>16652</v>
+        <v>14968</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="1"/>
-        <v>17000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -2932,11 +2952,11 @@
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>30408</v>
+        <v>26648</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>27000</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -2945,11 +2965,11 @@
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>53794</v>
+        <v>45919</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>54000</v>
+        <v>46000</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -2958,11 +2978,11 @@
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>93550</v>
+        <v>77716</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="1"/>
-        <v>94000</v>
+        <v>78000</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -2971,11 +2991,11 @@
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>161135</v>
+        <v>130182</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>160000</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -2984,11 +3004,11 @@
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>276030</v>
+        <v>216751</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="1"/>
-        <v>280000</v>
+        <v>220000</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -2997,11 +3017,11 @@
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>471351</v>
+        <v>359589</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>470000</v>
+        <v>360000</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -3010,11 +3030,11 @@
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>803397</v>
+        <v>595273</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="1"/>
-        <v>800000</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -3023,11 +3043,11 @@
       </c>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
-        <v>1367875</v>
+        <v>984150</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="1"/>
-        <v>1400000</v>
+        <v>980000</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -3036,11 +3056,11 @@
       </c>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
-        <v>2327488</v>
+        <v>1625798</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="1"/>
-        <v>2300000</v>
+        <v>1600000</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -3049,11 +3069,11 @@
       </c>
       <c r="C17" s="4">
         <f t="shared" si="0"/>
-        <v>3958831</v>
+        <v>2684517</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="1"/>
-        <v>4000000</v>
+        <v>2700000</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -3062,11 +3082,11 @@
       </c>
       <c r="C18" s="4">
         <f t="shared" si="0"/>
-        <v>6732113</v>
+        <v>4431403</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="1"/>
-        <v>6700000</v>
+        <v>4400000</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -3075,11 +3095,11 @@
       </c>
       <c r="C19" s="4">
         <f t="shared" si="0"/>
-        <v>11446692</v>
+        <v>7313765</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="1"/>
-        <v>11000000</v>
+        <v>7300000</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -3088,11 +3108,11 @@
       </c>
       <c r="C20" s="4">
         <f t="shared" si="0"/>
-        <v>19461476</v>
+        <v>12069663</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="1"/>
-        <v>19000000</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -3101,11 +3121,11 @@
       </c>
       <c r="C21" s="4">
         <f t="shared" si="0"/>
-        <v>33086610</v>
+        <v>19916894</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="1"/>
-        <v>33000000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -3114,11 +3134,11 @@
       </c>
       <c r="C22" s="4">
         <f t="shared" si="0"/>
-        <v>56249337</v>
+        <v>32864826</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="1"/>
-        <v>56000000</v>
+        <v>33000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing bug with gates; making searching better; Simpler heal skill;
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -474,6 +474,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -851,11 +852,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="641692432"/>
-        <c:axId val="641692824"/>
+        <c:axId val="652529416"/>
+        <c:axId val="652530592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="641692432"/>
+        <c:axId val="652529416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,12 +913,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="641692824"/>
+        <c:crossAx val="652530592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="641692824"/>
+        <c:axId val="652530592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,7 +975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="641692432"/>
+        <c:crossAx val="652529416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2840,8 +2841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3324,10 +3325,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y33" sqref="Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3430,6 +3431,10 @@
         <f t="shared" si="0"/>
         <v>11.23</v>
       </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Swarm missions, data tweaks
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -852,11 +851,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="652529416"/>
-        <c:axId val="652530592"/>
+        <c:axId val="639252400"/>
+        <c:axId val="639253968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="652529416"/>
+        <c:axId val="639252400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,12 +912,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652530592"/>
+        <c:crossAx val="639253968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="652530592"/>
+        <c:axId val="639253968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,7 +974,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652529416"/>
+        <c:crossAx val="639252400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2841,8 +2840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,7 +2867,7 @@
         <v>38</v>
       </c>
       <c r="G2" s="29">
-        <v>1.65</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -2913,11 +2912,11 @@
       </c>
       <c r="C5" s="4">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>3480</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="1"/>
-        <v>3600</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -2926,11 +2925,11 @@
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>7890</v>
+        <v>7497</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="1"/>
-        <v>7900</v>
+        <v>7500</v>
       </c>
       <c r="J6" s="20"/>
     </row>
@@ -2940,11 +2939,11 @@
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>14968</v>
+        <v>14006</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -2953,11 +2952,11 @@
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>26648</v>
+        <v>24549</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>27000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -2966,11 +2965,11 @@
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>45919</v>
+        <v>41630</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>46000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -2979,11 +2978,11 @@
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>77716</v>
+        <v>69301</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="1"/>
-        <v>78000</v>
+        <v>69000</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -2992,11 +2991,11 @@
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>130182</v>
+        <v>114129</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>130000</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -3005,11 +3004,11 @@
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>216751</v>
+        <v>186749</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="1"/>
-        <v>220000</v>
+        <v>190000</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -3018,11 +3017,11 @@
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>359589</v>
+        <v>304393</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>360000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -3031,11 +3030,11 @@
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>595273</v>
+        <v>494977</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="1"/>
-        <v>600000</v>
+        <v>490000</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -3044,11 +3043,11 @@
       </c>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
-        <v>984150</v>
+        <v>803724</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="1"/>
-        <v>980000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -3057,11 +3056,11 @@
       </c>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
-        <v>1625798</v>
+        <v>1303893</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="1"/>
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -3070,11 +3069,11 @@
       </c>
       <c r="C17" s="4">
         <f t="shared" si="0"/>
-        <v>2684517</v>
+        <v>2114167</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="1"/>
-        <v>2700000</v>
+        <v>2100000</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -3083,11 +3082,11 @@
       </c>
       <c r="C18" s="4">
         <f t="shared" si="0"/>
-        <v>4431403</v>
+        <v>3426811</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="1"/>
-        <v>4400000</v>
+        <v>3400000</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -3096,11 +3095,11 @@
       </c>
       <c r="C19" s="4">
         <f t="shared" si="0"/>
-        <v>7313765</v>
+        <v>5553293</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="1"/>
-        <v>7300000</v>
+        <v>5600000</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -3109,11 +3108,11 @@
       </c>
       <c r="C20" s="4">
         <f t="shared" si="0"/>
-        <v>12069663</v>
+        <v>8998196</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="1"/>
-        <v>12000000</v>
+        <v>9000000</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -3122,11 +3121,11 @@
       </c>
       <c r="C21" s="4">
         <f t="shared" si="0"/>
-        <v>19916894</v>
+        <v>14578937</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="1"/>
-        <v>20000000</v>
+        <v>15000000</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -3135,11 +3134,11 @@
       </c>
       <c r="C22" s="4">
         <f t="shared" si="0"/>
-        <v>32864826</v>
+        <v>23619739</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="1"/>
-        <v>33000000</v>
+        <v>24000000</v>
       </c>
     </row>
   </sheetData>
@@ -3327,8 +3326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y33" sqref="Y33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Armour cost entirely from first principles. Most stuff using encumbrance not baked-in agility penalties; Material penalties; Tidying up skills
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
     <sheet name="Levels and Experience" sheetId="2" r:id="rId2"/>
     <sheet name="Map Size" sheetId="3" r:id="rId3"/>
     <sheet name="Item Levels" sheetId="4" r:id="rId4"/>
-    <sheet name="Mercenary Cost" sheetId="5" r:id="rId5"/>
-    <sheet name="Relations Levels" sheetId="6" r:id="rId6"/>
-    <sheet name="Difficulty Scaling" sheetId="7" r:id="rId7"/>
-    <sheet name="Colony Growth" sheetId="8" r:id="rId8"/>
+    <sheet name="Encumbrance" sheetId="9" r:id="rId5"/>
+    <sheet name="Mercenary Cost" sheetId="5" r:id="rId6"/>
+    <sheet name="Relations Levels" sheetId="6" r:id="rId7"/>
+    <sheet name="Difficulty Scaling" sheetId="7" r:id="rId8"/>
+    <sheet name="Colony Growth" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>Width</t>
   </si>
@@ -218,6 +219,12 @@
   <si>
     <t>Exp (Tidy)</t>
   </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>MaxCarry</t>
+  </si>
 </sst>
 </file>
 
@@ -393,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -442,6 +449,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,11 +859,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="639252400"/>
-        <c:axId val="639253968"/>
+        <c:axId val="617018832"/>
+        <c:axId val="617008640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="639252400"/>
+        <c:axId val="617018832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,12 +920,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="639253968"/>
+        <c:crossAx val="617008640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="639253968"/>
+        <c:axId val="617008640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,7 +982,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="639252400"/>
+        <c:crossAx val="617018832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2840,7 +2848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -3443,10 +3451,280 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <f>POWER(B3,$F$3)*$F$4+$F$5</f>
+        <v>6.9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:C28" si="0">POWER(B4,$F$3)*$F$4+$F$5</f>
+        <v>8.5455844122715714</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>10.676537180435968</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>16.062305898749052</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>19.227244611029164</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>22.668233259706916</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>26.364675298172557</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>34.460498941515425</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>38.834585424518465</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>43.412297443487766</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>48.184949922928681</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>53.144883073351636</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>58.285275173800116</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>63.59999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>17</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>69.083516071950243</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
+        <v>74.730779131332369</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
+        <v>80.537171934545498</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>20</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
+        <v>86.498447189992433</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
+        <v>98.870232044503936</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>24</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" si="0"/>
+        <v>111.81795688823334</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>26</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
+        <v>125.31705661807122</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <v>28</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="0"/>
+        <v>139.3458660776553</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>30</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" si="0"/>
+        <v>153.88509052639483</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B2" sqref="B2:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3663,7 +3941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
@@ -5022,7 +5300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J48"/>
   <sheetViews>
@@ -5868,7 +6146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R41"/>
   <sheetViews>

</xml_diff>

<commit_message>
Bugfix for colonyview; Armour reduction changes; More accurate sector visibility; Hivebeasts; Xenomorphs adn Demons not selectable; PrimaryCreature bugfix;
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -15,10 +15,10 @@
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
     <sheet name="Levels and Experience" sheetId="2" r:id="rId2"/>
     <sheet name="Map Size" sheetId="3" r:id="rId3"/>
-    <sheet name="Item Levels" sheetId="4" r:id="rId4"/>
-    <sheet name="Encumbrance" sheetId="9" r:id="rId5"/>
-    <sheet name="Mercenary Cost" sheetId="5" r:id="rId6"/>
-    <sheet name="Relations Levels" sheetId="6" r:id="rId7"/>
+    <sheet name="Encumbrance" sheetId="9" r:id="rId4"/>
+    <sheet name="Armour Reduction" sheetId="10" r:id="rId5"/>
+    <sheet name="Relations Levels" sheetId="6" r:id="rId6"/>
+    <sheet name="Mercenary Cost" sheetId="5" r:id="rId7"/>
     <sheet name="Difficulty Scaling" sheetId="7" r:id="rId8"/>
     <sheet name="Colony Growth" sheetId="8" r:id="rId9"/>
   </sheets>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>Width</t>
   </si>
@@ -85,30 +85,6 @@
     <t>RandBase</t>
   </si>
   <si>
-    <t>Cost Modifier</t>
-  </si>
-  <si>
-    <t>Desc</t>
-  </si>
-  <si>
-    <t>Basic</t>
-  </si>
-  <si>
-    <t>Fine</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>Superb</t>
-  </si>
-  <si>
-    <t>Epic</t>
-  </si>
-  <si>
-    <t>Legendary</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
@@ -140,9 +116,6 @@
   </si>
   <si>
     <t>Outer bit</t>
-  </si>
-  <si>
-    <t>Util</t>
   </si>
   <si>
     <t>SoldierLevelExperience</t>
@@ -225,6 +198,30 @@
   <si>
     <t>MaxCarry</t>
   </si>
+  <si>
+    <t>Exp Scale</t>
+  </si>
+  <si>
+    <t>Armour</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>New Dmg</t>
+  </si>
+  <si>
+    <t>Exp2</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
 </sst>
 </file>
 
@@ -300,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -396,11 +393,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -415,9 +423,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -450,6 +455,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +502,626 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Armour Reduction'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Damage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Armour Reduction'!$B$3:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Armour Reduction'!$C$3:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.715996843424591</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.484160391041655</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.172248855821678</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87.055056329612412</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83.123789614278778</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.370052598409984</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.710678118654755</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62.996052494743658</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56.123102415468651</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44.544935907016963</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39.685026299204992</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35.355339059327378</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31.498026247371829</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.842513149602492</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.749013123685918</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.921256574801248</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.9372532809214773</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.480314143700312</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.5625</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.98431332023036966</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Armour Reduction'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>New Dmg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Armour Reduction'!$B$3:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Armour Reduction'!$D$3:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.064458573273242</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.591812522665393</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.144892671268622</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86.118675990610768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.3980943939046</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78.925220537571477</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71.113160110456874</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.29806574927926</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>58.282485186967683</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.933290315596146</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.151978235305769</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43.861617315434934</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36.51560942092317</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30.511241564292174</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25.570371161108223</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.48356373280761</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.089130275866257</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.260055429207236</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.913602200790223</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.8487089083892334</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.6710872889019068</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.1142663640113337</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.9954483247075605</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="41037864"/>
+        <c:axId val="41039432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="41037864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="41039432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="41039432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="41037864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -859,11 +1499,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="617018832"/>
-        <c:axId val="617008640"/>
+        <c:axId val="584757960"/>
+        <c:axId val="584765016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="617018832"/>
+        <c:axId val="584757960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,12 +1560,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617008640"/>
+        <c:crossAx val="584765016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="617008640"/>
+        <c:axId val="584765016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -982,7 +1622,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617018832"/>
+        <c:crossAx val="584757960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1032,6 +1672,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1587,7 +2267,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1908,10 +3139,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>3</v>
@@ -1922,10 +3153,10 @@
       <c r="I4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="27">
+      <c r="M4" s="26">
         <v>0.86</v>
       </c>
     </row>
@@ -1958,10 +3189,10 @@
         <f>INT($G5*($H5+1)*$M$5)</f>
         <v>2</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="27">
+      <c r="L5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="26">
         <v>0.01</v>
       </c>
     </row>
@@ -2174,8 +3405,8 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="L12" s="26" t="s">
-        <v>59</v>
+      <c r="L12" s="25" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -2857,24 +4088,24 @@
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="6"/>
-    <col min="6" max="6" width="22.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="18"/>
+    <col min="6" max="6" width="22.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="29">
+        <v>52</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="28">
         <v>1.62</v>
       </c>
     </row>
@@ -2888,10 +4119,10 @@
       <c r="D3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="29">
+      <c r="F3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="28">
         <v>4</v>
       </c>
     </row>
@@ -2907,10 +4138,10 @@
         <f t="shared" ref="D4:D22" si="1">ROUND($C4,2-(1+INT(LOG10($C4))))</f>
         <v>1000</v>
       </c>
-      <c r="F4" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="29">
+      <c r="F4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="28">
         <v>1000</v>
       </c>
     </row>
@@ -2939,7 +4170,7 @@
         <f t="shared" si="1"/>
         <v>7500</v>
       </c>
-      <c r="J6" s="20"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -3332,128 +4563,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H14"/>
+  <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="13">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="13">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="13">
-        <f>ROUND(POWER(B3+1,$H$2) * POWER($H$3,B3),2)</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="13">
-        <f t="shared" ref="D4:D8" si="0">ROUND(POWER(B4+1,$H$2) * POWER($H$3,B4),2)</f>
-        <v>2.5499999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="13">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="13">
-        <f t="shared" si="0"/>
-        <v>4.41</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="13">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="13">
-        <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="13">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="13">
-        <f t="shared" si="0"/>
-        <v>8.7799999999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="13">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="13">
-        <f t="shared" si="0"/>
-        <v>11.23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -3461,10 +4573,10 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -3487,7 +4599,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4">
-        <f t="shared" ref="C4:C28" si="0">POWER(B4,$F$3)*$F$4+$F$5</f>
+        <f t="shared" ref="C4:C27" si="0">POWER(B4,$F$3)*$F$4+$F$5</f>
         <v>8.5455844122715714</v>
       </c>
       <c r="E4" t="s">
@@ -3712,236 +4824,407 @@
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
-      <c r="C28" s="30"/>
+      <c r="C28" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F22"/>
+  <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="32">
+        <f>100*POWER($G$3,B3/$G$4)</f>
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <f>100*POWER($H$3,POWER(B3/$H$4,$H$5))</f>
+        <v>100</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
-        <f t="shared" ref="C3:C22" si="0">$B3*POWER($F$4,$F$5*$B3)*$F$3</f>
-        <v>17.141191951192397</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+      <c r="C4" s="32">
+        <f>100*POWER($G$3,B4/$G$4)</f>
+        <v>97.715996843424591</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D27" si="0">100*POWER($H$3,POWER(B4/$H$4,$H$5))</f>
+        <v>97.064458573273242</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="15">
+        <v>30</v>
+      </c>
+      <c r="H4" s="15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="4">
-        <f t="shared" si="0"/>
-        <v>39.176061534349742</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4">
-        <f t="shared" si="0"/>
-        <v>67.152439065201392</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="32">
+        <f>100*POWER($G$3,B5/$G$4)</f>
+        <v>95.484160391041655</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>94.591812522665393</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" si="0"/>
-        <v>102.31758648954383</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="32">
+        <f>100*POWER($G$3,B6/$G$4)</f>
+        <v>91.172248855821678</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>90.144892671268622</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4">
-        <f t="shared" si="0"/>
-        <v>146.15378250000009</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C7" s="32">
+        <f>100*POWER($G$3,B7/$G$4)</f>
+        <v>87.055056329612412</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>86.118675990610768</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="0"/>
-        <v>200.42000321802604</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C8" s="32">
+        <f>100*POWER($G$3,B8/$G$4)</f>
+        <v>83.123789614278778</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>82.3980943939046</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="0"/>
-        <v>267.20071357923865</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C9" s="32">
+        <f>100*POWER($G$3,B9/$G$4)</f>
+        <v>79.370052598409984</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>78.925220537571477</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="0"/>
-        <v>348.96295016817601</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C10" s="32">
+        <f>100*POWER($G$3,B10/$G$4)</f>
+        <v>70.710678118654755</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>71.113160110456874</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="0"/>
-        <v>448.62306845153205</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C11" s="32">
+        <f>100*POWER($G$3,B11/$G$4)</f>
+        <v>62.996052494743658</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>64.29806574927926</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4">
-        <f t="shared" si="0"/>
-        <v>569.62475037486206</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C12" s="32">
+        <f>100*POWER($G$3,B12/$G$4)</f>
+        <v>56.123102415468651</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>58.282485186967683</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
-        <v>11</v>
-      </c>
-      <c r="C13" s="4">
-        <f t="shared" si="0"/>
-        <v>716.03012699720796</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C13" s="32">
+        <f>100*POWER($G$3,B13/$G$4)</f>
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>52.933290315596146</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
-        <v>12</v>
-      </c>
-      <c r="C14" s="4">
-        <f t="shared" si="0"/>
-        <v>892.62617088696811</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C14" s="32">
+        <f>100*POWER($G$3,B14/$G$4)</f>
+        <v>44.544935907016963</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>48.151978235305769</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4">
-        <f t="shared" si="0"/>
-        <v>1105.0488609211561</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C15" s="32">
+        <f>100*POWER($G$3,B15/$G$4)</f>
+        <v>39.685026299204992</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>43.861617315434934</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4">
-        <f t="shared" si="0"/>
-        <v>1359.9280254715111</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C16" s="32">
+        <f>100*POWER($G$3,B16/$G$4)</f>
+        <v>35.355339059327378</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
-        <v>15</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" si="0"/>
-        <v>1665.0562374580884</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="C17" s="32">
+        <f>100*POWER($G$3,B17/$G$4)</f>
+        <v>31.498026247371829</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>36.51560942092317</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
-        <v>16</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="0"/>
-        <v>2029.5856765012818</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C18" s="32">
+        <f>100*POWER($G$3,B18/$G$4)</f>
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>30.511241564292174</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
-        <v>17</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="0"/>
-        <v>2464.2575010795235</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C19" s="32">
+        <f>100*POWER($G$3,B19/$G$4)</f>
+        <v>19.842513149602492</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>25.570371161108223</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
-        <v>18</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="0"/>
-        <v>2981.6690006943409</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C20" s="32">
+        <f>100*POWER($G$3,B20/$G$4)</f>
+        <v>15.749013123685918</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>21.48356373280761</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
-        <v>19</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="0"/>
-        <v>3596.5846401504168</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="C21" s="32">
+        <f>100*POWER($G$3,B21/$G$4)</f>
+        <v>12.5</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>18.089130275866257</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
-        <v>20</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="0"/>
-        <v>4326.2980831949862</v>
+        <v>100</v>
+      </c>
+      <c r="C22" s="32">
+        <f>100*POWER($G$3,B22/$G$4)</f>
+        <v>9.921256574801248</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>15.260055429207236</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>120</v>
+      </c>
+      <c r="C23" s="32">
+        <f>100*POWER($G$3,B23/$G$4)</f>
+        <v>6.25</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>10.913602200790223</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>140</v>
+      </c>
+      <c r="C24" s="32">
+        <f>100*POWER($G$3,B24/$G$4)</f>
+        <v>3.9372532809214773</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>7.8487089083892334</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>160</v>
+      </c>
+      <c r="C25" s="32">
+        <f>100*POWER($G$3,B25/$G$4)</f>
+        <v>2.480314143700312</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>5.6710872889019068</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <v>180</v>
+      </c>
+      <c r="C26" s="32">
+        <f>100*POWER($G$3,B26/$G$4)</f>
+        <v>1.5625</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>4.1142663640113337</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>200</v>
+      </c>
+      <c r="C27" s="32">
+        <f>100*POWER($G$3,B27/$G$4)</f>
+        <v>0.98431332023036966</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>2.9954483247075605</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
@@ -3957,15 +5240,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5292,6 +6572,228 @@
       <c r="E50">
         <f t="shared" si="2"/>
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C22" si="0">$B3*POWER($F$4,$F$5*$B3)*$F$3</f>
+        <v>17.141191951192397</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>39.176061534349742</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>67.152439065201392</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>102.31758648954383</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>146.15378250000009</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>200.42000321802604</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>267.20071357923865</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>348.96295016817601</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>448.62306845153205</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>569.62475037486206</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>716.03012699720796</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>892.62617088696811</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>1105.0488609211561</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>1359.9280254715111</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>1665.0562374580884</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>2029.5856765012818</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>17</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>2464.2575010795235</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
+        <v>2981.6690006943409</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
+        <v>3596.5846401504168</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>20</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
+        <v>4326.2980831949862</v>
       </c>
     </row>
   </sheetData>
@@ -5312,22 +6814,22 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -5346,13 +6848,13 @@
         <f>1+ROUND(B3+C3,0)</f>
         <v>1</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="15">
         <v>1</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="15">
         <v>2.8</v>
       </c>
     </row>
@@ -5372,13 +6874,13 @@
         <f t="shared" ref="D4:D48" si="2">1+ROUND(B4+C4,0)</f>
         <v>2</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="16">
+      <c r="H4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="15">
         <v>1</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="15">
         <v>0.75</v>
       </c>
     </row>
@@ -5417,10 +6919,10 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="16">
+      <c r="H6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="15">
         <v>5</v>
       </c>
       <c r="J6" s="13"/>
@@ -6157,24 +7659,24 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
-        <v>54</v>
+      <c r="B2" s="23" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="K3">
         <v>1.8</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>47</v>
+      <c r="B4" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
@@ -6191,472 +7693,472 @@
       <c r="G4" s="8">
         <v>5</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>48</v>
+      <c r="J4" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="K4">
         <v>2.5</v>
       </c>
-      <c r="N4" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
+      <c r="N4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+      <c r="B5" s="21">
         <v>0</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <f>POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
         <v>2.5</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <f t="shared" ref="D5:G5" si="0">POWER(D$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
         <v>8.7055056329612412</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <f t="shared" si="0"/>
         <v>18.061685139605196</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <f t="shared" si="0"/>
         <v>30.31433133020796</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="22">
         <f t="shared" si="0"/>
         <v>45.298728979855973</v>
       </c>
-      <c r="J5" s="21" t="s">
-        <v>50</v>
+      <c r="J5" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="K5">
         <v>365</v>
       </c>
-      <c r="N5" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
+      <c r="N5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <v>10</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="22">
         <f t="shared" ref="C6:G19" si="1">POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B6-$K$8)/$K$7))) / $K$5</f>
         <v>2.5</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="22">
         <f t="shared" si="1"/>
         <v>8.7055056329612412</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <f t="shared" si="1"/>
         <v>18.061685139605196</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="22">
         <f t="shared" si="1"/>
         <v>30.31433133020796</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="22">
         <f t="shared" si="1"/>
         <v>45.298728979855973</v>
       </c>
-      <c r="J6" s="21" t="s">
-        <v>52</v>
+      <c r="J6" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="K6">
         <v>1.1299999999999999</v>
       </c>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="21">
         <v>20</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="22">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <f t="shared" si="1"/>
         <v>8.7055056329612412</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <f t="shared" si="1"/>
         <v>18.061685139605196</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="22">
         <f t="shared" si="1"/>
         <v>30.31433133020796</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="22">
         <f t="shared" si="1"/>
         <v>45.298728979855973</v>
       </c>
-      <c r="J7" s="21" t="s">
-        <v>51</v>
+      <c r="J7" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="K7">
         <v>5</v>
       </c>
-      <c r="N7" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
+      <c r="N7" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="22">
+      <c r="B8" s="21">
         <v>30</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="22">
         <f t="shared" si="1"/>
         <v>3.1922499999999991</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <f t="shared" si="1"/>
         <v>11.116060142728207</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <f t="shared" si="1"/>
         <v>23.062965754761869</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <f t="shared" si="1"/>
         <v>38.708369675542535</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="22">
         <f t="shared" si="1"/>
         <v>57.841947034378073</v>
       </c>
-      <c r="J8" s="21" t="s">
-        <v>53</v>
+      <c r="J8" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="K8">
         <v>20</v>
       </c>
-      <c r="N8" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
+      <c r="N8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+      <c r="B9" s="21">
         <v>40</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="22">
         <f t="shared" si="1"/>
         <v>4.0761840249999981</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="22">
         <f t="shared" si="1"/>
         <v>14.194097196249643</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="22">
         <f t="shared" si="1"/>
         <v>29.449100972255422</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="22">
         <f t="shared" si="1"/>
         <v>49.426717238700256</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="22">
         <f t="shared" si="1"/>
         <v>73.858382168197352</v>
       </c>
-      <c r="N9" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
+      <c r="N9" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
+      <c r="B10" s="21">
         <v>50</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="22">
         <f t="shared" si="1"/>
         <v>5.2048793815224963</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <f t="shared" si="1"/>
         <v>18.124442709891163</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <f t="shared" si="1"/>
         <v>37.603557031472938</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="22">
         <f t="shared" si="1"/>
         <v>63.112975242096333</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="22">
         <f t="shared" si="1"/>
         <v>94.309768190571162</v>
       </c>
-      <c r="N10" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
+      <c r="N10" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
+      <c r="B11" s="21">
         <v>60</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="22">
         <f t="shared" si="1"/>
         <v>6.6461104822660744</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="22">
         <f t="shared" si="1"/>
         <v>23.143100896260023</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="22">
         <f t="shared" si="1"/>
         <v>48.01598197348779</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="22">
         <f t="shared" si="1"/>
         <v>80.5889580866328</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="22">
         <f t="shared" si="1"/>
         <v>120.4241430025403</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="22">
+      <c r="B12" s="21">
         <v>70</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="22">
         <f t="shared" si="1"/>
         <v>8.4864184748055482</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <f t="shared" si="1"/>
         <v>29.551425534434419</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="22">
         <f t="shared" si="1"/>
         <v>61.311607381946537</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="22">
         <f t="shared" si="1"/>
         <v>102.9040405808214</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="22">
         <f t="shared" si="1"/>
         <v>153.76958819994368</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
+      <c r="B13" s="21">
         <v>80</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="22">
         <f t="shared" si="1"/>
         <v>10.8363077504792</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <f t="shared" si="1"/>
         <v>37.7342152649193</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <f t="shared" si="1"/>
         <v>78.288791466007524</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="22">
         <f t="shared" si="1"/>
         <v>131.39816941765079</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="22">
         <f t="shared" si="1"/>
         <v>196.34838717250804</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="22">
+      <c r="B14" s="21">
         <v>90</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="22">
         <f t="shared" si="1"/>
         <v>13.836881366586889</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="22">
         <f t="shared" si="1"/>
         <v>48.182819471775439</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <f t="shared" si="1"/>
         <v>99.966957822944977</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="22">
         <f t="shared" si="1"/>
         <v>167.78232252939827</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="22">
         <f t="shared" si="1"/>
         <v>250.71725558057545</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="22">
+      <c r="B15" s="21">
         <v>100</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="22">
         <f t="shared" si="1"/>
         <v>17.668313816994797</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="22">
         <f t="shared" si="1"/>
         <v>61.524642183510053</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="22">
         <f t="shared" si="1"/>
         <v>127.64780844411843</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="22">
         <f t="shared" si="1"/>
         <v>214.24124763778863</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="22">
         <f t="shared" si="1"/>
         <v>320.14086365083676</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="22">
+      <c r="B16" s="21">
         <v>110</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="22">
         <f t="shared" si="1"/>
         <v>22.560669912920648</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <f t="shared" si="1"/>
         <v>78.560815604123974</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <f t="shared" si="1"/>
         <v>162.99348660229478</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="22">
         <f t="shared" si="1"/>
         <v>273.56464910869221</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="22">
         <f t="shared" si="1"/>
         <v>408.78786879575335</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="22">
+      <c r="B17" s="21">
         <v>120</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="22">
         <f t="shared" si="1"/>
         <v>28.807719411808367</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="22">
         <f t="shared" si="1"/>
         <v>100.31430544490587</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="22">
         <f t="shared" si="1"/>
         <v>208.12638304247014</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="22">
         <f t="shared" si="1"/>
         <v>349.31470044688899</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="22">
         <f t="shared" si="1"/>
         <v>521.98122966529729</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="22">
+      <c r="B18" s="21">
         <v>130</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="22">
         <f t="shared" si="1"/>
         <v>36.7845769169381</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <f t="shared" si="1"/>
         <v>128.09133662260027</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <f t="shared" si="1"/>
         <v>265.75657850693005</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="22">
         <f t="shared" si="1"/>
         <v>446.03994100063244</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="22">
         <f t="shared" si="1"/>
         <v>666.51783215961791</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="22">
+      <c r="B19" s="21">
         <v>140</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="22">
         <f t="shared" si="1"/>
         <v>46.97022626523826</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="22">
         <f t="shared" si="1"/>
         <v>163.55982773339827</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="22">
         <f t="shared" si="1"/>
         <v>339.34457509549895</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="22">
         <f t="shared" si="1"/>
         <v>569.54840066370753</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="22">
         <f t="shared" si="1"/>
         <v>851.07661988461609</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
-        <v>55</v>
+      <c r="B24" s="23" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E25" s="11" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="19" t="s">
-        <v>47</v>
+      <c r="B26" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="C26" s="8">
         <v>1</v>
@@ -6675,376 +8177,376 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="22">
+      <c r="B27" s="21">
         <v>0</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="22">
         <f t="shared" ref="C27:G41" si="2">POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
         <v>3.5</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="22">
         <f t="shared" si="2"/>
         <v>12.187707886145738</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="22">
         <f t="shared" si="2"/>
         <v>25.286359195447272</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="22">
         <f t="shared" si="2"/>
         <v>42.44006386229114</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27" s="22">
         <f t="shared" si="2"/>
         <v>63.418220571798358</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="22">
+      <c r="B28" s="21">
         <v>10</v>
       </c>
-      <c r="C28" s="23">
+      <c r="C28" s="22">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="22">
         <f t="shared" si="2"/>
         <v>12.187707886145738</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="22">
         <f t="shared" si="2"/>
         <v>25.286359195447272</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="22">
         <f t="shared" si="2"/>
         <v>42.44006386229114</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="22">
         <f t="shared" si="2"/>
         <v>63.418220571798358</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="22">
+      <c r="B29" s="21">
         <v>20</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="22">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="22">
         <f t="shared" si="2"/>
         <v>12.187707886145738</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="22">
         <f t="shared" si="2"/>
         <v>25.286359195447272</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="22">
         <f t="shared" si="2"/>
         <v>42.44006386229114</v>
       </c>
-      <c r="G29" s="23">
+      <c r="G29" s="22">
         <f t="shared" si="2"/>
         <v>63.418220571798358</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="22">
+      <c r="B30" s="21">
         <v>30</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="22">
         <f t="shared" si="2"/>
         <v>4.4691499999999991</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="22">
         <f t="shared" si="2"/>
         <v>15.56248419981949</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="22">
         <f t="shared" si="2"/>
         <v>32.288152056666611</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="22">
         <f t="shared" si="2"/>
         <v>54.191717545759545</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="22">
         <f t="shared" si="2"/>
         <v>80.978725848129301</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="22">
+      <c r="B31" s="21">
         <v>40</v>
       </c>
-      <c r="C31" s="23">
+      <c r="C31" s="22">
         <f t="shared" si="2"/>
         <v>5.7066576349999965</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="22">
         <f t="shared" si="2"/>
         <v>19.871736074749503</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="22">
         <f t="shared" si="2"/>
         <v>41.228741361157589</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="22">
         <f t="shared" si="2"/>
         <v>69.197404134180346</v>
       </c>
-      <c r="G31" s="23">
+      <c r="G31" s="22">
         <f t="shared" si="2"/>
         <v>103.40173503547628</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="22">
+      <c r="B32" s="21">
         <v>50</v>
       </c>
-      <c r="C32" s="23">
+      <c r="C32" s="22">
         <f t="shared" si="2"/>
         <v>7.2868311341314937</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="22">
         <f t="shared" si="2"/>
         <v>25.374219793847633</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="22">
         <f t="shared" si="2"/>
         <v>52.644979844062107</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="22">
         <f t="shared" si="2"/>
         <v>88.358165338934867</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="22">
         <f t="shared" si="2"/>
         <v>132.03367546679962</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="22">
+      <c r="B33" s="21">
         <v>60</v>
       </c>
-      <c r="C33" s="23">
+      <c r="C33" s="22">
         <f t="shared" si="2"/>
         <v>9.3045546751725041</v>
       </c>
-      <c r="D33" s="23">
+      <c r="D33" s="22">
         <f t="shared" si="2"/>
         <v>32.400341254764037</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="22">
         <f t="shared" si="2"/>
         <v>67.222374762882893</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="22">
         <f t="shared" si="2"/>
         <v>112.82454132128592</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="22">
         <f t="shared" si="2"/>
         <v>168.59380020355641</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="22">
+      <c r="B34" s="21">
         <v>70</v>
       </c>
-      <c r="C34" s="23">
+      <c r="C34" s="22">
         <f t="shared" si="2"/>
         <v>11.880985864727768</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D34" s="22">
         <f t="shared" si="2"/>
         <v>41.371995748208192</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="22">
         <f t="shared" si="2"/>
         <v>85.83625033472515</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="22">
         <f t="shared" si="2"/>
         <v>144.06565681314996</v>
       </c>
-      <c r="G34" s="23">
+      <c r="G34" s="22">
         <f t="shared" si="2"/>
         <v>215.27742347992114</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="22">
+      <c r="B35" s="21">
         <v>80</v>
       </c>
-      <c r="C35" s="23">
+      <c r="C35" s="22">
         <f t="shared" si="2"/>
         <v>15.170830850670884</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="22">
         <f t="shared" si="2"/>
         <v>52.82790137088702</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="22">
         <f t="shared" si="2"/>
         <v>109.6043080524105</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="22">
         <f t="shared" si="2"/>
         <v>183.95743718471113</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="22">
         <f t="shared" si="2"/>
         <v>274.88774204151122</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="22">
+      <c r="B36" s="21">
         <v>90</v>
       </c>
-      <c r="C36" s="23">
+      <c r="C36" s="22">
         <f t="shared" si="2"/>
         <v>19.371633913221643</v>
       </c>
-      <c r="D36" s="23">
+      <c r="D36" s="22">
         <f t="shared" si="2"/>
         <v>67.455947260485615</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="22">
         <f t="shared" si="2"/>
         <v>139.95374095212296</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="22">
         <f t="shared" si="2"/>
         <v>234.89525154115753</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="22">
         <f t="shared" si="2"/>
         <v>351.00415781280554</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="22">
+      <c r="B37" s="21">
         <v>100</v>
       </c>
-      <c r="C37" s="23">
+      <c r="C37" s="22">
         <f t="shared" si="2"/>
         <v>24.735639343792712</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D37" s="22">
         <f t="shared" si="2"/>
         <v>86.13449905691408</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="22">
         <f t="shared" si="2"/>
         <v>178.70693182176578</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="22">
         <f t="shared" si="2"/>
         <v>299.93774669290406</v>
       </c>
-      <c r="G37" s="23">
+      <c r="G37" s="22">
         <f t="shared" si="2"/>
         <v>448.19720911117139</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="22">
+      <c r="B38" s="21">
         <v>110</v>
       </c>
-      <c r="C38" s="23">
+      <c r="C38" s="22">
         <f t="shared" si="2"/>
         <v>31.584937878088908</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="22">
         <f t="shared" si="2"/>
         <v>109.98514184577355</v>
       </c>
-      <c r="E38" s="23">
+      <c r="E38" s="22">
         <f t="shared" si="2"/>
         <v>228.19088124321266</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="22">
         <f t="shared" si="2"/>
         <v>382.99050875216915</v>
       </c>
-      <c r="G38" s="23">
+      <c r="G38" s="22">
         <f t="shared" si="2"/>
         <v>572.30301631405462</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="22">
+      <c r="B39" s="21">
         <v>120</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C39" s="22">
         <f t="shared" si="2"/>
         <v>40.330807176531721</v>
       </c>
-      <c r="D39" s="23">
+      <c r="D39" s="22">
         <f t="shared" si="2"/>
         <v>140.44002762286823</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="22">
         <f t="shared" si="2"/>
         <v>291.3769362594582</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="22">
         <f t="shared" si="2"/>
         <v>489.04058062564462</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="22">
         <f t="shared" si="2"/>
         <v>730.77372153141607</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="22">
+      <c r="B40" s="21">
         <v>130</v>
       </c>
-      <c r="C40" s="23">
+      <c r="C40" s="22">
         <f t="shared" si="2"/>
         <v>51.498407683713339</v>
       </c>
-      <c r="D40" s="23">
+      <c r="D40" s="22">
         <f t="shared" si="2"/>
         <v>179.32787127164036</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="22">
         <f t="shared" si="2"/>
         <v>372.05920990970202</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="22">
         <f t="shared" si="2"/>
         <v>624.45591740088537</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G40" s="22">
         <f t="shared" si="2"/>
         <v>933.12496502346505</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="22">
+      <c r="B41" s="21">
         <v>140</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="22">
         <f t="shared" si="2"/>
         <v>65.758316771333554</v>
       </c>
-      <c r="D41" s="23">
+      <c r="D41" s="22">
         <f t="shared" si="2"/>
         <v>228.98375882675759</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E41" s="22">
         <f t="shared" si="2"/>
         <v>475.0824051336985</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="22">
         <f t="shared" si="2"/>
         <v>797.36776092919047</v>
       </c>
-      <c r="G41" s="23">
+      <c r="G41" s="22">
         <f t="shared" si="2"/>
         <v>1191.5072678384624</v>
       </c>

</xml_diff>

<commit_message>
Fixed size of creature waves in defend missions; Minor bugs/tweaks; MagFrag;
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
     <sheet name="Levels and Experience" sheetId="2" r:id="rId2"/>
-    <sheet name="Map Size" sheetId="3" r:id="rId3"/>
-    <sheet name="Encumbrance" sheetId="9" r:id="rId4"/>
-    <sheet name="Armour Reduction" sheetId="10" r:id="rId5"/>
-    <sheet name="Relations Levels" sheetId="6" r:id="rId6"/>
-    <sheet name="Mercenary Cost" sheetId="5" r:id="rId7"/>
-    <sheet name="Difficulty Scaling" sheetId="7" r:id="rId8"/>
-    <sheet name="Colony Growth" sheetId="8" r:id="rId9"/>
+    <sheet name="Mission Items" sheetId="11" r:id="rId3"/>
+    <sheet name="Map Size" sheetId="3" r:id="rId4"/>
+    <sheet name="Encumbrance" sheetId="9" r:id="rId5"/>
+    <sheet name="Armour Reduction" sheetId="10" r:id="rId6"/>
+    <sheet name="Relations Levels" sheetId="6" r:id="rId7"/>
+    <sheet name="Mercenary Cost" sheetId="5" r:id="rId8"/>
+    <sheet name="Difficulty Scaling" sheetId="7" r:id="rId9"/>
+    <sheet name="Colony Growth" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>Width</t>
   </si>
@@ -222,6 +223,30 @@
   <si>
     <t>n/a</t>
   </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Value/Hulk</t>
+  </si>
+  <si>
+    <t>Value/Prec</t>
+  </si>
+  <si>
+    <t>Mult</t>
+  </si>
+  <si>
+    <t>Hulk Base</t>
+  </si>
+  <si>
+    <t>Prec Base</t>
+  </si>
+  <si>
+    <t>Hulk Mult</t>
+  </si>
+  <si>
+    <t>Prec Mult</t>
+  </si>
 </sst>
 </file>
 
@@ -408,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -471,6 +496,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,11 +961,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="41037864"/>
-        <c:axId val="41039432"/>
+        <c:axId val="634414120"/>
+        <c:axId val="634412552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41037864"/>
+        <c:axId val="634414120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -994,12 +1023,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41039432"/>
+        <c:crossAx val="634412552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41039432"/>
+        <c:axId val="634412552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1057,7 +1086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41037864"/>
+        <c:crossAx val="634414120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1499,11 +1528,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="584757960"/>
-        <c:axId val="584765016"/>
+        <c:axId val="634404712"/>
+        <c:axId val="634413728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="584757960"/>
+        <c:axId val="634404712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,12 +1589,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="584765016"/>
+        <c:crossAx val="634413728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="584765016"/>
+        <c:axId val="634413728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1622,7 +1651,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="584757960"/>
+        <c:crossAx val="634404712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4075,6 +4104,915 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>4</v>
+      </c>
+      <c r="G4" s="8">
+        <v>5</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4">
+        <v>2.5</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="21">
+        <v>0</v>
+      </c>
+      <c r="C5" s="22">
+        <f>POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="22">
+        <f t="shared" ref="D5:G5" si="0">POWER(D$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
+        <v>8.7055056329612412</v>
+      </c>
+      <c r="E5" s="22">
+        <f t="shared" si="0"/>
+        <v>18.061685139605196</v>
+      </c>
+      <c r="F5" s="22">
+        <f t="shared" si="0"/>
+        <v>30.31433133020796</v>
+      </c>
+      <c r="G5" s="22">
+        <f t="shared" si="0"/>
+        <v>45.298728979855973</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5">
+        <v>365</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="21">
+        <v>10</v>
+      </c>
+      <c r="C6" s="22">
+        <f t="shared" ref="C6:G19" si="1">POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B6-$K$8)/$K$7))) / $K$5</f>
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="22">
+        <f t="shared" si="1"/>
+        <v>8.7055056329612412</v>
+      </c>
+      <c r="E6" s="22">
+        <f t="shared" si="1"/>
+        <v>18.061685139605196</v>
+      </c>
+      <c r="F6" s="22">
+        <f t="shared" si="1"/>
+        <v>30.31433133020796</v>
+      </c>
+      <c r="G6" s="22">
+        <f t="shared" si="1"/>
+        <v>45.298728979855973</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="21">
+        <v>20</v>
+      </c>
+      <c r="C7" s="22">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="22">
+        <f t="shared" si="1"/>
+        <v>8.7055056329612412</v>
+      </c>
+      <c r="E7" s="22">
+        <f t="shared" si="1"/>
+        <v>18.061685139605196</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" si="1"/>
+        <v>30.31433133020796</v>
+      </c>
+      <c r="G7" s="22">
+        <f t="shared" si="1"/>
+        <v>45.298728979855973</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="21">
+        <v>30</v>
+      </c>
+      <c r="C8" s="22">
+        <f t="shared" si="1"/>
+        <v>3.1922499999999991</v>
+      </c>
+      <c r="D8" s="22">
+        <f t="shared" si="1"/>
+        <v>11.116060142728207</v>
+      </c>
+      <c r="E8" s="22">
+        <f t="shared" si="1"/>
+        <v>23.062965754761869</v>
+      </c>
+      <c r="F8" s="22">
+        <f t="shared" si="1"/>
+        <v>38.708369675542535</v>
+      </c>
+      <c r="G8" s="22">
+        <f t="shared" si="1"/>
+        <v>57.841947034378073</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="21">
+        <v>40</v>
+      </c>
+      <c r="C9" s="22">
+        <f t="shared" si="1"/>
+        <v>4.0761840249999981</v>
+      </c>
+      <c r="D9" s="22">
+        <f t="shared" si="1"/>
+        <v>14.194097196249643</v>
+      </c>
+      <c r="E9" s="22">
+        <f t="shared" si="1"/>
+        <v>29.449100972255422</v>
+      </c>
+      <c r="F9" s="22">
+        <f t="shared" si="1"/>
+        <v>49.426717238700256</v>
+      </c>
+      <c r="G9" s="22">
+        <f t="shared" si="1"/>
+        <v>73.858382168197352</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="21">
+        <v>50</v>
+      </c>
+      <c r="C10" s="22">
+        <f t="shared" si="1"/>
+        <v>5.2048793815224963</v>
+      </c>
+      <c r="D10" s="22">
+        <f t="shared" si="1"/>
+        <v>18.124442709891163</v>
+      </c>
+      <c r="E10" s="22">
+        <f t="shared" si="1"/>
+        <v>37.603557031472938</v>
+      </c>
+      <c r="F10" s="22">
+        <f t="shared" si="1"/>
+        <v>63.112975242096333</v>
+      </c>
+      <c r="G10" s="22">
+        <f t="shared" si="1"/>
+        <v>94.309768190571162</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="21">
+        <v>60</v>
+      </c>
+      <c r="C11" s="22">
+        <f t="shared" si="1"/>
+        <v>6.6461104822660744</v>
+      </c>
+      <c r="D11" s="22">
+        <f t="shared" si="1"/>
+        <v>23.143100896260023</v>
+      </c>
+      <c r="E11" s="22">
+        <f t="shared" si="1"/>
+        <v>48.01598197348779</v>
+      </c>
+      <c r="F11" s="22">
+        <f t="shared" si="1"/>
+        <v>80.5889580866328</v>
+      </c>
+      <c r="G11" s="22">
+        <f t="shared" si="1"/>
+        <v>120.4241430025403</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="21">
+        <v>70</v>
+      </c>
+      <c r="C12" s="22">
+        <f t="shared" si="1"/>
+        <v>8.4864184748055482</v>
+      </c>
+      <c r="D12" s="22">
+        <f t="shared" si="1"/>
+        <v>29.551425534434419</v>
+      </c>
+      <c r="E12" s="22">
+        <f t="shared" si="1"/>
+        <v>61.311607381946537</v>
+      </c>
+      <c r="F12" s="22">
+        <f t="shared" si="1"/>
+        <v>102.9040405808214</v>
+      </c>
+      <c r="G12" s="22">
+        <f t="shared" si="1"/>
+        <v>153.76958819994368</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="21">
+        <v>80</v>
+      </c>
+      <c r="C13" s="22">
+        <f t="shared" si="1"/>
+        <v>10.8363077504792</v>
+      </c>
+      <c r="D13" s="22">
+        <f t="shared" si="1"/>
+        <v>37.7342152649193</v>
+      </c>
+      <c r="E13" s="22">
+        <f t="shared" si="1"/>
+        <v>78.288791466007524</v>
+      </c>
+      <c r="F13" s="22">
+        <f t="shared" si="1"/>
+        <v>131.39816941765079</v>
+      </c>
+      <c r="G13" s="22">
+        <f t="shared" si="1"/>
+        <v>196.34838717250804</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="21">
+        <v>90</v>
+      </c>
+      <c r="C14" s="22">
+        <f t="shared" si="1"/>
+        <v>13.836881366586889</v>
+      </c>
+      <c r="D14" s="22">
+        <f t="shared" si="1"/>
+        <v>48.182819471775439</v>
+      </c>
+      <c r="E14" s="22">
+        <f t="shared" si="1"/>
+        <v>99.966957822944977</v>
+      </c>
+      <c r="F14" s="22">
+        <f t="shared" si="1"/>
+        <v>167.78232252939827</v>
+      </c>
+      <c r="G14" s="22">
+        <f t="shared" si="1"/>
+        <v>250.71725558057545</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="21">
+        <v>100</v>
+      </c>
+      <c r="C15" s="22">
+        <f t="shared" si="1"/>
+        <v>17.668313816994797</v>
+      </c>
+      <c r="D15" s="22">
+        <f t="shared" si="1"/>
+        <v>61.524642183510053</v>
+      </c>
+      <c r="E15" s="22">
+        <f t="shared" si="1"/>
+        <v>127.64780844411843</v>
+      </c>
+      <c r="F15" s="22">
+        <f t="shared" si="1"/>
+        <v>214.24124763778863</v>
+      </c>
+      <c r="G15" s="22">
+        <f t="shared" si="1"/>
+        <v>320.14086365083676</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="21">
+        <v>110</v>
+      </c>
+      <c r="C16" s="22">
+        <f t="shared" si="1"/>
+        <v>22.560669912920648</v>
+      </c>
+      <c r="D16" s="22">
+        <f t="shared" si="1"/>
+        <v>78.560815604123974</v>
+      </c>
+      <c r="E16" s="22">
+        <f t="shared" si="1"/>
+        <v>162.99348660229478</v>
+      </c>
+      <c r="F16" s="22">
+        <f t="shared" si="1"/>
+        <v>273.56464910869221</v>
+      </c>
+      <c r="G16" s="22">
+        <f t="shared" si="1"/>
+        <v>408.78786879575335</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="21">
+        <v>120</v>
+      </c>
+      <c r="C17" s="22">
+        <f t="shared" si="1"/>
+        <v>28.807719411808367</v>
+      </c>
+      <c r="D17" s="22">
+        <f t="shared" si="1"/>
+        <v>100.31430544490587</v>
+      </c>
+      <c r="E17" s="22">
+        <f t="shared" si="1"/>
+        <v>208.12638304247014</v>
+      </c>
+      <c r="F17" s="22">
+        <f t="shared" si="1"/>
+        <v>349.31470044688899</v>
+      </c>
+      <c r="G17" s="22">
+        <f t="shared" si="1"/>
+        <v>521.98122966529729</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="21">
+        <v>130</v>
+      </c>
+      <c r="C18" s="22">
+        <f t="shared" si="1"/>
+        <v>36.7845769169381</v>
+      </c>
+      <c r="D18" s="22">
+        <f t="shared" si="1"/>
+        <v>128.09133662260027</v>
+      </c>
+      <c r="E18" s="22">
+        <f t="shared" si="1"/>
+        <v>265.75657850693005</v>
+      </c>
+      <c r="F18" s="22">
+        <f t="shared" si="1"/>
+        <v>446.03994100063244</v>
+      </c>
+      <c r="G18" s="22">
+        <f t="shared" si="1"/>
+        <v>666.51783215961791</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="21">
+        <v>140</v>
+      </c>
+      <c r="C19" s="22">
+        <f t="shared" si="1"/>
+        <v>46.97022626523826</v>
+      </c>
+      <c r="D19" s="22">
+        <f t="shared" si="1"/>
+        <v>163.55982773339827</v>
+      </c>
+      <c r="E19" s="22">
+        <f t="shared" si="1"/>
+        <v>339.34457509549895</v>
+      </c>
+      <c r="F19" s="22">
+        <f t="shared" si="1"/>
+        <v>569.54840066370753</v>
+      </c>
+      <c r="G19" s="22">
+        <f t="shared" si="1"/>
+        <v>851.07661988461609</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8">
+        <v>2</v>
+      </c>
+      <c r="E26" s="8">
+        <v>3</v>
+      </c>
+      <c r="F26" s="8">
+        <v>4</v>
+      </c>
+      <c r="G26" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="21">
+        <v>0</v>
+      </c>
+      <c r="C27" s="22">
+        <f t="shared" ref="C27:G41" si="2">POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
+        <v>3.5</v>
+      </c>
+      <c r="D27" s="22">
+        <f t="shared" si="2"/>
+        <v>12.187707886145738</v>
+      </c>
+      <c r="E27" s="22">
+        <f t="shared" si="2"/>
+        <v>25.286359195447272</v>
+      </c>
+      <c r="F27" s="22">
+        <f t="shared" si="2"/>
+        <v>42.44006386229114</v>
+      </c>
+      <c r="G27" s="22">
+        <f t="shared" si="2"/>
+        <v>63.418220571798358</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="21">
+        <v>10</v>
+      </c>
+      <c r="C28" s="22">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+      <c r="D28" s="22">
+        <f t="shared" si="2"/>
+        <v>12.187707886145738</v>
+      </c>
+      <c r="E28" s="22">
+        <f t="shared" si="2"/>
+        <v>25.286359195447272</v>
+      </c>
+      <c r="F28" s="22">
+        <f t="shared" si="2"/>
+        <v>42.44006386229114</v>
+      </c>
+      <c r="G28" s="22">
+        <f t="shared" si="2"/>
+        <v>63.418220571798358</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="21">
+        <v>20</v>
+      </c>
+      <c r="C29" s="22">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+      <c r="D29" s="22">
+        <f t="shared" si="2"/>
+        <v>12.187707886145738</v>
+      </c>
+      <c r="E29" s="22">
+        <f t="shared" si="2"/>
+        <v>25.286359195447272</v>
+      </c>
+      <c r="F29" s="22">
+        <f t="shared" si="2"/>
+        <v>42.44006386229114</v>
+      </c>
+      <c r="G29" s="22">
+        <f t="shared" si="2"/>
+        <v>63.418220571798358</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="21">
+        <v>30</v>
+      </c>
+      <c r="C30" s="22">
+        <f t="shared" si="2"/>
+        <v>4.4691499999999991</v>
+      </c>
+      <c r="D30" s="22">
+        <f t="shared" si="2"/>
+        <v>15.56248419981949</v>
+      </c>
+      <c r="E30" s="22">
+        <f t="shared" si="2"/>
+        <v>32.288152056666611</v>
+      </c>
+      <c r="F30" s="22">
+        <f t="shared" si="2"/>
+        <v>54.191717545759545</v>
+      </c>
+      <c r="G30" s="22">
+        <f t="shared" si="2"/>
+        <v>80.978725848129301</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="21">
+        <v>40</v>
+      </c>
+      <c r="C31" s="22">
+        <f t="shared" si="2"/>
+        <v>5.7066576349999965</v>
+      </c>
+      <c r="D31" s="22">
+        <f t="shared" si="2"/>
+        <v>19.871736074749503</v>
+      </c>
+      <c r="E31" s="22">
+        <f t="shared" si="2"/>
+        <v>41.228741361157589</v>
+      </c>
+      <c r="F31" s="22">
+        <f t="shared" si="2"/>
+        <v>69.197404134180346</v>
+      </c>
+      <c r="G31" s="22">
+        <f t="shared" si="2"/>
+        <v>103.40173503547628</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="21">
+        <v>50</v>
+      </c>
+      <c r="C32" s="22">
+        <f t="shared" si="2"/>
+        <v>7.2868311341314937</v>
+      </c>
+      <c r="D32" s="22">
+        <f t="shared" si="2"/>
+        <v>25.374219793847633</v>
+      </c>
+      <c r="E32" s="22">
+        <f t="shared" si="2"/>
+        <v>52.644979844062107</v>
+      </c>
+      <c r="F32" s="22">
+        <f t="shared" si="2"/>
+        <v>88.358165338934867</v>
+      </c>
+      <c r="G32" s="22">
+        <f t="shared" si="2"/>
+        <v>132.03367546679962</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="21">
+        <v>60</v>
+      </c>
+      <c r="C33" s="22">
+        <f t="shared" si="2"/>
+        <v>9.3045546751725041</v>
+      </c>
+      <c r="D33" s="22">
+        <f t="shared" si="2"/>
+        <v>32.400341254764037</v>
+      </c>
+      <c r="E33" s="22">
+        <f t="shared" si="2"/>
+        <v>67.222374762882893</v>
+      </c>
+      <c r="F33" s="22">
+        <f t="shared" si="2"/>
+        <v>112.82454132128592</v>
+      </c>
+      <c r="G33" s="22">
+        <f t="shared" si="2"/>
+        <v>168.59380020355641</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="21">
+        <v>70</v>
+      </c>
+      <c r="C34" s="22">
+        <f t="shared" si="2"/>
+        <v>11.880985864727768</v>
+      </c>
+      <c r="D34" s="22">
+        <f t="shared" si="2"/>
+        <v>41.371995748208192</v>
+      </c>
+      <c r="E34" s="22">
+        <f t="shared" si="2"/>
+        <v>85.83625033472515</v>
+      </c>
+      <c r="F34" s="22">
+        <f t="shared" si="2"/>
+        <v>144.06565681314996</v>
+      </c>
+      <c r="G34" s="22">
+        <f t="shared" si="2"/>
+        <v>215.27742347992114</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="21">
+        <v>80</v>
+      </c>
+      <c r="C35" s="22">
+        <f t="shared" si="2"/>
+        <v>15.170830850670884</v>
+      </c>
+      <c r="D35" s="22">
+        <f t="shared" si="2"/>
+        <v>52.82790137088702</v>
+      </c>
+      <c r="E35" s="22">
+        <f t="shared" si="2"/>
+        <v>109.6043080524105</v>
+      </c>
+      <c r="F35" s="22">
+        <f t="shared" si="2"/>
+        <v>183.95743718471113</v>
+      </c>
+      <c r="G35" s="22">
+        <f t="shared" si="2"/>
+        <v>274.88774204151122</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="21">
+        <v>90</v>
+      </c>
+      <c r="C36" s="22">
+        <f t="shared" si="2"/>
+        <v>19.371633913221643</v>
+      </c>
+      <c r="D36" s="22">
+        <f t="shared" si="2"/>
+        <v>67.455947260485615</v>
+      </c>
+      <c r="E36" s="22">
+        <f t="shared" si="2"/>
+        <v>139.95374095212296</v>
+      </c>
+      <c r="F36" s="22">
+        <f t="shared" si="2"/>
+        <v>234.89525154115753</v>
+      </c>
+      <c r="G36" s="22">
+        <f t="shared" si="2"/>
+        <v>351.00415781280554</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="21">
+        <v>100</v>
+      </c>
+      <c r="C37" s="22">
+        <f t="shared" si="2"/>
+        <v>24.735639343792712</v>
+      </c>
+      <c r="D37" s="22">
+        <f t="shared" si="2"/>
+        <v>86.13449905691408</v>
+      </c>
+      <c r="E37" s="22">
+        <f t="shared" si="2"/>
+        <v>178.70693182176578</v>
+      </c>
+      <c r="F37" s="22">
+        <f t="shared" si="2"/>
+        <v>299.93774669290406</v>
+      </c>
+      <c r="G37" s="22">
+        <f t="shared" si="2"/>
+        <v>448.19720911117139</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="21">
+        <v>110</v>
+      </c>
+      <c r="C38" s="22">
+        <f t="shared" si="2"/>
+        <v>31.584937878088908</v>
+      </c>
+      <c r="D38" s="22">
+        <f t="shared" si="2"/>
+        <v>109.98514184577355</v>
+      </c>
+      <c r="E38" s="22">
+        <f t="shared" si="2"/>
+        <v>228.19088124321266</v>
+      </c>
+      <c r="F38" s="22">
+        <f t="shared" si="2"/>
+        <v>382.99050875216915</v>
+      </c>
+      <c r="G38" s="22">
+        <f t="shared" si="2"/>
+        <v>572.30301631405462</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="21">
+        <v>120</v>
+      </c>
+      <c r="C39" s="22">
+        <f t="shared" si="2"/>
+        <v>40.330807176531721</v>
+      </c>
+      <c r="D39" s="22">
+        <f t="shared" si="2"/>
+        <v>140.44002762286823</v>
+      </c>
+      <c r="E39" s="22">
+        <f t="shared" si="2"/>
+        <v>291.3769362594582</v>
+      </c>
+      <c r="F39" s="22">
+        <f t="shared" si="2"/>
+        <v>489.04058062564462</v>
+      </c>
+      <c r="G39" s="22">
+        <f t="shared" si="2"/>
+        <v>730.77372153141607</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="21">
+        <v>130</v>
+      </c>
+      <c r="C40" s="22">
+        <f t="shared" si="2"/>
+        <v>51.498407683713339</v>
+      </c>
+      <c r="D40" s="22">
+        <f t="shared" si="2"/>
+        <v>179.32787127164036</v>
+      </c>
+      <c r="E40" s="22">
+        <f t="shared" si="2"/>
+        <v>372.05920990970202</v>
+      </c>
+      <c r="F40" s="22">
+        <f t="shared" si="2"/>
+        <v>624.45591740088537</v>
+      </c>
+      <c r="G40" s="22">
+        <f t="shared" si="2"/>
+        <v>933.12496502346505</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="21">
+        <v>140</v>
+      </c>
+      <c r="C41" s="22">
+        <f t="shared" si="2"/>
+        <v>65.758316771333554</v>
+      </c>
+      <c r="D41" s="22">
+        <f t="shared" si="2"/>
+        <v>228.98375882675759</v>
+      </c>
+      <c r="E41" s="22">
+        <f t="shared" si="2"/>
+        <v>475.0824051336985</v>
+      </c>
+      <c r="F41" s="22">
+        <f t="shared" si="2"/>
+        <v>797.36776092919047</v>
+      </c>
+      <c r="G41" s="22">
+        <f t="shared" si="2"/>
+        <v>1191.5072678384624</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J22"/>
@@ -4388,6 +5326,401 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="36">
+        <f>POWER($J$3,$B4)*$J$4</f>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="36">
+        <f t="shared" ref="C5:C28" si="0">POWER($J$3,$B5)*$J$4</f>
+        <v>6.2846000000000011</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="36">
+        <f t="shared" si="0"/>
+        <v>8.4213640000000023</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="36">
+        <f t="shared" si="0"/>
+        <v>11.284627760000005</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="36">
+        <f t="shared" si="0"/>
+        <v>15.121401198400006</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="36">
+        <f t="shared" si="0"/>
+        <v>20.262677605856013</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="36">
+        <f t="shared" si="0"/>
+        <v>27.151987991847054</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="36">
+        <f t="shared" si="0"/>
+        <v>36.383663909075061</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="36">
+        <f t="shared" si="0"/>
+        <v>48.754109638160585</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="36">
+        <f t="shared" si="0"/>
+        <v>65.330506915135189</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" s="36">
+        <f t="shared" si="0"/>
+        <v>87.542879266281147</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" s="36">
+        <f t="shared" si="0"/>
+        <v>117.30745821681678</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D5:D28" si="1">ROUND(POWER($J$5,$B15)*$J$6,0)*10</f>
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="36">
+        <f t="shared" si="0"/>
+        <v>157.1919940105345</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>5350</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="36">
+        <f t="shared" si="0"/>
+        <v>210.63727197411623</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>7010</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" s="36">
+        <f t="shared" si="0"/>
+        <v>282.25394444531571</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>9190</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E5:E28" si="2">ROUND(POWER($J$7,$B18)*$J$8,0)*10</f>
+        <v>14360</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" s="36">
+        <f t="shared" si="0"/>
+        <v>378.22028555672318</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>12040</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>18810</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="36">
+        <f t="shared" si="0"/>
+        <v>506.81518264600902</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>15770</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>24630</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21" s="36">
+        <f t="shared" si="0"/>
+        <v>679.13234474565229</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>20650</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>32270</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22" s="36">
+        <f t="shared" si="0"/>
+        <v>910.037341959174</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>27060</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>42280</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23" s="36">
+        <f t="shared" si="0"/>
+        <v>1219.4500382252934</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>35440</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>55380</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24" s="36">
+        <f t="shared" si="0"/>
+        <v>1634.0630512218931</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>46430</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>72550</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25" s="36">
+        <f t="shared" si="0"/>
+        <v>2189.6444886373374</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>60830</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>95040</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26" s="36">
+        <f t="shared" si="0"/>
+        <v>2934.1236147740319</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>79680</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>124500</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27" s="36">
+        <f t="shared" si="0"/>
+        <v>3931.7256437972032</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>104380</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>163100</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28" s="36">
+        <f t="shared" si="0"/>
+        <v>5268.5123626882532</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>136740</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>213660</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4561,7 +5894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F28"/>
   <sheetViews>
@@ -4831,11 +6164,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -4870,7 +6203,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="32">
-        <f>100*POWER($G$3,B3/$G$4)</f>
+        <f t="shared" ref="C3:C27" si="0">100*POWER($G$3,B3/$G$4)</f>
         <v>100</v>
       </c>
       <c r="D3">
@@ -4892,11 +6225,11 @@
         <v>1</v>
       </c>
       <c r="C4" s="32">
-        <f>100*POWER($G$3,B4/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>97.715996843424591</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D27" si="0">100*POWER($H$3,POWER(B4/$H$4,$H$5))</f>
+        <f t="shared" ref="D4:D27" si="1">100*POWER($H$3,POWER(B4/$H$4,$H$5))</f>
         <v>97.064458573273242</v>
       </c>
       <c r="F4" s="31" t="s">
@@ -4914,11 +6247,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="32">
-        <f>100*POWER($G$3,B5/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>95.484160391041655</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>94.591812522665393</v>
       </c>
       <c r="F5" s="35" t="s">
@@ -4936,11 +6269,11 @@
         <v>4</v>
       </c>
       <c r="C6" s="32">
-        <f>100*POWER($G$3,B6/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>91.172248855821678</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>90.144892671268622</v>
       </c>
     </row>
@@ -4949,11 +6282,11 @@
         <v>6</v>
       </c>
       <c r="C7" s="32">
-        <f>100*POWER($G$3,B7/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>87.055056329612412</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86.118675990610768</v>
       </c>
     </row>
@@ -4962,11 +6295,11 @@
         <v>8</v>
       </c>
       <c r="C8" s="32">
-        <f>100*POWER($G$3,B8/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>83.123789614278778</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>82.3980943939046</v>
       </c>
     </row>
@@ -4975,11 +6308,11 @@
         <v>10</v>
       </c>
       <c r="C9" s="32">
-        <f>100*POWER($G$3,B9/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>79.370052598409984</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>78.925220537571477</v>
       </c>
     </row>
@@ -4988,11 +6321,11 @@
         <v>15</v>
       </c>
       <c r="C10" s="32">
-        <f>100*POWER($G$3,B10/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>70.710678118654755</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71.113160110456874</v>
       </c>
     </row>
@@ -5001,11 +6334,11 @@
         <v>20</v>
       </c>
       <c r="C11" s="32">
-        <f>100*POWER($G$3,B11/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>62.996052494743658</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64.29806574927926</v>
       </c>
     </row>
@@ -5014,11 +6347,11 @@
         <v>25</v>
       </c>
       <c r="C12" s="32">
-        <f>100*POWER($G$3,B12/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>56.123102415468651</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58.282485186967683</v>
       </c>
     </row>
@@ -5027,11 +6360,11 @@
         <v>30</v>
       </c>
       <c r="C13" s="32">
-        <f>100*POWER($G$3,B13/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52.933290315596146</v>
       </c>
     </row>
@@ -5040,11 +6373,11 @@
         <v>35</v>
       </c>
       <c r="C14" s="32">
-        <f>100*POWER($G$3,B14/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>44.544935907016963</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48.151978235305769</v>
       </c>
     </row>
@@ -5053,11 +6386,11 @@
         <v>40</v>
       </c>
       <c r="C15" s="32">
-        <f>100*POWER($G$3,B15/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>39.685026299204992</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43.861617315434934</v>
       </c>
     </row>
@@ -5066,11 +6399,11 @@
         <v>45</v>
       </c>
       <c r="C16" s="32">
-        <f>100*POWER($G$3,B16/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>35.355339059327378</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
@@ -5079,11 +6412,11 @@
         <v>50</v>
       </c>
       <c r="C17" s="32">
-        <f>100*POWER($G$3,B17/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>31.498026247371829</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36.51560942092317</v>
       </c>
     </row>
@@ -5092,11 +6425,11 @@
         <v>60</v>
       </c>
       <c r="C18" s="32">
-        <f>100*POWER($G$3,B18/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30.511241564292174</v>
       </c>
     </row>
@@ -5105,11 +6438,11 @@
         <v>70</v>
       </c>
       <c r="C19" s="32">
-        <f>100*POWER($G$3,B19/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>19.842513149602492</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.570371161108223</v>
       </c>
     </row>
@@ -5118,11 +6451,11 @@
         <v>80</v>
       </c>
       <c r="C20" s="32">
-        <f>100*POWER($G$3,B20/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>15.749013123685918</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.48356373280761</v>
       </c>
     </row>
@@ -5131,11 +6464,11 @@
         <v>90</v>
       </c>
       <c r="C21" s="32">
-        <f>100*POWER($G$3,B21/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.089130275866257</v>
       </c>
     </row>
@@ -5144,11 +6477,11 @@
         <v>100</v>
       </c>
       <c r="C22" s="32">
-        <f>100*POWER($G$3,B22/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>9.921256574801248</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.260055429207236</v>
       </c>
     </row>
@@ -5157,11 +6490,11 @@
         <v>120</v>
       </c>
       <c r="C23" s="32">
-        <f>100*POWER($G$3,B23/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.913602200790223</v>
       </c>
     </row>
@@ -5170,11 +6503,11 @@
         <v>140</v>
       </c>
       <c r="C24" s="32">
-        <f>100*POWER($G$3,B24/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>3.9372532809214773</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.8487089083892334</v>
       </c>
     </row>
@@ -5183,11 +6516,11 @@
         <v>160</v>
       </c>
       <c r="C25" s="32">
-        <f>100*POWER($G$3,B25/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>2.480314143700312</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.6710872889019068</v>
       </c>
     </row>
@@ -5196,11 +6529,11 @@
         <v>180</v>
       </c>
       <c r="C26" s="32">
-        <f>100*POWER($G$3,B26/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>1.5625</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1142663640113337</v>
       </c>
     </row>
@@ -5209,11 +6542,11 @@
         <v>200</v>
       </c>
       <c r="C27" s="32">
-        <f>100*POWER($G$3,B27/$G$4)</f>
+        <f t="shared" si="0"/>
         <v>0.98431332023036966</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.9954483247075605</v>
       </c>
     </row>
@@ -5224,7 +6557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
@@ -6580,7 +7913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F22"/>
   <sheetViews>
@@ -6802,7 +8135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J48"/>
   <sheetViews>
@@ -7646,913 +8979,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E3" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8">
-        <v>2</v>
-      </c>
-      <c r="E4" s="8">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8">
-        <v>4</v>
-      </c>
-      <c r="G4" s="8">
-        <v>5</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4">
-        <v>2.5</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="21">
-        <v>0</v>
-      </c>
-      <c r="C5" s="22">
-        <f>POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
-        <v>2.5</v>
-      </c>
-      <c r="D5" s="22">
-        <f t="shared" ref="D5:G5" si="0">POWER(D$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B5-$K$8)/$K$7))) / $K$5</f>
-        <v>8.7055056329612412</v>
-      </c>
-      <c r="E5" s="22">
-        <f t="shared" si="0"/>
-        <v>18.061685139605196</v>
-      </c>
-      <c r="F5" s="22">
-        <f t="shared" si="0"/>
-        <v>30.31433133020796</v>
-      </c>
-      <c r="G5" s="22">
-        <f t="shared" si="0"/>
-        <v>45.298728979855973</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5">
-        <v>365</v>
-      </c>
-      <c r="N5" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="21">
-        <v>10</v>
-      </c>
-      <c r="C6" s="22">
-        <f t="shared" ref="C6:G19" si="1">POWER(C$4,$K$3)*($K$5*($K$4+0))*MAX(1,(POWER($K$6,($B6-$K$8)/$K$7))) / $K$5</f>
-        <v>2.5</v>
-      </c>
-      <c r="D6" s="22">
-        <f t="shared" si="1"/>
-        <v>8.7055056329612412</v>
-      </c>
-      <c r="E6" s="22">
-        <f t="shared" si="1"/>
-        <v>18.061685139605196</v>
-      </c>
-      <c r="F6" s="22">
-        <f t="shared" si="1"/>
-        <v>30.31433133020796</v>
-      </c>
-      <c r="G6" s="22">
-        <f t="shared" si="1"/>
-        <v>45.298728979855973</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="21">
-        <v>20</v>
-      </c>
-      <c r="C7" s="22">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="D7" s="22">
-        <f t="shared" si="1"/>
-        <v>8.7055056329612412</v>
-      </c>
-      <c r="E7" s="22">
-        <f t="shared" si="1"/>
-        <v>18.061685139605196</v>
-      </c>
-      <c r="F7" s="22">
-        <f t="shared" si="1"/>
-        <v>30.31433133020796</v>
-      </c>
-      <c r="G7" s="22">
-        <f t="shared" si="1"/>
-        <v>45.298728979855973</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7">
-        <v>5</v>
-      </c>
-      <c r="N7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="21">
-        <v>30</v>
-      </c>
-      <c r="C8" s="22">
-        <f t="shared" si="1"/>
-        <v>3.1922499999999991</v>
-      </c>
-      <c r="D8" s="22">
-        <f t="shared" si="1"/>
-        <v>11.116060142728207</v>
-      </c>
-      <c r="E8" s="22">
-        <f t="shared" si="1"/>
-        <v>23.062965754761869</v>
-      </c>
-      <c r="F8" s="22">
-        <f t="shared" si="1"/>
-        <v>38.708369675542535</v>
-      </c>
-      <c r="G8" s="22">
-        <f t="shared" si="1"/>
-        <v>57.841947034378073</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8">
-        <v>20</v>
-      </c>
-      <c r="N8" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="21">
-        <v>40</v>
-      </c>
-      <c r="C9" s="22">
-        <f t="shared" si="1"/>
-        <v>4.0761840249999981</v>
-      </c>
-      <c r="D9" s="22">
-        <f t="shared" si="1"/>
-        <v>14.194097196249643</v>
-      </c>
-      <c r="E9" s="22">
-        <f t="shared" si="1"/>
-        <v>29.449100972255422</v>
-      </c>
-      <c r="F9" s="22">
-        <f t="shared" si="1"/>
-        <v>49.426717238700256</v>
-      </c>
-      <c r="G9" s="22">
-        <f t="shared" si="1"/>
-        <v>73.858382168197352</v>
-      </c>
-      <c r="N9" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="21">
-        <v>50</v>
-      </c>
-      <c r="C10" s="22">
-        <f t="shared" si="1"/>
-        <v>5.2048793815224963</v>
-      </c>
-      <c r="D10" s="22">
-        <f t="shared" si="1"/>
-        <v>18.124442709891163</v>
-      </c>
-      <c r="E10" s="22">
-        <f t="shared" si="1"/>
-        <v>37.603557031472938</v>
-      </c>
-      <c r="F10" s="22">
-        <f t="shared" si="1"/>
-        <v>63.112975242096333</v>
-      </c>
-      <c r="G10" s="22">
-        <f t="shared" si="1"/>
-        <v>94.309768190571162</v>
-      </c>
-      <c r="N10" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="21">
-        <v>60</v>
-      </c>
-      <c r="C11" s="22">
-        <f t="shared" si="1"/>
-        <v>6.6461104822660744</v>
-      </c>
-      <c r="D11" s="22">
-        <f t="shared" si="1"/>
-        <v>23.143100896260023</v>
-      </c>
-      <c r="E11" s="22">
-        <f t="shared" si="1"/>
-        <v>48.01598197348779</v>
-      </c>
-      <c r="F11" s="22">
-        <f t="shared" si="1"/>
-        <v>80.5889580866328</v>
-      </c>
-      <c r="G11" s="22">
-        <f t="shared" si="1"/>
-        <v>120.4241430025403</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="21">
-        <v>70</v>
-      </c>
-      <c r="C12" s="22">
-        <f t="shared" si="1"/>
-        <v>8.4864184748055482</v>
-      </c>
-      <c r="D12" s="22">
-        <f t="shared" si="1"/>
-        <v>29.551425534434419</v>
-      </c>
-      <c r="E12" s="22">
-        <f t="shared" si="1"/>
-        <v>61.311607381946537</v>
-      </c>
-      <c r="F12" s="22">
-        <f t="shared" si="1"/>
-        <v>102.9040405808214</v>
-      </c>
-      <c r="G12" s="22">
-        <f t="shared" si="1"/>
-        <v>153.76958819994368</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="21">
-        <v>80</v>
-      </c>
-      <c r="C13" s="22">
-        <f t="shared" si="1"/>
-        <v>10.8363077504792</v>
-      </c>
-      <c r="D13" s="22">
-        <f t="shared" si="1"/>
-        <v>37.7342152649193</v>
-      </c>
-      <c r="E13" s="22">
-        <f t="shared" si="1"/>
-        <v>78.288791466007524</v>
-      </c>
-      <c r="F13" s="22">
-        <f t="shared" si="1"/>
-        <v>131.39816941765079</v>
-      </c>
-      <c r="G13" s="22">
-        <f t="shared" si="1"/>
-        <v>196.34838717250804</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="21">
-        <v>90</v>
-      </c>
-      <c r="C14" s="22">
-        <f t="shared" si="1"/>
-        <v>13.836881366586889</v>
-      </c>
-      <c r="D14" s="22">
-        <f t="shared" si="1"/>
-        <v>48.182819471775439</v>
-      </c>
-      <c r="E14" s="22">
-        <f t="shared" si="1"/>
-        <v>99.966957822944977</v>
-      </c>
-      <c r="F14" s="22">
-        <f t="shared" si="1"/>
-        <v>167.78232252939827</v>
-      </c>
-      <c r="G14" s="22">
-        <f t="shared" si="1"/>
-        <v>250.71725558057545</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="21">
-        <v>100</v>
-      </c>
-      <c r="C15" s="22">
-        <f t="shared" si="1"/>
-        <v>17.668313816994797</v>
-      </c>
-      <c r="D15" s="22">
-        <f t="shared" si="1"/>
-        <v>61.524642183510053</v>
-      </c>
-      <c r="E15" s="22">
-        <f t="shared" si="1"/>
-        <v>127.64780844411843</v>
-      </c>
-      <c r="F15" s="22">
-        <f t="shared" si="1"/>
-        <v>214.24124763778863</v>
-      </c>
-      <c r="G15" s="22">
-        <f t="shared" si="1"/>
-        <v>320.14086365083676</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="21">
-        <v>110</v>
-      </c>
-      <c r="C16" s="22">
-        <f t="shared" si="1"/>
-        <v>22.560669912920648</v>
-      </c>
-      <c r="D16" s="22">
-        <f t="shared" si="1"/>
-        <v>78.560815604123974</v>
-      </c>
-      <c r="E16" s="22">
-        <f t="shared" si="1"/>
-        <v>162.99348660229478</v>
-      </c>
-      <c r="F16" s="22">
-        <f t="shared" si="1"/>
-        <v>273.56464910869221</v>
-      </c>
-      <c r="G16" s="22">
-        <f t="shared" si="1"/>
-        <v>408.78786879575335</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="21">
-        <v>120</v>
-      </c>
-      <c r="C17" s="22">
-        <f t="shared" si="1"/>
-        <v>28.807719411808367</v>
-      </c>
-      <c r="D17" s="22">
-        <f t="shared" si="1"/>
-        <v>100.31430544490587</v>
-      </c>
-      <c r="E17" s="22">
-        <f t="shared" si="1"/>
-        <v>208.12638304247014</v>
-      </c>
-      <c r="F17" s="22">
-        <f t="shared" si="1"/>
-        <v>349.31470044688899</v>
-      </c>
-      <c r="G17" s="22">
-        <f t="shared" si="1"/>
-        <v>521.98122966529729</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="21">
-        <v>130</v>
-      </c>
-      <c r="C18" s="22">
-        <f t="shared" si="1"/>
-        <v>36.7845769169381</v>
-      </c>
-      <c r="D18" s="22">
-        <f t="shared" si="1"/>
-        <v>128.09133662260027</v>
-      </c>
-      <c r="E18" s="22">
-        <f t="shared" si="1"/>
-        <v>265.75657850693005</v>
-      </c>
-      <c r="F18" s="22">
-        <f t="shared" si="1"/>
-        <v>446.03994100063244</v>
-      </c>
-      <c r="G18" s="22">
-        <f t="shared" si="1"/>
-        <v>666.51783215961791</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="21">
-        <v>140</v>
-      </c>
-      <c r="C19" s="22">
-        <f t="shared" si="1"/>
-        <v>46.97022626523826</v>
-      </c>
-      <c r="D19" s="22">
-        <f t="shared" si="1"/>
-        <v>163.55982773339827</v>
-      </c>
-      <c r="E19" s="22">
-        <f t="shared" si="1"/>
-        <v>339.34457509549895</v>
-      </c>
-      <c r="F19" s="22">
-        <f t="shared" si="1"/>
-        <v>569.54840066370753</v>
-      </c>
-      <c r="G19" s="22">
-        <f t="shared" si="1"/>
-        <v>851.07661988461609</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="8">
-        <v>1</v>
-      </c>
-      <c r="D26" s="8">
-        <v>2</v>
-      </c>
-      <c r="E26" s="8">
-        <v>3</v>
-      </c>
-      <c r="F26" s="8">
-        <v>4</v>
-      </c>
-      <c r="G26" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="21">
-        <v>0</v>
-      </c>
-      <c r="C27" s="22">
-        <f t="shared" ref="C27:G41" si="2">POWER(C$4,$K$3)*($K$5*($K$4+1))*MAX(1,(POWER($K$6,($B27-$K$8)/$K$7))) / $K$5</f>
-        <v>3.5</v>
-      </c>
-      <c r="D27" s="22">
-        <f t="shared" si="2"/>
-        <v>12.187707886145738</v>
-      </c>
-      <c r="E27" s="22">
-        <f t="shared" si="2"/>
-        <v>25.286359195447272</v>
-      </c>
-      <c r="F27" s="22">
-        <f t="shared" si="2"/>
-        <v>42.44006386229114</v>
-      </c>
-      <c r="G27" s="22">
-        <f t="shared" si="2"/>
-        <v>63.418220571798358</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="21">
-        <v>10</v>
-      </c>
-      <c r="C28" s="22">
-        <f t="shared" si="2"/>
-        <v>3.5</v>
-      </c>
-      <c r="D28" s="22">
-        <f t="shared" si="2"/>
-        <v>12.187707886145738</v>
-      </c>
-      <c r="E28" s="22">
-        <f t="shared" si="2"/>
-        <v>25.286359195447272</v>
-      </c>
-      <c r="F28" s="22">
-        <f t="shared" si="2"/>
-        <v>42.44006386229114</v>
-      </c>
-      <c r="G28" s="22">
-        <f t="shared" si="2"/>
-        <v>63.418220571798358</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="21">
-        <v>20</v>
-      </c>
-      <c r="C29" s="22">
-        <f t="shared" si="2"/>
-        <v>3.5</v>
-      </c>
-      <c r="D29" s="22">
-        <f t="shared" si="2"/>
-        <v>12.187707886145738</v>
-      </c>
-      <c r="E29" s="22">
-        <f t="shared" si="2"/>
-        <v>25.286359195447272</v>
-      </c>
-      <c r="F29" s="22">
-        <f t="shared" si="2"/>
-        <v>42.44006386229114</v>
-      </c>
-      <c r="G29" s="22">
-        <f t="shared" si="2"/>
-        <v>63.418220571798358</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="21">
-        <v>30</v>
-      </c>
-      <c r="C30" s="22">
-        <f t="shared" si="2"/>
-        <v>4.4691499999999991</v>
-      </c>
-      <c r="D30" s="22">
-        <f t="shared" si="2"/>
-        <v>15.56248419981949</v>
-      </c>
-      <c r="E30" s="22">
-        <f t="shared" si="2"/>
-        <v>32.288152056666611</v>
-      </c>
-      <c r="F30" s="22">
-        <f t="shared" si="2"/>
-        <v>54.191717545759545</v>
-      </c>
-      <c r="G30" s="22">
-        <f t="shared" si="2"/>
-        <v>80.978725848129301</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="21">
-        <v>40</v>
-      </c>
-      <c r="C31" s="22">
-        <f t="shared" si="2"/>
-        <v>5.7066576349999965</v>
-      </c>
-      <c r="D31" s="22">
-        <f t="shared" si="2"/>
-        <v>19.871736074749503</v>
-      </c>
-      <c r="E31" s="22">
-        <f t="shared" si="2"/>
-        <v>41.228741361157589</v>
-      </c>
-      <c r="F31" s="22">
-        <f t="shared" si="2"/>
-        <v>69.197404134180346</v>
-      </c>
-      <c r="G31" s="22">
-        <f t="shared" si="2"/>
-        <v>103.40173503547628</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="21">
-        <v>50</v>
-      </c>
-      <c r="C32" s="22">
-        <f t="shared" si="2"/>
-        <v>7.2868311341314937</v>
-      </c>
-      <c r="D32" s="22">
-        <f t="shared" si="2"/>
-        <v>25.374219793847633</v>
-      </c>
-      <c r="E32" s="22">
-        <f t="shared" si="2"/>
-        <v>52.644979844062107</v>
-      </c>
-      <c r="F32" s="22">
-        <f t="shared" si="2"/>
-        <v>88.358165338934867</v>
-      </c>
-      <c r="G32" s="22">
-        <f t="shared" si="2"/>
-        <v>132.03367546679962</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="21">
-        <v>60</v>
-      </c>
-      <c r="C33" s="22">
-        <f t="shared" si="2"/>
-        <v>9.3045546751725041</v>
-      </c>
-      <c r="D33" s="22">
-        <f t="shared" si="2"/>
-        <v>32.400341254764037</v>
-      </c>
-      <c r="E33" s="22">
-        <f t="shared" si="2"/>
-        <v>67.222374762882893</v>
-      </c>
-      <c r="F33" s="22">
-        <f t="shared" si="2"/>
-        <v>112.82454132128592</v>
-      </c>
-      <c r="G33" s="22">
-        <f t="shared" si="2"/>
-        <v>168.59380020355641</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="21">
-        <v>70</v>
-      </c>
-      <c r="C34" s="22">
-        <f t="shared" si="2"/>
-        <v>11.880985864727768</v>
-      </c>
-      <c r="D34" s="22">
-        <f t="shared" si="2"/>
-        <v>41.371995748208192</v>
-      </c>
-      <c r="E34" s="22">
-        <f t="shared" si="2"/>
-        <v>85.83625033472515</v>
-      </c>
-      <c r="F34" s="22">
-        <f t="shared" si="2"/>
-        <v>144.06565681314996</v>
-      </c>
-      <c r="G34" s="22">
-        <f t="shared" si="2"/>
-        <v>215.27742347992114</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="21">
-        <v>80</v>
-      </c>
-      <c r="C35" s="22">
-        <f t="shared" si="2"/>
-        <v>15.170830850670884</v>
-      </c>
-      <c r="D35" s="22">
-        <f t="shared" si="2"/>
-        <v>52.82790137088702</v>
-      </c>
-      <c r="E35" s="22">
-        <f t="shared" si="2"/>
-        <v>109.6043080524105</v>
-      </c>
-      <c r="F35" s="22">
-        <f t="shared" si="2"/>
-        <v>183.95743718471113</v>
-      </c>
-      <c r="G35" s="22">
-        <f t="shared" si="2"/>
-        <v>274.88774204151122</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="21">
-        <v>90</v>
-      </c>
-      <c r="C36" s="22">
-        <f t="shared" si="2"/>
-        <v>19.371633913221643</v>
-      </c>
-      <c r="D36" s="22">
-        <f t="shared" si="2"/>
-        <v>67.455947260485615</v>
-      </c>
-      <c r="E36" s="22">
-        <f t="shared" si="2"/>
-        <v>139.95374095212296</v>
-      </c>
-      <c r="F36" s="22">
-        <f t="shared" si="2"/>
-        <v>234.89525154115753</v>
-      </c>
-      <c r="G36" s="22">
-        <f t="shared" si="2"/>
-        <v>351.00415781280554</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="21">
-        <v>100</v>
-      </c>
-      <c r="C37" s="22">
-        <f t="shared" si="2"/>
-        <v>24.735639343792712</v>
-      </c>
-      <c r="D37" s="22">
-        <f t="shared" si="2"/>
-        <v>86.13449905691408</v>
-      </c>
-      <c r="E37" s="22">
-        <f t="shared" si="2"/>
-        <v>178.70693182176578</v>
-      </c>
-      <c r="F37" s="22">
-        <f t="shared" si="2"/>
-        <v>299.93774669290406</v>
-      </c>
-      <c r="G37" s="22">
-        <f t="shared" si="2"/>
-        <v>448.19720911117139</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="21">
-        <v>110</v>
-      </c>
-      <c r="C38" s="22">
-        <f t="shared" si="2"/>
-        <v>31.584937878088908</v>
-      </c>
-      <c r="D38" s="22">
-        <f t="shared" si="2"/>
-        <v>109.98514184577355</v>
-      </c>
-      <c r="E38" s="22">
-        <f t="shared" si="2"/>
-        <v>228.19088124321266</v>
-      </c>
-      <c r="F38" s="22">
-        <f t="shared" si="2"/>
-        <v>382.99050875216915</v>
-      </c>
-      <c r="G38" s="22">
-        <f t="shared" si="2"/>
-        <v>572.30301631405462</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="21">
-        <v>120</v>
-      </c>
-      <c r="C39" s="22">
-        <f t="shared" si="2"/>
-        <v>40.330807176531721</v>
-      </c>
-      <c r="D39" s="22">
-        <f t="shared" si="2"/>
-        <v>140.44002762286823</v>
-      </c>
-      <c r="E39" s="22">
-        <f t="shared" si="2"/>
-        <v>291.3769362594582</v>
-      </c>
-      <c r="F39" s="22">
-        <f t="shared" si="2"/>
-        <v>489.04058062564462</v>
-      </c>
-      <c r="G39" s="22">
-        <f t="shared" si="2"/>
-        <v>730.77372153141607</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="21">
-        <v>130</v>
-      </c>
-      <c r="C40" s="22">
-        <f t="shared" si="2"/>
-        <v>51.498407683713339</v>
-      </c>
-      <c r="D40" s="22">
-        <f t="shared" si="2"/>
-        <v>179.32787127164036</v>
-      </c>
-      <c r="E40" s="22">
-        <f t="shared" si="2"/>
-        <v>372.05920990970202</v>
-      </c>
-      <c r="F40" s="22">
-        <f t="shared" si="2"/>
-        <v>624.45591740088537</v>
-      </c>
-      <c r="G40" s="22">
-        <f t="shared" si="2"/>
-        <v>933.12496502346505</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21">
-        <v>140</v>
-      </c>
-      <c r="C41" s="22">
-        <f t="shared" si="2"/>
-        <v>65.758316771333554</v>
-      </c>
-      <c r="D41" s="22">
-        <f t="shared" si="2"/>
-        <v>228.98375882675759</v>
-      </c>
-      <c r="E41" s="22">
-        <f t="shared" si="2"/>
-        <v>475.0824051336985</v>
-      </c>
-      <c r="F41" s="22">
-        <f t="shared" si="2"/>
-        <v>797.36776092919047</v>
-      </c>
-      <c r="G41" s="22">
-        <f t="shared" si="2"/>
-        <v>1191.5072678384624</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Support multiple bosses; Fix for swarm creatures; Better description of ship size
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
     <sheet name="Levels and Experience" sheetId="2" r:id="rId2"/>
     <sheet name="Mission Items" sheetId="11" r:id="rId3"/>
-    <sheet name="Map Size" sheetId="3" r:id="rId4"/>
-    <sheet name="Encumbrance" sheetId="9" r:id="rId5"/>
-    <sheet name="Armour Reduction" sheetId="10" r:id="rId6"/>
-    <sheet name="Relations Levels" sheetId="6" r:id="rId7"/>
-    <sheet name="Mercenary Cost" sheetId="5" r:id="rId8"/>
-    <sheet name="Difficulty Scaling" sheetId="7" r:id="rId9"/>
-    <sheet name="Colony Growth" sheetId="8" r:id="rId10"/>
+    <sheet name="Ships" sheetId="12" r:id="rId4"/>
+    <sheet name="Map Size" sheetId="3" r:id="rId5"/>
+    <sheet name="Encumbrance" sheetId="9" r:id="rId6"/>
+    <sheet name="Armour Reduction" sheetId="10" r:id="rId7"/>
+    <sheet name="Relations Levels" sheetId="6" r:id="rId8"/>
+    <sheet name="Mercenary Cost" sheetId="5" r:id="rId9"/>
+    <sheet name="Difficulty Scaling" sheetId="7" r:id="rId10"/>
+    <sheet name="Colony Growth" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
   <si>
     <t>Width</t>
   </si>
@@ -246,6 +247,60 @@
   </si>
   <si>
     <t>Prec Mult</t>
+  </si>
+  <si>
+    <t>Ship Name</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Hull</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Shuttle</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Light Freighter</t>
+  </si>
+  <si>
+    <t>Medium Freighter</t>
+  </si>
+  <si>
+    <t>Heavy Freighter</t>
+  </si>
+  <si>
+    <t>Corvette</t>
+  </si>
+  <si>
+    <t>Light Cruiser</t>
+  </si>
+  <si>
+    <t>Medium Cruiser</t>
+  </si>
+  <si>
+    <t>Heavy Cruiser</t>
+  </si>
+  <si>
+    <t>Flying Saucer</t>
+  </si>
+  <si>
+    <t>Bruiser</t>
+  </si>
+  <si>
+    <t>Armadillo</t>
   </si>
 </sst>
 </file>
@@ -961,11 +1016,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="634414120"/>
-        <c:axId val="634412552"/>
+        <c:axId val="199080368"/>
+        <c:axId val="199078016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634414120"/>
+        <c:axId val="199080368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1023,12 +1078,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634412552"/>
+        <c:crossAx val="199078016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="634412552"/>
+        <c:axId val="199078016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1086,7 +1141,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634414120"/>
+        <c:crossAx val="199080368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1150,7 +1205,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1528,11 +1582,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="634404712"/>
-        <c:axId val="634413728"/>
+        <c:axId val="199084288"/>
+        <c:axId val="199085072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634404712"/>
+        <c:axId val="199084288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,12 +1643,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634413728"/>
+        <c:crossAx val="199085072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="634413728"/>
+        <c:axId val="199085072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1651,7 +1705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634404712"/>
+        <c:crossAx val="199084288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4106,6 +4160,852 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>POWER(MIN($I$6,A3)/$I$3,$I$4)</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>POWER(MAX(0,A3-$I$6)/$J$3,$J$4)</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>1+ROUND(B3+C3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="15">
+        <v>1</v>
+      </c>
+      <c r="J3" s="15">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.5</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B48" si="0">POWER(MIN($I$6,A4)/$I$3,$I$4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C48" si="1">POWER(MAX(0,A4-$I$6)/$J$3,$J$4)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D48" si="2">1+ROUND(B4+C4,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="15">
+        <v>1</v>
+      </c>
+      <c r="J4" s="15">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="15">
+        <v>5</v>
+      </c>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2.5</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3.5</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4.5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.46198883129171492</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.77696950424091227</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>1.0531068011637541</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>1.3067017417552778</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>1.544752759668611</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>1.7711074679558145</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>1.9881768219176268</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>2.197601620895596</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>2.4005643849798499</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>2.5979541161172355</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>2.7904612136214872</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>2.9786358416662546</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>3.1629257048074275</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>3.3437015248821096</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>3.5212748169149664</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>3.6959106503337189</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>22</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>3.8678370351754467</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>23</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>4.037251971830587</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>24</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>4.2043288433264205</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>4.3692206064732311</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>4.5320630960351513</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>4.6929776628776771</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>4.8520733044687701</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>29</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>5.0094484032067692</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>30</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>5.1651921580697824</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>31</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>5.3193857737727885</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>5.4721034562358728</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>33</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>5.6234132519034921</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>34</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>5.7733777600998772</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>35</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>5.9220547413339508</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>36</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>6.069497639707075</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>6.2157560339272981</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>38</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>6.3608760286087715</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>39</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>6.5049005953291763</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>40</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>6.6478698711812365</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5328,7 +6228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -5496,7 +6396,7 @@
         <v>117.30745821681678</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D5:D28" si="1">ROUND(POWER($J$5,$B15)*$J$6,0)*10</f>
+        <f t="shared" ref="D15:D28" si="1">ROUND(POWER($J$5,$B15)*$J$6,0)*10</f>
         <v>4090</v>
       </c>
     </row>
@@ -5539,7 +6439,7 @@
         <v>9190</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E5:E28" si="2">ROUND(POWER($J$7,$B18)*$J$8,0)*10</f>
+        <f t="shared" ref="E18:E28" si="2">ROUND(POWER($J$7,$B18)*$J$8,0)*10</f>
         <v>14360</v>
       </c>
     </row>
@@ -5721,10 +6621,352 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f>(C4*2)+(D4*4)+(E4*8)+F4+4</f>
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <f>CEILING(SQRT(G4)-3,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G15" si="0">(C5*2)+(D5*4)+(E5*8)+F5+4</f>
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H15" si="1">CEILING(SQRT(G5)-3,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5894,7 +7136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F28"/>
   <sheetViews>
@@ -6164,7 +7406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H27"/>
   <sheetViews>
@@ -6557,7 +7799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
@@ -7913,7 +9155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F22"/>
   <sheetViews>
@@ -8133,850 +9375,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J48"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <f>POWER(MIN($I$6,A3)/$I$3,$I$4)</f>
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <f>POWER(MAX(0,A3-$I$6)/$J$3,$J$4)</f>
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <f>1+ROUND(B3+C3,0)</f>
-        <v>1</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="15">
-        <v>1</v>
-      </c>
-      <c r="J3" s="15">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0.5</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B48" si="0">POWER(MIN($I$6,A4)/$I$3,$I$4)</f>
-        <v>0.5</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C48" si="1">POWER(MAX(0,A4-$I$6)/$J$3,$J$4)</f>
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D48" si="2">1+ROUND(B4+C4,0)</f>
-        <v>2</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="15">
-        <v>1</v>
-      </c>
-      <c r="J4" s="15">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1.5</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="15">
-        <v>5</v>
-      </c>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2.5</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3.5</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4.5</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>0.46198883129171492</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>0.77696950424091227</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>1.0531068011637541</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>1.3067017417552778</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>1.544752759668611</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>11</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>1.7711074679558145</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>12</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>1.9881768219176268</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>13</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>2.197601620895596</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>14</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
-        <v>2.4005643849798499</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>15</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
-        <v>2.5979541161172355</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>16</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
-        <v>2.7904612136214872</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>17</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="1"/>
-        <v>2.9786358416662546</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>18</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>3.1629257048074275</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>19</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>3.3437015248821096</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>20</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>3.5212748169149664</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>21</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>3.6959106503337189</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>22</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="1"/>
-        <v>3.8678370351754467</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>23</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="1"/>
-        <v>4.037251971830587</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>24</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="1"/>
-        <v>4.2043288433264205</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>25</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="1"/>
-        <v>4.3692206064732311</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>26</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="1"/>
-        <v>4.5320630960351513</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>27</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="1"/>
-        <v>4.6929776628776771</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>28</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="1"/>
-        <v>4.8520733044687701</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>29</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="1"/>
-        <v>5.0094484032067692</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>30</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="1"/>
-        <v>5.1651921580697824</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>31</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="1"/>
-        <v>5.3193857737727885</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>32</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="1"/>
-        <v>5.4721034562358728</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>33</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="1"/>
-        <v>5.6234132519034921</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>34</v>
-      </c>
-      <c r="B42">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C42">
-        <f t="shared" si="1"/>
-        <v>5.7733777600998772</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>35</v>
-      </c>
-      <c r="B43">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="1"/>
-        <v>5.9220547413339508</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>36</v>
-      </c>
-      <c r="B44">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C44">
-        <f t="shared" si="1"/>
-        <v>6.069497639707075</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>37</v>
-      </c>
-      <c r="B45">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="1"/>
-        <v>6.2157560339272981</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>38</v>
-      </c>
-      <c r="B46">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="1"/>
-        <v>6.3608760286087715</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>39</v>
-      </c>
-      <c r="B47">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="1"/>
-        <v>6.5049005953291763</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>40</v>
-      </c>
-      <c r="B48">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C48">
-        <f t="shared" si="1"/>
-        <v>6.6478698711812365</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Better bugs; quieter shotgun; Minor bugfixes; Easier levelling;
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -488,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -555,6 +555,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,11 +1020,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199080368"/>
-        <c:axId val="199078016"/>
+        <c:axId val="515561824"/>
+        <c:axId val="515566136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="199080368"/>
+        <c:axId val="515561824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1078,12 +1082,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199078016"/>
+        <c:crossAx val="515566136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199078016"/>
+        <c:axId val="515566136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1141,7 +1145,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199080368"/>
+        <c:crossAx val="515561824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1582,11 +1586,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199084288"/>
-        <c:axId val="199085072"/>
+        <c:axId val="515556336"/>
+        <c:axId val="515563392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="199084288"/>
+        <c:axId val="515556336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1643,12 +1647,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199085072"/>
+        <c:crossAx val="515563392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199085072"/>
+        <c:axId val="515563392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1705,7 +1709,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199084288"/>
+        <c:crossAx val="515556336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5917,44 +5921,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="6"/>
     <col min="6" max="6" width="22.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="27" t="s">
         <v>29</v>
       </c>
       <c r="G2" s="28">
-        <v>1.62</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
+      <c r="B3" s="38">
         <v>1</v>
       </c>
       <c r="C3" s="4">
         <v>0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="39">
         <v>0</v>
       </c>
       <c r="F3" s="27" t="s">
@@ -5965,15 +5969,15 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+      <c r="B4" s="38">
         <v>2</v>
       </c>
       <c r="C4" s="4">
-        <f t="shared" ref="C4:C22" si="0">INT($G$4*((POWER($G$2,$B4-2)*$G$3)-($G$3-1)))</f>
+        <f>INT($G$4*((POWER($G$2,$B4-2)*$G$3)-($G$3-1)))</f>
         <v>1000</v>
       </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D22" si="1">ROUND($C4,2-(1+INT(LOG10($C4))))</f>
+      <c r="D4" s="39">
+        <f>ROUND($C4,3-(1+INT(LOG10($C4))))</f>
         <v>1000</v>
       </c>
       <c r="F4" s="27" t="s">
@@ -5984,238 +5988,238 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="B5" s="38">
         <v>3</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" si="0"/>
-        <v>3480</v>
-      </c>
-      <c r="D5" s="4">
-        <f t="shared" si="1"/>
-        <v>3500</v>
+        <f t="shared" ref="C4:C22" si="0">INT($G$4*((POWER($G$2,$B5-2)*$G$3)-($G$3-1)))</f>
+        <v>3400</v>
+      </c>
+      <c r="D5" s="39">
+        <f t="shared" ref="D5:D22" si="1">ROUND($C5,3-(1+INT(LOG10($C5))))</f>
+        <v>3400</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="B6" s="38">
         <v>4</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>7497</v>
-      </c>
-      <c r="D6" s="4">
-        <f t="shared" si="1"/>
-        <v>7500</v>
+        <v>7240</v>
+      </c>
+      <c r="D6" s="39">
+        <f t="shared" si="1"/>
+        <v>7240</v>
       </c>
       <c r="J6" s="19"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="38">
         <v>5</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>14006</v>
-      </c>
-      <c r="D7" s="4">
-        <f t="shared" si="1"/>
-        <v>14000</v>
+        <v>13384</v>
+      </c>
+      <c r="D7" s="39">
+        <f t="shared" si="1"/>
+        <v>13400</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+      <c r="B8" s="38">
         <v>6</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>24549</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="1"/>
-        <v>25000</v>
+        <v>23214</v>
+      </c>
+      <c r="D8" s="39">
+        <f t="shared" si="1"/>
+        <v>23200</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
+      <c r="B9" s="38">
         <v>7</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>41630</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="1"/>
-        <v>42000</v>
+        <v>38943</v>
+      </c>
+      <c r="D9" s="39">
+        <f t="shared" si="1"/>
+        <v>38900</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
+      <c r="B10" s="38">
         <v>8</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>69301</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="1"/>
-        <v>69000</v>
+        <v>64108</v>
+      </c>
+      <c r="D10" s="39">
+        <f t="shared" si="1"/>
+        <v>64100</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+      <c r="B11" s="38">
         <v>9</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>114129</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="1"/>
-        <v>110000</v>
+        <v>104374</v>
+      </c>
+      <c r="D11" s="39">
+        <f t="shared" si="1"/>
+        <v>104000</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
+      <c r="B12" s="38">
         <v>10</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>186749</v>
-      </c>
-      <c r="D12" s="4">
-        <f t="shared" si="1"/>
-        <v>190000</v>
+        <v>168798</v>
+      </c>
+      <c r="D12" s="39">
+        <f t="shared" si="1"/>
+        <v>169000</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
+      <c r="B13" s="38">
         <v>11</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>304393</v>
-      </c>
-      <c r="D13" s="4">
-        <f t="shared" si="1"/>
-        <v>300000</v>
+        <v>271877</v>
+      </c>
+      <c r="D13" s="39">
+        <f t="shared" si="1"/>
+        <v>272000</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
+      <c r="B14" s="38">
         <v>12</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>494977</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" si="1"/>
-        <v>490000</v>
+        <v>436804</v>
+      </c>
+      <c r="D14" s="39">
+        <f t="shared" si="1"/>
+        <v>437000</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
+      <c r="B15" s="38">
         <v>13</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
-        <v>803724</v>
-      </c>
-      <c r="D15" s="4">
-        <f t="shared" si="1"/>
-        <v>800000</v>
+        <v>700687</v>
+      </c>
+      <c r="D15" s="39">
+        <f t="shared" si="1"/>
+        <v>701000</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="3">
+      <c r="B16" s="38">
         <v>14</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
-        <v>1303893</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" si="1"/>
-        <v>1300000</v>
+        <v>1122899</v>
+      </c>
+      <c r="D16" s="39">
+        <f t="shared" si="1"/>
+        <v>1120000</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="3">
+      <c r="B17" s="38">
         <v>15</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="0"/>
-        <v>2114167</v>
-      </c>
-      <c r="D17" s="4">
-        <f t="shared" si="1"/>
-        <v>2100000</v>
+        <v>1798439</v>
+      </c>
+      <c r="D17" s="39">
+        <f t="shared" si="1"/>
+        <v>1800000</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="3">
+      <c r="B18" s="38">
         <v>16</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="0"/>
-        <v>3426811</v>
-      </c>
-      <c r="D18" s="4">
-        <f t="shared" si="1"/>
-        <v>3400000</v>
+        <v>2879303</v>
+      </c>
+      <c r="D18" s="39">
+        <f t="shared" si="1"/>
+        <v>2880000</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="3">
+      <c r="B19" s="38">
         <v>17</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="0"/>
-        <v>5553293</v>
-      </c>
-      <c r="D19" s="4">
-        <f t="shared" si="1"/>
-        <v>5600000</v>
+        <v>4608686</v>
+      </c>
+      <c r="D19" s="39">
+        <f t="shared" si="1"/>
+        <v>4610000</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3">
+      <c r="B20" s="38">
         <v>18</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="0"/>
-        <v>8998196</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="1"/>
-        <v>9000000</v>
+        <v>7375697</v>
+      </c>
+      <c r="D20" s="39">
+        <f t="shared" si="1"/>
+        <v>7380000</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="3">
+      <c r="B21" s="38">
         <v>19</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="0"/>
-        <v>14578937</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="1"/>
-        <v>15000000</v>
+        <v>11802916</v>
+      </c>
+      <c r="D21" s="39">
+        <f t="shared" si="1"/>
+        <v>11800000</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="3">
+      <c r="B22" s="38">
         <v>20</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="0"/>
-        <v>23619739</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="1"/>
-        <v>24000000</v>
+        <v>18886465</v>
+      </c>
+      <c r="D22" s="39">
+        <f t="shared" si="1"/>
+        <v>18900000</v>
       </c>
     </row>
   </sheetData>
@@ -6623,7 +6627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor fixes; Fixing enemy choice at high levels; Harder distant planets
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
   <si>
     <t>Width</t>
   </si>
@@ -112,12 +112,6 @@
   </si>
   <si>
     <t>Inner Rad</t>
-  </si>
-  <si>
-    <t>Inner bit</t>
-  </si>
-  <si>
-    <t>Outer bit</t>
   </si>
   <si>
     <t>SoldierLevelExperience</t>
@@ -301,6 +295,15 @@
   </si>
   <si>
     <t>Armadillo</t>
+  </si>
+  <si>
+    <t>Outer 2</t>
+  </si>
+  <si>
+    <t>Modified</t>
+  </si>
+  <si>
+    <t>Outer2</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -559,6 +562,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1020,11 +1026,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="515561824"/>
-        <c:axId val="515566136"/>
+        <c:axId val="508667360"/>
+        <c:axId val="508675200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="515561824"/>
+        <c:axId val="508667360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1082,12 +1088,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515566136"/>
+        <c:crossAx val="508675200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="515566136"/>
+        <c:axId val="508675200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1145,7 +1151,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515561824"/>
+        <c:crossAx val="508667360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1208,36 +1214,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1249,7 +1225,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Difficulty Scaling'!$D$2</c:f>
+              <c:f>'Difficulty Scaling'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1397,41 +1373,56 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>32</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>33</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>34</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>36</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>37</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>38</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>39</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>40</c:v>
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Difficulty Scaling'!$D$3:$D$53</c:f>
+              <c:f>'Difficulty Scaling'!$E$3:$E$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -1439,139 +1430,518 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>15.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Difficulty Scaling'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Modified</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Difficulty Scaling'!$A$3:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Difficulty Scaling'!$F$3:$F$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10</c:v>
+                  <c:v>10.199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10</c:v>
+                  <c:v>10.4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>11</c:v>
+                  <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11</c:v>
+                  <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>11</c:v>
+                  <c:v>11.4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>11</c:v>
+                  <c:v>11.6</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>12</c:v>
+                  <c:v>12.7</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>12</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>12</c:v>
+                  <c:v>13.4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12</c:v>
+                  <c:v>13.8</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>12</c:v>
+                  <c:v>14.2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>12</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>13</c:v>
+                  <c:v>14.9</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>13</c:v>
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>15.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>15.9</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>16.899999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1586,13 +1956,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="515556336"/>
-        <c:axId val="515563392"/>
+        <c:axId val="508664224"/>
+        <c:axId val="508667752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="515556336"/>
+        <c:axId val="508664224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="60"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1647,12 +2018,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515563392"/>
+        <c:crossAx val="508667752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="515563392"/>
+        <c:axId val="508667752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,7 +2080,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515556336"/>
+        <c:crossAx val="508664224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2909,16 +3280,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3226,10 +3597,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>3</v>
@@ -3277,7 +3648,7 @@
         <v>2</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M5" s="26">
         <v>0.01</v>
@@ -3493,7 +3864,7 @@
         <v>8</v>
       </c>
       <c r="L12" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -4164,87 +4535,118 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J48"/>
+  <dimension ref="A2:L53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="F2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
-        <f>POWER(MIN($I$6,A3)/$I$3,$I$4)</f>
+        <f>POWER(MIN($J$6,A3)/$J$3,$J$4)</f>
         <v>0</v>
       </c>
       <c r="C3">
-        <f>POWER(MAX(0,A3-$I$6)/$J$3,$J$4)</f>
+        <f>POWER(MAX(0,A3-$J$6)/$K$3,$K$4)</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f>1+ROUND(B3+C3,0)</f>
+        <f>POWER(MAX(0,A3-$J$6)/$L$3,$L$4)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>1+ROUND(B3+C3,1)</f>
         <v>1</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="F3">
+        <f>1+ROUND(B3+D3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="15">
+      <c r="J3" s="15">
         <v>1</v>
       </c>
-      <c r="J3" s="15">
+      <c r="K3" s="15">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="40">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.5</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B48" si="0">POWER(MIN($I$6,A4)/$I$3,$I$4)</f>
+        <f t="shared" ref="B4:B48" si="0">POWER(MIN($J$6,A4)/$J$3,$J$4)</f>
         <v>0.5</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C48" si="1">POWER(MAX(0,A4-$I$6)/$J$3,$J$4)</f>
+        <f t="shared" ref="C4:C48" si="1">POWER(MAX(0,A4-$J$6)/$K$3,$K$4)</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D48" si="2">1+ROUND(B4+C4,0)</f>
-        <v>2</v>
-      </c>
-      <c r="H4" s="14" t="s">
+        <f t="shared" ref="D4:D53" si="2">POWER(MAX(0,A4-$J$6)/$L$3,$L$4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E58" si="3">1+ROUND(B4+C4,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F53" si="4">1+ROUND(B4+D4,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="15">
+      <c r="J4" s="15">
         <v>1</v>
       </c>
-      <c r="J4" s="15">
+      <c r="K4" s="15">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" s="40">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4258,12 +4660,20 @@
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="F5">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
       <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.5</v>
       </c>
@@ -4277,17 +4687,25 @@
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="H6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="15">
+      <c r="J6" s="15">
         <v>5</v>
       </c>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4301,10 +4719,18 @@
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.5</v>
       </c>
@@ -4318,10 +4744,18 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>3.5</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -4335,10 +4769,18 @@
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3.5</v>
       </c>
@@ -4352,10 +4794,18 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>4.5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -4369,10 +4819,18 @@
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4.5</v>
       </c>
@@ -4386,10 +4844,18 @@
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>5.5</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -4403,10 +4869,18 @@
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -4420,10 +4894,18 @@
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.36246255803490574</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -4437,10 +4919,18 @@
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.6533390962161274</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>6.8</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -4454,10 +4944,18 @@
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.92218110097346973</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>7.1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
@@ -4471,10 +4969,18 @@
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.1776443254130531</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>7.3</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -4488,10 +4994,18 @@
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.4235989361633579</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>7.5</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
@@ -4505,10 +5019,18 @@
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.6622322877266087</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>7.8</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="4"/>
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -4522,10 +5044,18 @@
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
+        <v>1.8949444582901722</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
@@ -4539,10 +5069,18 @@
       </c>
       <c r="D21">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.1227049861390666</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="4"/>
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
@@ -4556,10 +5094,18 @@
       </c>
       <c r="D22">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.3462229798387728</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>8.4</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
@@ -4573,10 +5119,18 @@
       </c>
       <c r="D23">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.5660383995790244</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>8.6</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16</v>
       </c>
@@ -4590,10 +5144,18 @@
       </c>
       <c r="D24">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.7825753497553483</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17</v>
       </c>
@@ -4607,10 +5169,18 @@
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
+        <v>2.9961752365605294</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>18</v>
       </c>
@@ -4624,10 +5194,18 @@
       </c>
       <c r="D26">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.2071184525071126</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
@@ -4641,10 +5219,18 @@
       </c>
       <c r="D27">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.4156391393116934</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
@@ -4658,10 +5244,18 @@
       </c>
       <c r="D28">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.621935577051683</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>9.5</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>21</v>
       </c>
@@ -4675,10 +5269,18 @@
       </c>
       <c r="D29">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.8261777014882994</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>22</v>
       </c>
@@ -4692,10 +5294,18 @@
       </c>
       <c r="D30">
         <f t="shared" si="2"/>
+        <v>4.028512673725654</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>9.9</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>23</v>
       </c>
@@ -4709,10 +5319,18 @@
       </c>
       <c r="D31">
         <f t="shared" si="2"/>
+        <v>4.2290690919357088</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>24</v>
       </c>
@@ -4726,10 +5344,18 @@
       </c>
       <c r="D32">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.4279602333888501</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>25</v>
       </c>
@@ -4743,10 +5369,18 @@
       </c>
       <c r="D33">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.6252865893955004</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>10.4</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>26</v>
       </c>
@@ -4760,10 +5394,18 @@
       </c>
       <c r="D34">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.8211378750500362</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>10.5</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="4"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>27</v>
       </c>
@@ -4777,10 +5419,18 @@
       </c>
       <c r="D35">
         <f t="shared" si="2"/>
+        <v>5.0155946424330002</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>10.7</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>28</v>
       </c>
@@ -4794,10 +5444,18 @@
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.2087295899889892</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>10.9</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="4"/>
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>29</v>
       </c>
@@ -4811,10 +5469,18 @@
       </c>
       <c r="D37">
         <f t="shared" si="2"/>
+        <v>5.4006086360265817</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="4"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>30</v>
       </c>
@@ -4828,12 +5494,20 @@
       </c>
       <c r="D38">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.5912918068913386</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>11.2</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="4"/>
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
@@ -4841,16 +5515,24 @@
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>5.3193857737727885</v>
+        <v>5.4721034562358728</v>
       </c>
       <c r="D39">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.9692854964308104</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>11.5</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
@@ -4858,16 +5540,24 @@
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>5.4721034562358728</v>
+        <v>5.7733777600998772</v>
       </c>
       <c r="D40">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.3430984100943029</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>11.8</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="4"/>
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
@@ -4875,16 +5565,24 @@
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>5.6234132519034921</v>
+        <v>6.069497639707075</v>
       </c>
       <c r="D41">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.7130609587083541</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="3"/>
+        <v>12.1</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="4"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
@@ -4892,16 +5590,24 @@
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>5.7733777600998772</v>
+        <v>6.3608760286087715</v>
       </c>
       <c r="D42">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7.0794578438413795</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="3"/>
+        <v>12.4</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="4"/>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
@@ -4909,16 +5615,24 @@
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>5.9220547413339508</v>
+        <v>6.6478698711812365</v>
       </c>
       <c r="D43">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7.4425367672065939</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="3"/>
+        <v>12.6</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="4"/>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
@@ -4926,16 +5640,24 @@
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>6.069497639707075</v>
+        <v>6.9307904697597307</v>
       </c>
       <c r="D44">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7.8025150774346717</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="3"/>
+        <v>12.9</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="4"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
@@ -4943,16 +5665,24 @@
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>6.2157560339272981</v>
+        <v>7.2099114647321967</v>
       </c>
       <c r="D45">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8.1595849279431594</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="3"/>
+        <v>13.2</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="4"/>
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
@@ -4960,16 +5690,24 @@
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>6.3608760286087715</v>
+        <v>7.4854750825681302</v>
       </c>
       <c r="D46">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8.5139173387511722</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="3"/>
+        <v>13.5</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="4"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
@@ -4977,16 +5715,24 @@
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>6.5049005953291763</v>
+        <v>7.7576970937680656</v>
       </c>
       <c r="D47">
         <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8.865665437297249</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="3"/>
+        <v>13.8</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="4"/>
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
@@ -4994,11 +5740,144 @@
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>6.6478698711812365</v>
+        <v>8.0267707946348086</v>
       </c>
       <c r="D48">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>9.21496707469257</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="4"/>
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>52</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ref="B49:B58" si="5">POWER(MIN($J$6,A49)/$J$3,$J$4)</f>
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49:C58" si="6">POWER(MAX(0,A49-$J$6)/$K$3,$K$4)</f>
+        <v>8.292870239843845</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>9.5619469601927403</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="3"/>
+        <v>14.3</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="4"/>
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>54</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="6"/>
+        <v>8.5561528926107702</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>9.9067184193376274</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="3"/>
+        <v>14.6</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="4"/>
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>56</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="6"/>
+        <v>8.8167618168334734</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>10.249384854763781</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="3"/>
+        <v>14.8</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="4"/>
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>58</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="6"/>
+        <v>9.0748275051947083</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>10.590040969659048</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="3"/>
+        <v>15.1</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="4"/>
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>60</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="6"/>
+        <v>9.3304694151105512</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>10.928773799926171</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="3"/>
+        <v>15.3</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="4"/>
+        <v>16.899999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -5020,15 +5899,15 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E3" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K3">
         <v>1.8</v>
@@ -5036,7 +5915,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
@@ -5054,13 +5933,13 @@
         <v>5</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K4">
         <v>2.5</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O4" s="24"/>
       <c r="P4" s="24"/>
@@ -5092,13 +5971,13 @@
         <v>45.298728979855973</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K5">
         <v>365</v>
       </c>
       <c r="N5" s="24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O5" s="24"/>
       <c r="P5" s="24"/>
@@ -5130,7 +6009,7 @@
         <v>45.298728979855973</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K6">
         <v>1.1299999999999999</v>
@@ -5166,13 +6045,13 @@
         <v>45.298728979855973</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K7">
         <v>5</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O7" s="24"/>
       <c r="P7" s="24"/>
@@ -5204,13 +6083,13 @@
         <v>57.841947034378073</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K8">
         <v>20</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O8" s="24"/>
       <c r="P8" s="24"/>
@@ -5242,7 +6121,7 @@
         <v>73.858382168197352</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O9" s="24"/>
       <c r="P9" s="24"/>
@@ -5274,7 +6153,7 @@
         <v>94.309768190571162</v>
       </c>
       <c r="N10" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O10" s="24"/>
       <c r="P10" s="24"/>
@@ -5508,17 +6387,17 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E25" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="8">
         <v>1</v>
@@ -5921,7 +6800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -5939,13 +6818,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G2" s="28">
         <v>1.6</v>
@@ -5962,7 +6841,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G3" s="28">
         <v>4</v>
@@ -5981,7 +6860,7 @@
         <v>1000</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="28">
         <v>1000</v>
@@ -5992,7 +6871,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C4:C22" si="0">INT($G$4*((POWER($G$2,$B5-2)*$G$3)-($G$3-1)))</f>
+        <f t="shared" ref="C5:C22" si="0">INT($G$4*((POWER($G$2,$B5-2)*$G$3)-($G$3-1)))</f>
         <v>3400</v>
       </c>
       <c r="D5" s="39">
@@ -6247,13 +7126,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>63</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>65</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>7</v>
@@ -6271,7 +7150,7 @@
         <v>4.6900000000000004</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J4">
         <v>3.5</v>
@@ -6286,7 +7165,7 @@
         <v>6.2846000000000011</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J5">
         <v>1.31</v>
@@ -6301,7 +7180,7 @@
         <v>8.4213640000000023</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J6">
         <v>16</v>
@@ -6316,7 +7195,7 @@
         <v>11.284627760000005</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J7">
         <v>1.31</v>
@@ -6331,7 +7210,7 @@
         <v>15.121401198400006</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J8">
         <v>25</v>
@@ -6638,22 +7517,22 @@
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>11</v>
@@ -6661,7 +7540,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -6686,7 +7565,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -6711,7 +7590,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -6736,7 +7615,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -6761,7 +7640,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -6786,7 +7665,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -6811,7 +7690,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -6836,7 +7715,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -6861,7 +7740,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12">
         <v>6</v>
@@ -6886,7 +7765,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -6911,7 +7790,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -6936,7 +7815,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15">
         <v>8</v>
@@ -7152,10 +8031,10 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -7429,19 +8308,19 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="H2" s="33" t="s">
         <v>57</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -7479,7 +8358,7 @@
         <v>97.064458573273242</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" s="15">
         <v>30</v>
@@ -7501,10 +8380,10 @@
         <v>94.591812522665393</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="15">
         <v>0.9</v>

</xml_diff>

<commit_message>
Improving build skill, fabrication etc.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Mercenary Cost" sheetId="5" r:id="rId9"/>
     <sheet name="Difficulty Scaling" sheetId="7" r:id="rId10"/>
     <sheet name="Colony Growth" sheetId="8" r:id="rId11"/>
+    <sheet name="Build Diff" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
   <si>
     <t>Width</t>
   </si>
@@ -304,6 +305,12 @@
   </si>
   <si>
     <t>Outer2</t>
+  </si>
+  <si>
+    <t>Relative Diff</t>
+  </si>
+  <si>
+    <t>Prob</t>
   </si>
 </sst>
 </file>
@@ -1026,11 +1033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="508667360"/>
-        <c:axId val="508675200"/>
+        <c:axId val="633059056"/>
+        <c:axId val="633052392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="508667360"/>
+        <c:axId val="633059056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1088,12 +1095,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508675200"/>
+        <c:crossAx val="633052392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="508675200"/>
+        <c:axId val="633052392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1151,7 +1158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508667360"/>
+        <c:crossAx val="633059056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1956,11 +1963,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="508664224"/>
-        <c:axId val="508667752"/>
+        <c:axId val="633050040"/>
+        <c:axId val="633053960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="508664224"/>
+        <c:axId val="633050040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -2018,12 +2025,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508667752"/>
+        <c:crossAx val="633053960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="508667752"/>
+        <c:axId val="633053960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2080,7 +2087,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508664224"/>
+        <c:crossAx val="633050040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4537,7 +4544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -4626,7 +4633,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E58" si="3">1+ROUND(B4+C4,1)</f>
+        <f t="shared" ref="E4:E53" si="3">1+ROUND(B4+C4,1)</f>
         <v>1.5</v>
       </c>
       <c r="F4">
@@ -5760,11 +5767,11 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <f t="shared" ref="B49:B58" si="5">POWER(MIN($J$6,A49)/$J$3,$J$4)</f>
+        <f t="shared" ref="B49:B53" si="5">POWER(MIN($J$6,A49)/$J$3,$J$4)</f>
         <v>5</v>
       </c>
       <c r="C49">
-        <f t="shared" ref="C49:C58" si="6">POWER(MAX(0,A49-$J$6)/$K$3,$K$4)</f>
+        <f t="shared" ref="C49:C53" si="6">POWER(MAX(0,A49-$J$6)/$K$3,$K$4)</f>
         <v>8.292870239843845</v>
       </c>
       <c r="D49">
@@ -6788,6 +6795,228 @@
       <c r="G41" s="22">
         <f t="shared" si="2"/>
         <v>1191.5072678384624</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="40">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>-10</v>
+      </c>
+      <c r="C3">
+        <f>1/(1+EXP(-$B3*$F$2))</f>
+        <v>1.2339457598623172E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>-9</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C23" si="0">1/(1+EXP(-B4))</f>
+        <v>1.2339457598623172E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>-8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3.3535013046647811E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>-7</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>9.1105119440064539E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>-6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>2.4726231566347743E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>-5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>6.6928509242848554E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>-4</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>1.7986209962091559E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>-3</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>4.7425873177566781E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>-2</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.11920292202211755</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>-1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.2689414213699951</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.7310585786300049</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.88079707797788231</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.95257412682243336</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.98201379003790845</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.99330714907571527</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.99752737684336534</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.9990889488055994</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0.99966464986953363</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.99987660542401369</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.99995460213129761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Better Mercs; Ice creatures; tweaks
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -1033,11 +1033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="633059056"/>
-        <c:axId val="633052392"/>
+        <c:axId val="653284144"/>
+        <c:axId val="653284928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="633059056"/>
+        <c:axId val="653284144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1095,12 +1095,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="633052392"/>
+        <c:crossAx val="653284928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="633052392"/>
+        <c:axId val="653284928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1158,7 +1158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="633059056"/>
+        <c:crossAx val="653284144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1963,11 +1963,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="633050040"/>
-        <c:axId val="633053960"/>
+        <c:axId val="653278264"/>
+        <c:axId val="653276304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="633050040"/>
+        <c:axId val="653278264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -2025,12 +2025,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="633053960"/>
+        <c:crossAx val="653276304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="633053960"/>
+        <c:axId val="653276304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2087,7 +2087,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="633050040"/>
+        <c:crossAx val="653278264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6807,7 +6807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
@@ -10271,8 +10271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10291,13 +10291,13 @@
       </c>
       <c r="C3" s="4">
         <f t="shared" ref="C3:C22" si="0">$B3*POWER($F$4,$F$5*$B3)*$F$3</f>
-        <v>17.141191951192397</v>
+        <v>8.0823725227664784</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -10306,13 +10306,13 @@
       </c>
       <c r="C4" s="4">
         <f t="shared" si="0"/>
-        <v>39.176061534349742</v>
+        <v>21.774915198923519</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -10321,13 +10321,13 @@
       </c>
       <c r="C5" s="4">
         <f t="shared" si="0"/>
-        <v>67.152439065201392</v>
+        <v>43.998244072337414</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -10336,7 +10336,7 @@
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>102.31758648954383</v>
+        <v>79.024488653385092</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -10345,7 +10345,7 @@
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>146.15378250000009</v>
+        <v>133.06361577453981</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -10354,7 +10354,7 @@
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>200.42000321802604</v>
+        <v>215.09394238321934</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -10363,7 +10363,7 @@
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>267.20071357923865</v>
+        <v>338.03571078115363</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -10372,7 +10372,7 @@
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>348.96295016817601</v>
+        <v>520.40581724408241</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -10381,7 +10381,7 @@
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>448.62306845153205</v>
+        <v>788.64631462151328</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -10390,7 +10390,7 @@
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>569.62475037486206</v>
+        <v>1180.3950561996239</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -10399,7 +10399,7 @@
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>716.03012699720796</v>
+        <v>1749.0719708434926</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -10408,7 +10408,7 @@
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>892.62617088696811</v>
+        <v>2570.300224997538</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -10417,7 +10417,7 @@
       </c>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
-        <v>1105.0488609211561</v>
+        <v>3750.8834844326066</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -10426,7 +10426,7 @@
       </c>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
-        <v>1359.9280254715111</v>
+        <v>5441.3400839676069</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -10435,7 +10435,7 @@
       </c>
       <c r="C17" s="4">
         <f t="shared" si="0"/>
-        <v>1665.0562374580884</v>
+        <v>7853.3817110156533</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -10444,7 +10444,7 @@
       </c>
       <c r="C18" s="4">
         <f t="shared" si="0"/>
-        <v>2029.5856765012818</v>
+        <v>11284.258942561721</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -10453,7 +10453,7 @@
       </c>
       <c r="C19" s="4">
         <f t="shared" si="0"/>
-        <v>2464.2575010795235</v>
+        <v>16150.634740535708</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -10462,7 +10462,7 @@
       </c>
       <c r="C20" s="4">
         <f t="shared" si="0"/>
-        <v>2981.6690006943409</v>
+        <v>23035.667020966474</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
       </c>
       <c r="C21" s="4">
         <f t="shared" si="0"/>
-        <v>3596.5846401504168</v>
+        <v>32754.388900956412</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -10480,7 +10480,7 @@
       </c>
       <c r="C22" s="4">
         <f t="shared" si="0"/>
-        <v>4326.2980831949862</v>
+        <v>46444.4162900171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing construction chance, weakining hive spawn
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="12720" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures Per Level" sheetId="1" r:id="rId1"/>
@@ -1033,11 +1033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="653284144"/>
-        <c:axId val="653284928"/>
+        <c:axId val="513095160"/>
+        <c:axId val="510329336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="653284144"/>
+        <c:axId val="513095160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1095,12 +1095,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="653284928"/>
+        <c:crossAx val="510329336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="653284928"/>
+        <c:axId val="510329336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1158,7 +1158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="653284144"/>
+        <c:crossAx val="513095160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1963,11 +1963,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="653278264"/>
-        <c:axId val="653276304"/>
+        <c:axId val="512541632"/>
+        <c:axId val="512619080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="653278264"/>
+        <c:axId val="512541632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -2025,12 +2025,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="653276304"/>
+        <c:crossAx val="512619080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="653276304"/>
+        <c:axId val="512619080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2087,7 +2087,425 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="653278264"/>
+        <c:crossAx val="512541632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Build Diff'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Prob</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Build Diff'!$B$3:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Build Diff'!$C$3:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.8312567555274113E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7313528403278421E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0728381752463738E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0697939828597031E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0346948776147878E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13411267636614951</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1979033167907106</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28839676921547225</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40985560245783575</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55679935243531631</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.70710678118654757</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.83064702559367087</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.91215041804185149</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95751099393483607</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9802215449597278</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99096608924720953</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99591035181227039</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99815618021458152</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99917025522171421</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9996269159872414</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99983231087494551</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="514505032"/>
+        <c:axId val="514507384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="514505032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="514507384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="514507384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="514505032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2177,6 +2595,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3248,6 +3706,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3297,6 +4271,41 @@
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6807,8 +7816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6827,7 +7836,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="40">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -6835,8 +7844,8 @@
         <v>-10</v>
       </c>
       <c r="C3">
-        <f>1/(1+EXP(-$B3*$F$2))</f>
-        <v>1.2339457598623172E-4</v>
+        <f>SQRT(1/(1+EXP(-$B3*$F$2)))</f>
+        <v>1.8312567555274113E-2</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -6844,8 +7853,8 @@
         <v>-9</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C23" si="0">1/(1+EXP(-B4))</f>
-        <v>1.2339457598623172E-4</v>
+        <f t="shared" ref="C4:C23" si="0">SQRT(1/(1+EXP(-$B4*$F$2)))</f>
+        <v>2.7313528403278421E-2</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -6854,7 +7863,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>3.3535013046647811E-4</v>
+        <v>4.0728381752463738E-2</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -6863,7 +7872,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>9.1105119440064539E-4</v>
+        <v>6.0697939828597031E-2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -6872,7 +7881,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>2.4726231566347743E-3</v>
+        <v>9.0346948776147878E-2</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -6881,7 +7890,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>6.6928509242848554E-3</v>
+        <v>0.13411267636614951</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -6890,7 +7899,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>1.7986209962091559E-2</v>
+        <v>0.1979033167907106</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -6899,7 +7908,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>4.7425873177566781E-2</v>
+        <v>0.28839676921547225</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -6908,7 +7917,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.11920292202211755</v>
+        <v>0.40985560245783575</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -6917,7 +7926,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0.2689414213699951</v>
+        <v>0.55679935243531631</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -6926,7 +7935,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.70710678118654757</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -6935,7 +7944,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0.7310585786300049</v>
+        <v>0.83064702559367087</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -6944,7 +7953,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.88079707797788231</v>
+        <v>0.91215041804185149</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -6953,7 +7962,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.95257412682243336</v>
+        <v>0.95751099393483607</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -6962,7 +7971,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.98201379003790845</v>
+        <v>0.9802215449597278</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -6971,7 +7980,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.99330714907571527</v>
+        <v>0.99096608924720953</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -6980,7 +7989,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.99752737684336534</v>
+        <v>0.99591035181227039</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -6989,7 +7998,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>0.9990889488055994</v>
+        <v>0.99815618021458152</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -6998,7 +8007,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>0.99966464986953363</v>
+        <v>0.99917025522171421</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -7007,7 +8016,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>0.99987660542401369</v>
+        <v>0.9996269159872414</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -7016,12 +8025,13 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>0.99995460213129761</v>
+        <v>0.99983231087494551</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10271,7 +11281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>